<commit_message>
adding new refactor code like write_header, write_footer, write_summary
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -306,7 +306,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -359,10 +359,12 @@
       <left style="thin">
         <color rgb="00000000"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
     </border>
     <border>
       <left style="thin">
@@ -371,22 +373,6 @@
       <right style="thin">
         <color rgb="00000000"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="00000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="00000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="00000000"/>
-      </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -425,12 +411,10 @@
       <left style="thin">
         <color rgb="00000000"/>
       </left>
-      <right style="thin">
-        <color rgb="00000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="00000000"/>
-      </top>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -439,29 +423,14 @@
       <right style="thin">
         <color rgb="00000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="00000000"/>
       </left>
-      <right style="thin">
-        <color rgb="00000000"/>
-      </right>
-      <bottom style="thin">
-        <color rgb="00000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="00000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color rgb="00000000"/>
       </right>
@@ -481,7 +450,7 @@
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
@@ -776,34 +745,22 @@
     <xf numFmtId="0" fontId="40" fillId="4" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="40" fillId="4" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="41" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="4" fontId="41" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="4" fontId="38" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="35" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="168" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -812,56 +769,70 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="39" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="39" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="4" fontId="39" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="4" fontId="39" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="39" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="39" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="4" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="39" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="39" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="39" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="3" fontId="38" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="38" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="38" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="38" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="38" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="38" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="38" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="38" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="38" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1550,7 +1521,7 @@
         </is>
       </c>
       <c r="E3" s="108" t="n">
-        <v>45803</v>
+        <v>45819</v>
       </c>
     </row>
     <row r="4" ht="30" customFormat="1" customHeight="1" s="35">
@@ -1564,7 +1535,7 @@
       </c>
       <c r="E4" s="57" t="inlineStr">
         <is>
-          <t>KB25012</t>
+          <t>JF25030</t>
         </is>
       </c>
     </row>
@@ -1662,355 +1633,556 @@
     <row r="15" ht="36" customHeight="1">
       <c r="A15" s="109" t="inlineStr">
         <is>
-          <t>NO.</t>
+          <t>No.</t>
         </is>
       </c>
       <c r="B15" s="109" t="inlineStr">
         <is>
-          <t>P.O. Nº</t>
+          <t>ITEM Nº</t>
         </is>
       </c>
       <c r="C15" s="109" t="inlineStr">
         <is>
-          <t>ITEM Nº</t>
+          <t>Quantity</t>
         </is>
       </c>
       <c r="D15" s="109" t="inlineStr">
         <is>
-          <t>Description</t>
+          <t>Unit Price(USD)</t>
         </is>
       </c>
       <c r="E15" s="109" t="inlineStr">
         <is>
-          <t>Quantity</t>
-        </is>
-      </c>
-      <c r="F15" s="110" t="n"/>
-      <c r="G15" s="109" t="inlineStr">
-        <is>
-          <t>Unit Price(USD)</t>
-        </is>
-      </c>
-      <c r="H15" s="109" t="inlineStr">
-        <is>
           <t>Total value(USD)</t>
         </is>
       </c>
     </row>
-    <row r="16" ht="36" customHeight="1">
-      <c r="A16" s="111" t="n"/>
-      <c r="B16" s="111" t="n"/>
-      <c r="C16" s="111" t="n"/>
-      <c r="D16" s="111" t="n"/>
-      <c r="E16" s="112" t="inlineStr">
-        <is>
-          <t>PCS</t>
-        </is>
-      </c>
-      <c r="F16" s="109" t="inlineStr">
-        <is>
-          <t>SF</t>
-        </is>
-      </c>
-      <c r="G16" s="111" t="n"/>
-      <c r="H16" s="111" t="n"/>
+    <row r="16" ht="30" customHeight="1">
+      <c r="A16" s="110" t="n">
+        <v>1</v>
+      </c>
+      <c r="B16" s="110" t="inlineStr">
+        <is>
+          <t>01.10.U756033</t>
+        </is>
+      </c>
+      <c r="C16" s="111" t="n">
+        <v>7438.8</v>
+      </c>
+      <c r="D16" s="111" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="E16" s="111">
+        <f>D16 * C16</f>
+        <v/>
+      </c>
     </row>
     <row r="17" ht="30" customFormat="1" customHeight="1" s="36">
-      <c r="A17" s="113" t="n">
-        <v>1</v>
-      </c>
-      <c r="B17" s="113" t="inlineStr">
-        <is>
-          <t>RB0604</t>
-        </is>
-      </c>
-      <c r="C17" s="113" t="inlineStr">
-        <is>
-          <t>1.23.07.0154J</t>
-        </is>
-      </c>
-      <c r="D17" s="114" t="inlineStr">
-        <is>
-          <t>LEATHER</t>
-        </is>
-      </c>
-      <c r="E17" s="115" t="n"/>
-      <c r="F17" s="116" t="n">
-        <v>31925.1</v>
-      </c>
-      <c r="G17" s="116" t="n">
+      <c r="A17" s="110" t="n">
+        <v>2</v>
+      </c>
+      <c r="B17" s="110" t="inlineStr">
+        <is>
+          <t>01.10.U756033</t>
+        </is>
+      </c>
+      <c r="C17" s="111" t="n">
+        <v>242.7</v>
+      </c>
+      <c r="D17" s="111" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="E17" s="111">
+        <f>D17 * C17</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" ht="30" customFormat="1" customHeight="1" s="36">
+      <c r="A18" s="110" t="n">
+        <v>3</v>
+      </c>
+      <c r="B18" s="110" t="inlineStr">
+        <is>
+          <t>01.10.W653191</t>
+        </is>
+      </c>
+      <c r="C18" s="111" t="n">
+        <v>5748.5</v>
+      </c>
+      <c r="D18" s="111" t="n">
         <v>1.3</v>
       </c>
-      <c r="H17" s="116">
-        <f>G17 * F17</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" ht="30" customFormat="1" customHeight="1" s="36">
-      <c r="A18" s="113" t="n">
-        <v>2</v>
-      </c>
-      <c r="B18" s="113" t="inlineStr">
-        <is>
-          <t>RB3358</t>
-        </is>
-      </c>
-      <c r="C18" s="113" t="inlineStr">
-        <is>
-          <t>1.23.07.0157J</t>
-        </is>
-      </c>
-      <c r="D18" s="117" t="n"/>
-      <c r="E18" s="118" t="n"/>
-      <c r="F18" s="116" t="n">
-        <v>11067.7</v>
-      </c>
-      <c r="G18" s="116" t="n">
-        <v>1.47</v>
-      </c>
-      <c r="H18" s="116">
-        <f>G18 * F18</f>
+      <c r="E18" s="111">
+        <f>D18 * C18</f>
         <v/>
       </c>
     </row>
     <row r="19" ht="30" customFormat="1" customHeight="1" s="36">
-      <c r="A19" s="113" t="n">
-        <v>3</v>
-      </c>
-      <c r="B19" s="113" t="inlineStr">
-        <is>
-          <t>SJ0B-317</t>
-        </is>
-      </c>
-      <c r="C19" s="113" t="inlineStr">
-        <is>
-          <t>1.23.07.0220D</t>
-        </is>
-      </c>
-      <c r="D19" s="117" t="n"/>
-      <c r="E19" s="118" t="n"/>
-      <c r="F19" s="116" t="n">
-        <v>78616.8</v>
-      </c>
-      <c r="G19" s="116" t="n">
-        <v>1.47</v>
-      </c>
-      <c r="H19" s="116">
-        <f>G19 * F19</f>
+      <c r="A19" s="110" t="n">
+        <v>4</v>
+      </c>
+      <c r="B19" s="110" t="inlineStr">
+        <is>
+          <t>01.10.W783049</t>
+        </is>
+      </c>
+      <c r="C19" s="111" t="n">
+        <v>9263.5</v>
+      </c>
+      <c r="D19" s="111" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="E19" s="111">
+        <f>D19 * C19</f>
         <v/>
       </c>
     </row>
     <row r="20" ht="30" customFormat="1" customHeight="1" s="36">
-      <c r="A20" s="113" t="n">
-        <v>4</v>
-      </c>
-      <c r="B20" s="113" t="inlineStr">
-        <is>
-          <t>SJ0B-317</t>
-        </is>
-      </c>
-      <c r="C20" s="113" t="inlineStr">
-        <is>
-          <t>1.23.07.0220D</t>
-        </is>
-      </c>
-      <c r="D20" s="111" t="n"/>
-      <c r="E20" s="119" t="n"/>
-      <c r="F20" s="116" t="n">
-        <v>1588.2</v>
-      </c>
-      <c r="G20" s="116" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="H20" s="116">
-        <f>G20 * F20</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" ht="36" customFormat="1" customHeight="1" s="36">
-      <c r="A21" s="120" t="inlineStr">
-        <is>
-          <t xml:space="preserve">TOTAL OF: </t>
-        </is>
-      </c>
-      <c r="B21" s="121" t="n"/>
-      <c r="C21" s="121" t="n"/>
-      <c r="D21" s="120" t="inlineStr">
-        <is>
-          <t>0 PALLETS</t>
-        </is>
-      </c>
-      <c r="E21" s="120">
-        <f>SUM(E17:E20)</f>
-        <v/>
-      </c>
-      <c r="F21" s="120">
-        <f>SUM(F17:F20)</f>
-        <v/>
-      </c>
-      <c r="G21" s="121" t="n"/>
-      <c r="H21" s="120">
-        <f>SUM(H17:H20)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="22" ht="41.1" customFormat="1" customHeight="1" s="36">
-      <c r="A22" s="45" t="inlineStr">
+      <c r="A20" s="110" t="n">
+        <v>5</v>
+      </c>
+      <c r="B20" s="110" t="inlineStr">
+        <is>
+          <t>01.10.W783049</t>
+        </is>
+      </c>
+      <c r="C20" s="111" t="n">
+        <v>112.5</v>
+      </c>
+      <c r="D20" s="111" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="E20" s="111">
+        <f>D20 * C20</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" ht="30" customFormat="1" customHeight="1" s="36">
+      <c r="A21" s="110" t="n">
+        <v>6</v>
+      </c>
+      <c r="B21" s="110" t="inlineStr">
+        <is>
+          <t>01.10.W783049</t>
+        </is>
+      </c>
+      <c r="C21" s="111" t="n">
+        <v>10077.9</v>
+      </c>
+      <c r="D21" s="111" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="E21" s="111">
+        <f>D21 * C21</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" ht="30" customFormat="1" customHeight="1" s="36">
+      <c r="A22" s="110" t="n">
+        <v>7</v>
+      </c>
+      <c r="B22" s="110" t="inlineStr">
+        <is>
+          <t>01.10.U741023</t>
+        </is>
+      </c>
+      <c r="C22" s="111" t="n">
+        <v>18953.2</v>
+      </c>
+      <c r="D22" s="111" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="E22" s="111">
+        <f>D22 * C22</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" ht="30" customFormat="1" customHeight="1" s="36">
+      <c r="A23" s="110" t="n">
+        <v>8</v>
+      </c>
+      <c r="B23" s="110" t="inlineStr">
+        <is>
+          <t>01.10.U741023</t>
+        </is>
+      </c>
+      <c r="C23" s="111" t="n">
+        <v>56.5</v>
+      </c>
+      <c r="D23" s="111" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="E23" s="111">
+        <f>D23 * C23</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" ht="30" customFormat="1" customHeight="1" s="36">
+      <c r="A24" s="110" t="n">
+        <v>9</v>
+      </c>
+      <c r="B24" s="110" t="inlineStr">
+        <is>
+          <t>01.10.U741023</t>
+        </is>
+      </c>
+      <c r="C24" s="111" t="n">
+        <v>487.6</v>
+      </c>
+      <c r="D24" s="111" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="E24" s="111">
+        <f>D24 * C24</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" ht="30" customFormat="1" customHeight="1" s="36">
+      <c r="A25" s="110" t="n">
+        <v>10</v>
+      </c>
+      <c r="B25" s="110" t="inlineStr">
+        <is>
+          <t>01.10.U741023</t>
+        </is>
+      </c>
+      <c r="C25" s="111" t="n">
+        <v>9892.700000000001</v>
+      </c>
+      <c r="D25" s="111" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="E25" s="111">
+        <f>D25 * C25</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" ht="30" customFormat="1" customHeight="1" s="37">
+      <c r="A26" s="110" t="n">
+        <v>11</v>
+      </c>
+      <c r="B26" s="110" t="inlineStr">
+        <is>
+          <t>01.10.U722233</t>
+        </is>
+      </c>
+      <c r="C26" s="111" t="n">
+        <v>9198.4</v>
+      </c>
+      <c r="D26" s="111" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="E26" s="111">
+        <f>D26 * C26</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" ht="30" customFormat="1" customHeight="1" s="37">
+      <c r="A27" s="110" t="n">
+        <v>12</v>
+      </c>
+      <c r="B27" s="110" t="inlineStr">
+        <is>
+          <t>01.10.U722233</t>
+        </is>
+      </c>
+      <c r="C27" s="111" t="n">
+        <v>635.8</v>
+      </c>
+      <c r="D27" s="111" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="E27" s="111">
+        <f>D27 * C27</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" ht="30" customHeight="1">
+      <c r="A28" s="110" t="n">
+        <v>13</v>
+      </c>
+      <c r="B28" s="110" t="inlineStr">
+        <is>
+          <t>01.10.U722233</t>
+        </is>
+      </c>
+      <c r="C28" s="111" t="n">
+        <v>9074.200000000001</v>
+      </c>
+      <c r="D28" s="111" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="E28" s="111">
+        <f>D28 * C28</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" ht="30" customHeight="1">
+      <c r="A29" s="110" t="n">
+        <v>14</v>
+      </c>
+      <c r="B29" s="110" t="inlineStr">
+        <is>
+          <t>01.10.U722233</t>
+        </is>
+      </c>
+      <c r="C29" s="111" t="n">
+        <v>247</v>
+      </c>
+      <c r="D29" s="111" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="E29" s="111">
+        <f>D29 * C29</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" ht="30" customHeight="1">
+      <c r="A30" s="110" t="n">
+        <v>15</v>
+      </c>
+      <c r="B30" s="110" t="inlineStr">
+        <is>
+          <t>01.10.U528110</t>
+        </is>
+      </c>
+      <c r="C30" s="111" t="n">
+        <v>25569.9</v>
+      </c>
+      <c r="D30" s="111" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="E30" s="111">
+        <f>D30 * C30</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" ht="30" customHeight="1">
+      <c r="A31" s="110" t="n">
+        <v>16</v>
+      </c>
+      <c r="B31" s="110" t="inlineStr">
+        <is>
+          <t>01.10.U528110</t>
+        </is>
+      </c>
+      <c r="C31" s="111" t="n">
+        <v>1162.8</v>
+      </c>
+      <c r="D31" s="111" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="E31" s="111">
+        <f>D31 * C31</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" ht="30" customHeight="1">
+      <c r="A32" s="110" t="n">
+        <v>17</v>
+      </c>
+      <c r="B32" s="110" t="inlineStr">
+        <is>
+          <t>01.10.U528103</t>
+        </is>
+      </c>
+      <c r="C32" s="111" t="n">
+        <v>20551.4</v>
+      </c>
+      <c r="D32" s="111" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="E32" s="111">
+        <f>D32 * C32</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" ht="30" customHeight="1">
+      <c r="A33" s="110" t="n">
+        <v>18</v>
+      </c>
+      <c r="B33" s="110" t="inlineStr">
+        <is>
+          <t>01.10.U528103</t>
+        </is>
+      </c>
+      <c r="C33" s="111" t="n">
+        <v>1513.7</v>
+      </c>
+      <c r="D33" s="111" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="E33" s="111">
+        <f>D33 * C33</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" ht="36" customHeight="1">
+      <c r="A34" s="112" t="inlineStr">
+        <is>
+          <t>TOTAL:</t>
+        </is>
+      </c>
+      <c r="B34" s="113" t="n"/>
+      <c r="C34" s="114">
+        <f>SUM(C16:C33)</f>
+        <v/>
+      </c>
+      <c r="D34" s="112" t="n"/>
+      <c r="E34" s="114">
+        <f>SUM(E16:E33)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="94" t="n"/>
+      <c r="C35" s="115" t="n"/>
+      <c r="D35" s="115" t="n"/>
+      <c r="E35" s="115" t="n"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="45" t="inlineStr">
         <is>
           <t>FCA:</t>
         </is>
       </c>
-      <c r="B22" s="46" t="inlineStr">
+      <c r="B36" s="46" t="inlineStr">
         <is>
           <t>BAVET, SVAY RIENG</t>
         </is>
       </c>
-      <c r="C22" s="41" t="n"/>
-      <c r="D22" s="41" t="n"/>
-      <c r="E22" s="41" t="n"/>
-    </row>
-    <row r="23" ht="29.1" customFormat="1" customHeight="1" s="36">
-      <c r="A23" s="41" t="inlineStr">
+      <c r="C36" s="41" t="n"/>
+      <c r="D36" s="41" t="n"/>
+      <c r="E36" s="41" t="n"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="41" t="inlineStr">
         <is>
           <t>Term of Payment: 100% TT after shipment</t>
         </is>
       </c>
-      <c r="B23" s="41" t="n"/>
-      <c r="C23" s="41" t="n"/>
-      <c r="D23" s="41" t="n"/>
-      <c r="E23" s="41" t="n"/>
-    </row>
-    <row r="24" ht="29.1" customFormat="1" customHeight="1" s="36">
-      <c r="A24" s="41" t="inlineStr">
+      <c r="B37" s="41" t="n"/>
+      <c r="C37" s="41" t="n"/>
+      <c r="D37" s="41" t="n"/>
+      <c r="E37" s="41" t="n"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="41" t="inlineStr">
         <is>
           <t>Transaction method: FCA(USD)</t>
         </is>
       </c>
-      <c r="B24" s="41" t="n"/>
-      <c r="C24" s="41" t="n"/>
-      <c r="D24" s="41" t="n"/>
-      <c r="E24" s="41" t="n"/>
-    </row>
-    <row r="25" ht="29.1" customFormat="1" customHeight="1" s="36">
-      <c r="A25" s="41" t="inlineStr">
+      <c r="B38" s="41" t="n"/>
+      <c r="C38" s="41" t="n"/>
+      <c r="D38" s="41" t="n"/>
+      <c r="E38" s="41" t="n"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="41" t="inlineStr">
         <is>
           <t xml:space="preserve">Beneficiary bank information: </t>
         </is>
       </c>
-      <c r="B25" s="41" t="n"/>
-      <c r="C25" s="41" t="inlineStr">
+      <c r="B39" s="41" t="n"/>
+      <c r="C39" s="41" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO.,LTD.</t>
         </is>
       </c>
-      <c r="D25" s="41" t="n"/>
-      <c r="E25" s="41" t="n"/>
-    </row>
-    <row r="26" ht="45.95" customFormat="1" customHeight="1" s="37">
-      <c r="A26" s="41" t="inlineStr">
+      <c r="D39" s="41" t="n"/>
+      <c r="E39" s="41" t="n"/>
+    </row>
+    <row r="40" ht="45.95" customHeight="1">
+      <c r="A40" s="41" t="inlineStr">
         <is>
           <t xml:space="preserve">Beneficiary Bank' s Name: </t>
         </is>
       </c>
-      <c r="B26" s="41" t="n"/>
-      <c r="C26" s="91" t="inlineStr">
+      <c r="B40" s="41" t="n"/>
+      <c r="C40" s="91" t="inlineStr">
         <is>
           <t>BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
  /BANK OF CHINA PHNOM PENH BRANCH</t>
         </is>
       </c>
     </row>
-    <row r="27" ht="41.1" customFormat="1" customHeight="1" s="37">
-      <c r="A27" s="41" t="inlineStr">
+    <row r="41" ht="41.1" customHeight="1">
+      <c r="A41" s="41" t="inlineStr">
         <is>
           <t xml:space="preserve">Bank Address:  </t>
         </is>
       </c>
-      <c r="B27" s="41" t="n"/>
-      <c r="C27" s="91" t="inlineStr">
+      <c r="B41" s="41" t="n"/>
+      <c r="C41" s="91" t="inlineStr">
         <is>
           <t>1st AND 2nd FLOOR,CANADIA TOWER,No.315 ANDDUONG ST.
 PHNOM PEMH,CAMBODIA.</t>
         </is>
       </c>
     </row>
-    <row r="28" ht="29.1" customHeight="1">
-      <c r="A28" s="41" t="inlineStr">
+    <row r="42" ht="29.1" customHeight="1">
+      <c r="A42" s="41" t="inlineStr">
         <is>
           <t>Bank account :</t>
         </is>
       </c>
-      <c r="B28" s="41" t="n"/>
-      <c r="C28" s="92" t="inlineStr">
+      <c r="B42" s="41" t="n"/>
+      <c r="C42" s="92" t="inlineStr">
         <is>
           <t>100001100764430</t>
         </is>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="41" t="inlineStr">
+    <row r="43">
+      <c r="A43" s="41" t="inlineStr">
         <is>
           <t>SWIFT CODE  ：</t>
         </is>
       </c>
-      <c r="B29" s="41" t="n"/>
-      <c r="C29" s="41" t="inlineStr">
+      <c r="B43" s="41" t="n"/>
+      <c r="C43" s="41" t="inlineStr">
         <is>
           <t>BKCHKHPPXXX</t>
         </is>
       </c>
-      <c r="D29" s="41" t="n"/>
-      <c r="E29" s="41" t="n"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="41" t="n"/>
-      <c r="B30" s="41" t="n"/>
-      <c r="C30" s="41" t="n"/>
-      <c r="D30" s="41" t="n"/>
-      <c r="E30" s="41" t="n"/>
-      <c r="F30" s="41" t="n"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="37" t="inlineStr">
+      <c r="D43" s="41" t="n"/>
+      <c r="E43" s="41" t="n"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="41" t="n"/>
+      <c r="B44" s="41" t="n"/>
+      <c r="C44" s="41" t="n"/>
+      <c r="D44" s="41" t="n"/>
+      <c r="E44" s="41" t="n"/>
+      <c r="F44" s="41" t="n"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="37" t="inlineStr">
         <is>
           <t>The Buyer:</t>
         </is>
       </c>
-      <c r="D31" s="47" t="inlineStr">
+      <c r="D45" s="47" t="inlineStr">
         <is>
           <t>The Seller:</t>
         </is>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="73" t="inlineStr">
+    <row r="46">
+      <c r="A46" s="73" t="inlineStr">
         <is>
           <t>JASON FURNITURE VIET NAM COMPANY LIMITED</t>
         </is>
       </c>
-      <c r="B32" s="72" t="n"/>
-      <c r="C32" s="48" t="n"/>
-      <c r="D32" s="73" t="inlineStr">
+      <c r="B46" s="72" t="n"/>
+      <c r="C46" s="48" t="n"/>
+      <c r="D46" s="73" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO.,LTD.</t>
         </is>
       </c>
-      <c r="E32" s="73" t="n"/>
-    </row>
-    <row r="33"/>
-    <row r="34"/>
-    <row r="35"/>
-    <row r="36"/>
-    <row r="37"/>
-    <row r="38"/>
-    <row r="39"/>
-    <row r="40"/>
-    <row r="41"/>
-    <row r="42"/>
-    <row r="43"/>
-    <row r="44"/>
-    <row r="45"/>
-    <row r="46"/>
+      <c r="E46" s="73" t="n"/>
+    </row>
     <row r="47"/>
     <row r="48"/>
     <row r="49"/>
@@ -2166,28 +2338,18 @@
     <row r="199"/>
     <row r="200" ht="27.95" customHeight="1"/>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="C22:E22"/>
+  <mergeCells count="11">
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="C40:E40"/>
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="D17:D20"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="E15:F15"/>
     <mergeCell ref="B11:E11"/>
+    <mergeCell ref="A13:E13"/>
     <mergeCell ref="A14:E14"/>
-    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="A34:B34"/>
     <mergeCell ref="A200:B200"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="B10:E10"/>
   </mergeCells>
   <pageMargins left="0.432638888888889" right="0.314583333333333" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9" scale="43"/>
@@ -2255,12 +2417,12 @@
           <t>Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="B5" s="122" t="n"/>
-      <c r="C5" s="122" t="n"/>
-      <c r="D5" s="122" t="n"/>
-      <c r="E5" s="122" t="n"/>
-      <c r="F5" s="122" t="n"/>
-      <c r="G5" s="122" t="n"/>
+      <c r="B5" s="116" t="n"/>
+      <c r="C5" s="116" t="n"/>
+      <c r="D5" s="116" t="n"/>
+      <c r="E5" s="116" t="n"/>
+      <c r="F5" s="116" t="n"/>
+      <c r="G5" s="116" t="n"/>
     </row>
     <row r="6" ht="83.25" customHeight="1">
       <c r="A6" s="100" t="inlineStr">
@@ -2268,12 +2430,12 @@
           <t>INVOICE</t>
         </is>
       </c>
-      <c r="B6" s="123" t="n"/>
-      <c r="C6" s="123" t="n"/>
-      <c r="D6" s="123" t="n"/>
-      <c r="E6" s="123" t="n"/>
-      <c r="F6" s="123" t="n"/>
-      <c r="G6" s="123" t="n"/>
+      <c r="B6" s="117" t="n"/>
+      <c r="C6" s="117" t="n"/>
+      <c r="D6" s="117" t="n"/>
+      <c r="E6" s="117" t="n"/>
+      <c r="F6" s="117" t="n"/>
+      <c r="G6" s="117" t="n"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="4" t="n"/>
@@ -2288,7 +2450,7 @@
       </c>
       <c r="G7" s="58" t="inlineStr">
         <is>
-          <t>CLF2025-152</t>
+          <t>CLF2025-171</t>
         </is>
       </c>
     </row>
@@ -2311,7 +2473,7 @@
       </c>
       <c r="G8" s="86" t="inlineStr">
         <is>
-          <t>KB25012</t>
+          <t>JF25030</t>
         </is>
       </c>
     </row>
@@ -2328,8 +2490,8 @@
           <t>Date:</t>
         </is>
       </c>
-      <c r="G9" s="124" t="n">
-        <v>45803</v>
+      <c r="G9" s="118" t="n">
+        <v>45819</v>
       </c>
     </row>
     <row r="10" ht="22.5" customHeight="1">
@@ -2464,425 +2626,802 @@
       <c r="B20" s="20" t="n"/>
     </row>
     <row r="21" ht="35" customHeight="1">
-      <c r="A21" s="125" t="inlineStr">
-        <is>
-          <t>NO.</t>
-        </is>
-      </c>
-      <c r="B21" s="125" t="inlineStr">
+      <c r="A21" s="119" t="inlineStr">
+        <is>
+          <t>Mark &amp; Nº</t>
+        </is>
+      </c>
+      <c r="B21" s="119" t="inlineStr">
         <is>
           <t>P.O. Nº</t>
         </is>
       </c>
-      <c r="C21" s="125" t="inlineStr">
+      <c r="C21" s="119" t="inlineStr">
         <is>
           <t>ITEM Nº</t>
         </is>
       </c>
-      <c r="D21" s="125" t="inlineStr">
+      <c r="D21" s="119" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="E21" s="125" t="inlineStr">
+      <c r="E21" s="119" t="inlineStr">
         <is>
           <t>Quantity</t>
         </is>
       </c>
-      <c r="F21" s="110" t="n"/>
-      <c r="G21" s="125" t="inlineStr">
+      <c r="F21" s="119" t="inlineStr">
         <is>
           <t>Unit price (USD)</t>
         </is>
       </c>
-      <c r="H21" s="125" t="inlineStr">
+      <c r="G21" s="119" t="inlineStr">
         <is>
           <t>Amount (USD)</t>
         </is>
       </c>
     </row>
     <row r="22" ht="35" customHeight="1">
-      <c r="A22" s="111" t="n"/>
-      <c r="B22" s="111" t="n"/>
-      <c r="C22" s="111" t="n"/>
-      <c r="D22" s="111" t="n"/>
-      <c r="E22" s="125" t="inlineStr">
-        <is>
-          <t>PCS</t>
-        </is>
-      </c>
-      <c r="F22" s="125" t="inlineStr">
-        <is>
-          <t>SF</t>
-        </is>
-      </c>
-      <c r="G22" s="111" t="n"/>
-      <c r="H22" s="111" t="n"/>
-      <c r="L22" s="49" t="n"/>
-      <c r="M22" s="50" t="n"/>
-      <c r="N22" s="51" t="n"/>
-      <c r="O22" s="51" t="n"/>
+      <c r="A22" s="120" t="inlineStr">
+        <is>
+          <t>VENDOR#:</t>
+        </is>
+      </c>
+      <c r="B22" s="121" t="inlineStr">
+        <is>
+          <t>9000619872</t>
+        </is>
+      </c>
+      <c r="C22" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U756033</t>
+        </is>
+      </c>
+      <c r="D22" s="122" t="inlineStr">
+        <is>
+          <t>BUFFALO HIDE</t>
+        </is>
+      </c>
+      <c r="E22" s="123" t="n">
+        <v>7438.8</v>
+      </c>
+      <c r="F22" s="123" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="G22" s="123">
+        <f>F22 * E22</f>
+        <v/>
+      </c>
     </row>
     <row r="23" ht="35" customHeight="1">
-      <c r="A23" s="126" t="inlineStr">
-        <is>
-          <t>VENDOR#:</t>
-        </is>
-      </c>
-      <c r="B23" s="127" t="inlineStr">
-        <is>
-          <t>RB0604</t>
-        </is>
-      </c>
-      <c r="C23" s="127" t="inlineStr">
-        <is>
-          <t>1.23.07.0154J</t>
-        </is>
-      </c>
-      <c r="D23" s="110" t="n"/>
-      <c r="E23" s="126" t="n"/>
-      <c r="F23" s="128" t="n">
-        <v>31925.1</v>
-      </c>
-      <c r="G23" s="128" t="n">
+      <c r="A23" s="124" t="inlineStr">
+        <is>
+          <t>Des: LEATHER</t>
+        </is>
+      </c>
+      <c r="B23" s="121" t="inlineStr">
+        <is>
+          <t>9000619872</t>
+        </is>
+      </c>
+      <c r="C23" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U756033</t>
+        </is>
+      </c>
+      <c r="D23" s="122" t="inlineStr">
+        <is>
+          <t>BUFFALO HIDE</t>
+        </is>
+      </c>
+      <c r="E23" s="123" t="n">
+        <v>242.7</v>
+      </c>
+      <c r="F23" s="123" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="G23" s="123">
+        <f>F23 * E23</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" ht="35" customHeight="1">
+      <c r="A24" s="124" t="inlineStr">
+        <is>
+          <t>MADE IN CAMBODIA</t>
+        </is>
+      </c>
+      <c r="B24" s="121" t="inlineStr">
+        <is>
+          <t>9000691966</t>
+        </is>
+      </c>
+      <c r="C24" s="121" t="inlineStr">
+        <is>
+          <t>01.10.W653191</t>
+        </is>
+      </c>
+      <c r="D24" s="122" t="inlineStr">
+        <is>
+          <t>BUFFALO HIDE</t>
+        </is>
+      </c>
+      <c r="E24" s="123" t="n">
+        <v>5748.5</v>
+      </c>
+      <c r="F24" s="123" t="n">
         <v>1.3</v>
       </c>
-      <c r="H23" s="128">
-        <f>G23 * F23</f>
-        <v/>
-      </c>
-    </row>
-    <row r="24" ht="35" customHeight="1">
-      <c r="A24" s="129" t="inlineStr">
-        <is>
-          <t>Des: LEATHER</t>
-        </is>
-      </c>
-      <c r="B24" s="127" t="inlineStr">
-        <is>
-          <t>RB3358</t>
-        </is>
-      </c>
-      <c r="C24" s="127" t="inlineStr">
-        <is>
-          <t>1.23.07.0157J</t>
-        </is>
-      </c>
-      <c r="D24" s="130" t="n"/>
-      <c r="E24" s="129" t="n"/>
-      <c r="F24" s="131" t="n">
-        <v>11067.7</v>
-      </c>
-      <c r="G24" s="131" t="n">
-        <v>1.47</v>
-      </c>
-      <c r="H24" s="131">
-        <f>G24 * F24</f>
+      <c r="G24" s="123">
+        <f>F24 * E24</f>
         <v/>
       </c>
     </row>
     <row r="25" ht="35" customHeight="1">
-      <c r="A25" s="129" t="inlineStr">
-        <is>
-          <t>MADE IN CAMBODIA</t>
-        </is>
-      </c>
-      <c r="B25" s="127" t="inlineStr">
-        <is>
-          <t>SJ0B-317</t>
-        </is>
-      </c>
-      <c r="C25" s="127" t="inlineStr">
-        <is>
-          <t>1.23.07.0220D</t>
-        </is>
-      </c>
-      <c r="D25" s="130" t="n"/>
-      <c r="E25" s="129" t="n"/>
-      <c r="F25" s="131" t="n">
-        <v>78616.8</v>
-      </c>
-      <c r="G25" s="131" t="n">
-        <v>1.47</v>
-      </c>
-      <c r="H25" s="131">
-        <f>G25 * F25</f>
+      <c r="A25" s="124" t="n"/>
+      <c r="B25" s="121" t="inlineStr">
+        <is>
+          <t>9000606101</t>
+        </is>
+      </c>
+      <c r="C25" s="121" t="inlineStr">
+        <is>
+          <t>01.10.W783049</t>
+        </is>
+      </c>
+      <c r="D25" s="122" t="inlineStr">
+        <is>
+          <t>BUFFALO HIDE</t>
+        </is>
+      </c>
+      <c r="E25" s="123" t="n">
+        <v>9263.5</v>
+      </c>
+      <c r="F25" s="123" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="G25" s="123">
+        <f>F25 * E25</f>
         <v/>
       </c>
     </row>
     <row r="26" ht="35" customHeight="1">
-      <c r="A26" s="132" t="n">
-        <v>4</v>
-      </c>
-      <c r="B26" s="127" t="inlineStr">
-        <is>
-          <t>SJ0B-317</t>
-        </is>
-      </c>
-      <c r="C26" s="127" t="inlineStr">
-        <is>
-          <t>1.23.07.0220D</t>
-        </is>
-      </c>
-      <c r="D26" s="130" t="n"/>
-      <c r="E26" s="133" t="n"/>
-      <c r="F26" s="134" t="n">
-        <v>1588.2</v>
-      </c>
-      <c r="G26" s="134" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="H26" s="134">
-        <f>G26 * F26</f>
+      <c r="A26" s="124" t="n"/>
+      <c r="B26" s="121" t="inlineStr">
+        <is>
+          <t>9000606101</t>
+        </is>
+      </c>
+      <c r="C26" s="121" t="inlineStr">
+        <is>
+          <t>01.10.W783049</t>
+        </is>
+      </c>
+      <c r="D26" s="122" t="inlineStr">
+        <is>
+          <t>BUFFALO HIDE</t>
+        </is>
+      </c>
+      <c r="E26" s="123" t="n">
+        <v>112.5</v>
+      </c>
+      <c r="F26" s="123" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="G26" s="123">
+        <f>F26 * E26</f>
         <v/>
       </c>
     </row>
     <row r="27" ht="35" customFormat="1" customHeight="1" s="1">
-      <c r="A27" s="135" t="inlineStr">
-        <is>
-          <t xml:space="preserve">TOTAL OF: </t>
-        </is>
-      </c>
-      <c r="B27" s="121" t="n"/>
-      <c r="C27" s="121" t="n"/>
-      <c r="D27" s="125" t="inlineStr">
-        <is>
-          <t>0 PALLETS</t>
-        </is>
-      </c>
-      <c r="E27" s="125">
-        <f>SUM(E23:E26)</f>
-        <v/>
-      </c>
-      <c r="F27" s="125">
-        <f>SUM(F23:F26)</f>
-        <v/>
-      </c>
-      <c r="G27" s="121" t="n"/>
-      <c r="H27" s="121" t="n"/>
-    </row>
-    <row r="28" ht="42" customHeight="1">
-      <c r="A28" s="101" t="inlineStr">
+      <c r="A27" s="124" t="n"/>
+      <c r="B27" s="121" t="inlineStr">
+        <is>
+          <t>9000678466</t>
+        </is>
+      </c>
+      <c r="C27" s="121" t="inlineStr">
+        <is>
+          <t>01.10.W783049</t>
+        </is>
+      </c>
+      <c r="D27" s="122" t="inlineStr">
+        <is>
+          <t>BUFFALO HIDE</t>
+        </is>
+      </c>
+      <c r="E27" s="123" t="n">
+        <v>10077.9</v>
+      </c>
+      <c r="F27" s="123" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="G27" s="123">
+        <f>F27 * E27</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" ht="35" customHeight="1">
+      <c r="A28" s="124" t="n"/>
+      <c r="B28" s="121" t="inlineStr">
+        <is>
+          <t>9000707953</t>
+        </is>
+      </c>
+      <c r="C28" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U741023</t>
+        </is>
+      </c>
+      <c r="D28" s="122" t="inlineStr">
+        <is>
+          <t>BUFFALO HIDE</t>
+        </is>
+      </c>
+      <c r="E28" s="123" t="n">
+        <v>18953.2</v>
+      </c>
+      <c r="F28" s="123" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="G28" s="123">
+        <f>F28 * E28</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" ht="35" customHeight="1">
+      <c r="A29" s="124" t="n"/>
+      <c r="B29" s="121" t="inlineStr">
+        <is>
+          <t>9000707953</t>
+        </is>
+      </c>
+      <c r="C29" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U741023</t>
+        </is>
+      </c>
+      <c r="D29" s="122" t="inlineStr">
+        <is>
+          <t>BUFFALO HIDE</t>
+        </is>
+      </c>
+      <c r="E29" s="123" t="n">
+        <v>56.5</v>
+      </c>
+      <c r="F29" s="123" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="G29" s="123">
+        <f>F29 * E29</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" ht="35" customHeight="1">
+      <c r="A30" s="124" t="n"/>
+      <c r="B30" s="121" t="inlineStr">
+        <is>
+          <t>9000707953</t>
+        </is>
+      </c>
+      <c r="C30" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U741023</t>
+        </is>
+      </c>
+      <c r="D30" s="122" t="inlineStr">
+        <is>
+          <t>BUFFALO HIDE</t>
+        </is>
+      </c>
+      <c r="E30" s="123" t="n">
+        <v>487.6</v>
+      </c>
+      <c r="F30" s="123" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="G30" s="123">
+        <f>F30 * E30</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" ht="35" customHeight="1">
+      <c r="A31" s="124" t="n"/>
+      <c r="B31" s="121" t="inlineStr">
+        <is>
+          <t>9000719487</t>
+        </is>
+      </c>
+      <c r="C31" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U741023</t>
+        </is>
+      </c>
+      <c r="D31" s="122" t="inlineStr">
+        <is>
+          <t>BUFFALO HIDE</t>
+        </is>
+      </c>
+      <c r="E31" s="123" t="n">
+        <v>9892.700000000001</v>
+      </c>
+      <c r="F31" s="123" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="G31" s="123">
+        <f>F31 * E31</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" ht="35" customHeight="1">
+      <c r="A32" s="124" t="n"/>
+      <c r="B32" s="121" t="inlineStr">
+        <is>
+          <t>9000719487</t>
+        </is>
+      </c>
+      <c r="C32" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U722233</t>
+        </is>
+      </c>
+      <c r="D32" s="122" t="inlineStr">
+        <is>
+          <t>BUFFALO HIDE</t>
+        </is>
+      </c>
+      <c r="E32" s="123" t="n">
+        <v>9198.4</v>
+      </c>
+      <c r="F32" s="123" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="G32" s="123">
+        <f>F32 * E32</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" ht="35" customHeight="1">
+      <c r="A33" s="124" t="n"/>
+      <c r="B33" s="121" t="inlineStr">
+        <is>
+          <t>9000719487</t>
+        </is>
+      </c>
+      <c r="C33" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U722233</t>
+        </is>
+      </c>
+      <c r="D33" s="122" t="inlineStr">
+        <is>
+          <t>BUFFALO HIDE</t>
+        </is>
+      </c>
+      <c r="E33" s="123" t="n">
+        <v>635.8</v>
+      </c>
+      <c r="F33" s="123" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="G33" s="123">
+        <f>F33 * E33</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" ht="35" customHeight="1">
+      <c r="A34" s="124" t="n"/>
+      <c r="B34" s="121" t="inlineStr">
+        <is>
+          <t>9000719487</t>
+        </is>
+      </c>
+      <c r="C34" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U722233</t>
+        </is>
+      </c>
+      <c r="D34" s="122" t="inlineStr">
+        <is>
+          <t>cow lol</t>
+        </is>
+      </c>
+      <c r="E34" s="123" t="n">
+        <v>9074.200000000001</v>
+      </c>
+      <c r="F34" s="123" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="G34" s="123">
+        <f>F34 * E34</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" ht="35" customHeight="1">
+      <c r="A35" s="124" t="n"/>
+      <c r="B35" s="121" t="inlineStr">
+        <is>
+          <t>9000719487</t>
+        </is>
+      </c>
+      <c r="C35" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U722233</t>
+        </is>
+      </c>
+      <c r="D35" s="122" t="inlineStr">
+        <is>
+          <t>cow lol</t>
+        </is>
+      </c>
+      <c r="E35" s="123" t="n">
+        <v>247</v>
+      </c>
+      <c r="F35" s="123" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="G35" s="123">
+        <f>F35 * E35</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" ht="35" customHeight="1">
+      <c r="A36" s="124" t="n"/>
+      <c r="B36" s="121" t="inlineStr">
+        <is>
+          <t>9000707052</t>
+        </is>
+      </c>
+      <c r="C36" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U528110</t>
+        </is>
+      </c>
+      <c r="D36" s="122" t="inlineStr">
+        <is>
+          <t>cow lol</t>
+        </is>
+      </c>
+      <c r="E36" s="123" t="n">
+        <v>25569.9</v>
+      </c>
+      <c r="F36" s="123" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="G36" s="123">
+        <f>F36 * E36</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" ht="35" customHeight="1">
+      <c r="A37" s="124" t="n"/>
+      <c r="B37" s="121" t="inlineStr">
+        <is>
+          <t>9000707052</t>
+        </is>
+      </c>
+      <c r="C37" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U528110</t>
+        </is>
+      </c>
+      <c r="D37" s="122" t="inlineStr">
+        <is>
+          <t>cow lol</t>
+        </is>
+      </c>
+      <c r="E37" s="123" t="n">
+        <v>1162.8</v>
+      </c>
+      <c r="F37" s="123" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="G37" s="123">
+        <f>F37 * E37</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" ht="35" customHeight="1">
+      <c r="A38" s="124" t="n"/>
+      <c r="B38" s="121" t="inlineStr">
+        <is>
+          <t>9000707052</t>
+        </is>
+      </c>
+      <c r="C38" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U528103</t>
+        </is>
+      </c>
+      <c r="D38" s="122" t="inlineStr">
+        <is>
+          <t>cow lol</t>
+        </is>
+      </c>
+      <c r="E38" s="123" t="n">
+        <v>20551.4</v>
+      </c>
+      <c r="F38" s="123" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="G38" s="123">
+        <f>F38 * E38</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" ht="35" customHeight="1">
+      <c r="A39" s="124" t="n"/>
+      <c r="B39" s="121" t="inlineStr">
+        <is>
+          <t>9000707052</t>
+        </is>
+      </c>
+      <c r="C39" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U528103</t>
+        </is>
+      </c>
+      <c r="D39" s="122" t="inlineStr">
+        <is>
+          <t>cow lol</t>
+        </is>
+      </c>
+      <c r="E39" s="123" t="n">
+        <v>1513.7</v>
+      </c>
+      <c r="F39" s="123" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="G39" s="123">
+        <f>F39 * E39</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" ht="35" customHeight="1">
+      <c r="A40" s="112" t="n"/>
+      <c r="B40" s="112" t="inlineStr">
+        <is>
+          <t>TOTAL:</t>
+        </is>
+      </c>
+      <c r="C40" s="112" t="n"/>
+      <c r="D40" s="112" t="inlineStr">
+        <is>
+          <t>16 PALLETS</t>
+        </is>
+      </c>
+      <c r="E40" s="112">
+        <f>SUM(E22:E39)</f>
+        <v/>
+      </c>
+      <c r="F40" s="112" t="n"/>
+      <c r="G40" s="112">
+        <f>SUM(G22:G39)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" ht="21" customHeight="1">
+      <c r="A41" s="21" t="n"/>
+      <c r="B41" s="21" t="n"/>
+      <c r="C41" s="22" t="n"/>
+      <c r="D41" s="22" t="n"/>
+      <c r="E41" s="22" t="n"/>
+      <c r="F41" s="22" t="n"/>
+      <c r="G41" s="18" t="n"/>
+      <c r="L41" s="49" t="n"/>
+      <c r="M41" s="50" t="n"/>
+      <c r="N41" s="51" t="n"/>
+      <c r="O41" s="51" t="n"/>
+    </row>
+    <row r="42" ht="42" customHeight="1">
+      <c r="A42" s="101" t="inlineStr">
         <is>
           <t>Country of Original Cambodia</t>
         </is>
       </c>
-      <c r="D28" s="101" t="n"/>
-      <c r="E28" s="4" t="n"/>
-      <c r="F28" s="33" t="n"/>
-      <c r="G28" s="96" t="n"/>
-      <c r="L28" s="49" t="n"/>
-      <c r="M28" s="50" t="n"/>
-      <c r="N28" s="51" t="n"/>
-      <c r="O28" s="51" t="n"/>
-    </row>
-    <row r="29" ht="61.5" customHeight="1">
-      <c r="A29" s="28" t="inlineStr">
+      <c r="D42" s="101" t="n"/>
+      <c r="E42" s="4" t="n"/>
+      <c r="F42" s="33" t="n"/>
+      <c r="G42" s="96" t="n"/>
+      <c r="L42" s="49" t="n"/>
+      <c r="M42" s="50" t="n"/>
+      <c r="N42" s="51" t="n"/>
+      <c r="O42" s="51" t="n"/>
+    </row>
+    <row r="43" ht="61.5" customHeight="1">
+      <c r="A43" s="28" t="inlineStr">
         <is>
           <t>Manufacture:</t>
         </is>
       </c>
-      <c r="B29" s="102" t="inlineStr">
+      <c r="B43" s="102" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
 XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="D29" s="102" t="n"/>
-      <c r="E29" s="102" t="n"/>
-      <c r="F29" s="4" t="n"/>
-      <c r="G29" s="96" t="n"/>
-      <c r="L29" s="49" t="n"/>
-      <c r="M29" s="50" t="n"/>
-      <c r="N29" s="51" t="n"/>
-      <c r="O29" s="51" t="n"/>
-    </row>
-    <row r="30" ht="42" customHeight="1">
-      <c r="A30" s="103" t="inlineStr">
+      <c r="D43" s="102" t="n"/>
+      <c r="E43" s="102" t="n"/>
+      <c r="F43" s="4" t="n"/>
+      <c r="G43" s="96" t="n"/>
+      <c r="L43" s="49" t="n"/>
+      <c r="M43" s="50" t="n"/>
+      <c r="N43" s="51" t="n"/>
+      <c r="O43" s="51" t="n"/>
+    </row>
+    <row r="44" ht="42" customHeight="1">
+      <c r="A44" s="103" t="inlineStr">
         <is>
           <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
                                                   /BANK OF CHINA PHNOM PENH BRANCH</t>
         </is>
       </c>
-      <c r="D30" s="103" t="n"/>
-      <c r="E30" s="103" t="n"/>
-      <c r="F30" s="103" t="n"/>
-      <c r="G30" s="96" t="n"/>
-      <c r="L30" s="49" t="n"/>
-      <c r="M30" s="50" t="n"/>
-      <c r="N30" s="51" t="n"/>
-      <c r="O30" s="51" t="n"/>
-    </row>
-    <row r="31" ht="24.75" customHeight="1">
-      <c r="A31" s="99" t="inlineStr">
+      <c r="D44" s="103" t="n"/>
+      <c r="E44" s="103" t="n"/>
+      <c r="F44" s="103" t="n"/>
+      <c r="G44" s="96" t="n"/>
+      <c r="L44" s="49" t="n"/>
+      <c r="M44" s="50" t="n"/>
+      <c r="N44" s="51" t="n"/>
+      <c r="O44" s="51" t="n"/>
+    </row>
+    <row r="45" ht="24.75" customHeight="1">
+      <c r="A45" s="99" t="inlineStr">
         <is>
           <t>A/C NO:100001100764430</t>
         </is>
       </c>
-      <c r="L31" s="49" t="n"/>
-      <c r="M31" s="50" t="n"/>
-      <c r="N31" s="51" t="n"/>
-      <c r="O31" s="51" t="n"/>
-    </row>
-    <row r="32" ht="27" customHeight="1">
-      <c r="A32" s="99" t="inlineStr">
+      <c r="L45" s="49" t="n"/>
+      <c r="M45" s="50" t="n"/>
+      <c r="N45" s="51" t="n"/>
+      <c r="O45" s="51" t="n"/>
+    </row>
+    <row r="46" ht="27" customHeight="1">
+      <c r="A46" s="99" t="inlineStr">
         <is>
           <t>SWIFT CODE  ：BKCHKHPPXXX</t>
         </is>
       </c>
-      <c r="L32" s="49" t="n"/>
-      <c r="M32" s="50" t="n"/>
-      <c r="N32" s="51" t="n"/>
-      <c r="O32" s="51" t="n"/>
-    </row>
-    <row r="33" ht="27.75" customHeight="1">
-      <c r="E33" s="81" t="inlineStr">
+      <c r="L46" s="49" t="n"/>
+      <c r="M46" s="50" t="n"/>
+      <c r="N46" s="51" t="n"/>
+      <c r="O46" s="51" t="n"/>
+    </row>
+    <row r="47" ht="21" customHeight="1">
+      <c r="E47" s="81" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
       </c>
-      <c r="F33" s="81" t="n"/>
-      <c r="G33" s="81" t="n"/>
-      <c r="H33" s="81" t="n"/>
-      <c r="L33" s="49" t="n"/>
-      <c r="M33" s="50" t="n"/>
-      <c r="N33" s="51" t="n"/>
-      <c r="O33" s="51" t="n"/>
-    </row>
-    <row r="34" ht="27.75" customHeight="1">
-      <c r="D34" s="78" t="n"/>
-      <c r="E34" s="76" t="n"/>
-      <c r="F34" s="79" t="inlineStr">
+      <c r="F47" s="81" t="n"/>
+      <c r="G47" s="81" t="n"/>
+      <c r="H47" s="81" t="n"/>
+      <c r="L47" s="49" t="n"/>
+      <c r="M47" s="50" t="n"/>
+      <c r="N47" s="51" t="n"/>
+      <c r="O47" s="51" t="n"/>
+    </row>
+    <row r="48" ht="21" customHeight="1">
+      <c r="D48" s="78" t="n"/>
+      <c r="E48" s="76" t="n"/>
+      <c r="F48" s="79" t="inlineStr">
         <is>
           <t>Sign &amp; Stamp</t>
         </is>
       </c>
-      <c r="G34" s="80" t="n"/>
-      <c r="L34" s="49" t="n"/>
-      <c r="M34" s="50" t="n"/>
-      <c r="N34" s="51" t="n"/>
-      <c r="O34" s="51" t="n"/>
-    </row>
-    <row r="35" ht="27.75" customHeight="1">
-      <c r="D35" s="78" t="n"/>
-      <c r="E35" s="76" t="n"/>
-      <c r="F35" s="76" t="n"/>
-      <c r="G35" s="80" t="n"/>
-      <c r="L35" s="49" t="n"/>
-      <c r="M35" s="50" t="n"/>
-      <c r="N35" s="51" t="n"/>
-      <c r="O35" s="51" t="n"/>
-    </row>
-    <row r="36" ht="24.75" customHeight="1">
-      <c r="D36" s="78" t="n"/>
-      <c r="E36" s="76" t="n"/>
-      <c r="F36" s="76" t="n"/>
-      <c r="G36" s="80" t="n"/>
-      <c r="L36" s="49" t="n"/>
-      <c r="M36" s="50" t="n"/>
-      <c r="N36" s="51" t="n"/>
-      <c r="O36" s="51" t="n"/>
-    </row>
-    <row r="37" ht="21" customHeight="1">
-      <c r="D37" s="78" t="n"/>
-      <c r="E37" s="76" t="n"/>
-      <c r="F37" s="77" t="inlineStr">
+      <c r="G48" s="80" t="n"/>
+      <c r="L48" s="49" t="n"/>
+      <c r="M48" s="50" t="n"/>
+      <c r="N48" s="51" t="n"/>
+      <c r="O48" s="51" t="n"/>
+    </row>
+    <row r="49" ht="21" customHeight="1">
+      <c r="D49" s="78" t="n"/>
+      <c r="E49" s="76" t="n"/>
+      <c r="F49" s="76" t="n"/>
+      <c r="G49" s="80" t="n"/>
+      <c r="L49" s="49" t="n"/>
+      <c r="M49" s="50" t="n"/>
+      <c r="N49" s="51" t="n"/>
+      <c r="O49" s="51" t="n"/>
+    </row>
+    <row r="50" ht="21" customHeight="1">
+      <c r="D50" s="78" t="n"/>
+      <c r="E50" s="76" t="n"/>
+      <c r="F50" s="76" t="n"/>
+      <c r="G50" s="80" t="n"/>
+      <c r="L50" s="49" t="n"/>
+      <c r="M50" s="50" t="n"/>
+      <c r="N50" s="51" t="n"/>
+      <c r="O50" s="51" t="n"/>
+    </row>
+    <row r="51" ht="17.25" customHeight="1">
+      <c r="D51" s="78" t="n"/>
+      <c r="E51" s="76" t="n"/>
+      <c r="F51" s="77" t="inlineStr">
         <is>
           <t>ZENG XUELI</t>
         </is>
       </c>
-      <c r="G37" s="77" t="n"/>
-      <c r="L37" s="49" t="n"/>
-      <c r="M37" s="50" t="n"/>
-      <c r="N37" s="51" t="n"/>
-      <c r="O37" s="51" t="n"/>
-    </row>
-    <row r="38" ht="21" customHeight="1">
-      <c r="D38" s="74" t="n"/>
-      <c r="E38" s="74" t="n"/>
-      <c r="F38" s="74" t="n"/>
-      <c r="G38" s="75" t="n"/>
-    </row>
-    <row r="39" ht="21" customHeight="1">
-      <c r="D39" s="74" t="n"/>
-      <c r="E39" s="74" t="n"/>
-      <c r="F39" s="74" t="n"/>
-      <c r="G39" s="75" t="n"/>
-    </row>
-    <row r="40" ht="21" customHeight="1">
-      <c r="D40" s="74" t="n"/>
-      <c r="E40" s="74" t="n"/>
-      <c r="F40" s="74" t="n"/>
-      <c r="G40" s="75" t="n"/>
-    </row>
-    <row r="41" ht="21" customHeight="1">
-      <c r="D41" s="74" t="n"/>
-      <c r="E41" s="74" t="n"/>
-      <c r="F41" s="74" t="n"/>
-      <c r="G41" s="75" t="n"/>
-    </row>
-    <row r="42" ht="21" customHeight="1">
-      <c r="D42" s="74" t="n"/>
-      <c r="E42" s="74" t="n"/>
-      <c r="F42" s="74" t="n"/>
-      <c r="G42" s="75" t="n"/>
-    </row>
-    <row r="43" ht="21" customHeight="1">
-      <c r="D43" s="74" t="n"/>
-      <c r="E43" s="74" t="n"/>
-      <c r="F43" s="74" t="n"/>
-      <c r="G43" s="75" t="n"/>
-    </row>
-    <row r="44" ht="21" customHeight="1">
-      <c r="D44" s="74" t="n"/>
-      <c r="E44" s="74" t="n"/>
-      <c r="F44" s="74" t="n"/>
-      <c r="G44" s="75" t="n"/>
-    </row>
-    <row r="45" ht="25.5" customHeight="1">
-      <c r="D45" s="74" t="n"/>
-      <c r="E45" s="74" t="n"/>
-      <c r="F45" s="74" t="n"/>
-      <c r="G45" s="75" t="n"/>
-    </row>
-    <row r="46" ht="21" customHeight="1">
-      <c r="D46" s="74" t="n"/>
-      <c r="E46" s="74" t="n"/>
-      <c r="F46" s="74" t="n"/>
-      <c r="G46" s="75" t="n"/>
-    </row>
-    <row r="47" ht="21" customHeight="1">
-      <c r="D47" s="74" t="n"/>
-      <c r="E47" s="74" t="n"/>
-      <c r="F47" s="74" t="n"/>
-      <c r="G47" s="75" t="n"/>
-    </row>
-    <row r="48" ht="21" customHeight="1">
-      <c r="D48" s="74" t="n"/>
-      <c r="E48" s="74" t="n"/>
-      <c r="F48" s="74" t="n"/>
-      <c r="G48" s="75" t="n"/>
-    </row>
-    <row r="49" ht="21" customHeight="1">
-      <c r="D49" s="74" t="n"/>
-      <c r="E49" s="74" t="n"/>
-      <c r="F49" s="74" t="n"/>
-      <c r="G49" s="75" t="n"/>
-    </row>
-    <row r="50" ht="21" customHeight="1"/>
-    <row r="51" ht="17.25" customHeight="1"/>
-    <row r="52"/>
-    <row r="53"/>
-    <row r="54"/>
-    <row r="55"/>
-    <row r="56"/>
-    <row r="57"/>
-    <row r="58"/>
-    <row r="59"/>
-    <row r="60"/>
-    <row r="61"/>
-    <row r="62"/>
-    <row r="63" ht="15" customHeight="1"/>
+      <c r="G51" s="77" t="n"/>
+      <c r="L51" s="49" t="n"/>
+      <c r="M51" s="50" t="n"/>
+      <c r="N51" s="51" t="n"/>
+      <c r="O51" s="51" t="n"/>
+    </row>
+    <row r="52">
+      <c r="D52" s="74" t="n"/>
+      <c r="E52" s="74" t="n"/>
+      <c r="F52" s="74" t="n"/>
+      <c r="G52" s="75" t="n"/>
+    </row>
+    <row r="53">
+      <c r="D53" s="74" t="n"/>
+      <c r="E53" s="74" t="n"/>
+      <c r="F53" s="74" t="n"/>
+      <c r="G53" s="75" t="n"/>
+    </row>
+    <row r="54">
+      <c r="D54" s="74" t="n"/>
+      <c r="E54" s="74" t="n"/>
+      <c r="F54" s="74" t="n"/>
+      <c r="G54" s="75" t="n"/>
+    </row>
+    <row r="55">
+      <c r="D55" s="74" t="n"/>
+      <c r="E55" s="74" t="n"/>
+      <c r="F55" s="74" t="n"/>
+      <c r="G55" s="75" t="n"/>
+    </row>
+    <row r="56">
+      <c r="D56" s="74" t="n"/>
+      <c r="E56" s="74" t="n"/>
+      <c r="F56" s="74" t="n"/>
+      <c r="G56" s="75" t="n"/>
+    </row>
+    <row r="57">
+      <c r="D57" s="74" t="n"/>
+      <c r="E57" s="74" t="n"/>
+      <c r="F57" s="74" t="n"/>
+      <c r="G57" s="75" t="n"/>
+    </row>
+    <row r="58">
+      <c r="D58" s="74" t="n"/>
+      <c r="E58" s="74" t="n"/>
+      <c r="F58" s="74" t="n"/>
+      <c r="G58" s="75" t="n"/>
+    </row>
+    <row r="59">
+      <c r="D59" s="74" t="n"/>
+      <c r="E59" s="74" t="n"/>
+      <c r="F59" s="74" t="n"/>
+      <c r="G59" s="75" t="n"/>
+    </row>
+    <row r="60">
+      <c r="D60" s="74" t="n"/>
+      <c r="E60" s="74" t="n"/>
+      <c r="F60" s="74" t="n"/>
+      <c r="G60" s="75" t="n"/>
+    </row>
+    <row r="61">
+      <c r="D61" s="74" t="n"/>
+      <c r="E61" s="74" t="n"/>
+      <c r="F61" s="74" t="n"/>
+      <c r="G61" s="75" t="n"/>
+    </row>
+    <row r="62">
+      <c r="D62" s="74" t="n"/>
+      <c r="E62" s="74" t="n"/>
+      <c r="F62" s="74" t="n"/>
+      <c r="G62" s="75" t="n"/>
+    </row>
+    <row r="63" ht="15" customHeight="1">
+      <c r="D63" s="74" t="n"/>
+      <c r="E63" s="74" t="n"/>
+      <c r="F63" s="74" t="n"/>
+      <c r="G63" s="75" t="n"/>
+    </row>
     <row r="64"/>
     <row r="65"/>
     <row r="66"/>
@@ -3021,29 +3560,19 @@
     <row r="199"/>
     <row r="200"/>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="A28:C28"/>
+  <mergeCells count="12">
+    <mergeCell ref="A42:C42"/>
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B40"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="A3:G3"/>
     <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="A2:G2"/>
     <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="A46:G46"/>
   </mergeCells>
   <conditionalFormatting sqref="J23:J35">
     <cfRule type="duplicateValues" priority="1" stopIfTrue="1"/>
@@ -3117,14 +3646,14 @@
           <t>Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="B5" s="122" t="n"/>
-      <c r="C5" s="122" t="n"/>
-      <c r="D5" s="122" t="n"/>
-      <c r="E5" s="122" t="n"/>
-      <c r="F5" s="122" t="n"/>
-      <c r="G5" s="122" t="n"/>
-      <c r="H5" s="122" t="n"/>
-      <c r="I5" s="122" t="n"/>
+      <c r="B5" s="116" t="n"/>
+      <c r="C5" s="116" t="n"/>
+      <c r="D5" s="116" t="n"/>
+      <c r="E5" s="116" t="n"/>
+      <c r="F5" s="116" t="n"/>
+      <c r="G5" s="116" t="n"/>
+      <c r="H5" s="116" t="n"/>
+      <c r="I5" s="116" t="n"/>
     </row>
     <row r="6" ht="54" customHeight="1">
       <c r="A6" s="100" t="inlineStr">
@@ -3132,14 +3661,14 @@
           <t>PACKING LIST</t>
         </is>
       </c>
-      <c r="B6" s="123" t="n"/>
-      <c r="C6" s="123" t="n"/>
-      <c r="D6" s="123" t="n"/>
-      <c r="E6" s="123" t="n"/>
-      <c r="F6" s="123" t="n"/>
-      <c r="G6" s="123" t="n"/>
-      <c r="H6" s="123" t="n"/>
-      <c r="I6" s="123" t="n"/>
+      <c r="B6" s="117" t="n"/>
+      <c r="C6" s="117" t="n"/>
+      <c r="D6" s="117" t="n"/>
+      <c r="E6" s="117" t="n"/>
+      <c r="F6" s="117" t="n"/>
+      <c r="G6" s="117" t="n"/>
+      <c r="H6" s="117" t="n"/>
+      <c r="I6" s="117" t="n"/>
     </row>
     <row r="7" ht="18" customHeight="1">
       <c r="A7" s="4" t="n"/>
@@ -3156,7 +3685,7 @@
       </c>
       <c r="I7" s="87" t="inlineStr">
         <is>
-          <t>CLF2025-152</t>
+          <t>CLF2025-171</t>
         </is>
       </c>
     </row>
@@ -3180,7 +3709,7 @@
       </c>
       <c r="I8" s="85" t="inlineStr">
         <is>
-          <t>KB25012</t>
+          <t>JF25030</t>
         </is>
       </c>
     </row>
@@ -3198,8 +3727,8 @@
           <t>Date:</t>
         </is>
       </c>
-      <c r="I9" s="124" t="n">
-        <v>45803</v>
+      <c r="I9" s="118" t="n">
+        <v>45819</v>
       </c>
     </row>
     <row r="10" ht="22.5" customHeight="1">
@@ -3348,769 +3877,1409 @@
       <c r="B20" s="65" t="n"/>
     </row>
     <row r="21" ht="27" customHeight="1">
-      <c r="A21" s="136" t="inlineStr">
+      <c r="A21" s="125" t="inlineStr">
         <is>
           <t>Mark &amp; Nº</t>
         </is>
       </c>
-      <c r="B21" s="136" t="inlineStr">
+      <c r="B21" s="125" t="inlineStr">
         <is>
           <t>P.O Nº</t>
         </is>
       </c>
-      <c r="C21" s="136" t="inlineStr">
+      <c r="C21" s="125" t="inlineStr">
         <is>
           <t>ITEM Nº</t>
         </is>
       </c>
-      <c r="D21" s="136" t="inlineStr">
+      <c r="D21" s="125" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="E21" s="136" t="inlineStr">
+      <c r="E21" s="125" t="inlineStr">
         <is>
           <t>Quantity</t>
         </is>
       </c>
-      <c r="F21" s="110" t="n"/>
-      <c r="G21" s="136" t="inlineStr">
+      <c r="F21" s="113" t="n"/>
+      <c r="G21" s="125" t="inlineStr">
         <is>
           <t>G.W (kgs)</t>
         </is>
       </c>
-      <c r="H21" s="136" t="inlineStr">
+      <c r="H21" s="125" t="inlineStr">
         <is>
           <t>N.W (kgs)</t>
         </is>
       </c>
-      <c r="I21" s="136" t="inlineStr">
+      <c r="I21" s="125" t="inlineStr">
         <is>
           <t>CBM</t>
         </is>
       </c>
     </row>
     <row r="22" ht="27" customHeight="1">
-      <c r="A22" s="111" t="n"/>
-      <c r="B22" s="111" t="n"/>
-      <c r="C22" s="111" t="n"/>
-      <c r="D22" s="111" t="n"/>
-      <c r="E22" s="136" t="inlineStr">
+      <c r="A22" s="126" t="n"/>
+      <c r="B22" s="126" t="n"/>
+      <c r="C22" s="126" t="n"/>
+      <c r="D22" s="126" t="n"/>
+      <c r="E22" s="125" t="inlineStr">
         <is>
           <t>PCS</t>
         </is>
       </c>
-      <c r="F22" s="136" t="inlineStr">
+      <c r="F22" s="125" t="inlineStr">
         <is>
           <t>SF</t>
         </is>
       </c>
-      <c r="G22" s="111" t="n"/>
-      <c r="H22" s="111" t="n"/>
-      <c r="I22" s="111" t="n"/>
+      <c r="G22" s="126" t="n"/>
+      <c r="H22" s="126" t="n"/>
+      <c r="I22" s="126" t="n"/>
     </row>
     <row r="23" ht="27" customHeight="1">
-      <c r="A23" s="137" t="inlineStr">
+      <c r="A23" s="127" t="inlineStr">
         <is>
           <t>VENDOR#:</t>
         </is>
       </c>
-      <c r="B23" s="127" t="inlineStr">
-        <is>
-          <t>RB0604</t>
-        </is>
-      </c>
-      <c r="C23" s="127" t="inlineStr">
-        <is>
-          <t>1.23.07.0154J</t>
-        </is>
-      </c>
-      <c r="D23" s="138" t="inlineStr">
+      <c r="B23" s="121" t="inlineStr">
+        <is>
+          <t>9000619872</t>
+        </is>
+      </c>
+      <c r="C23" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U756033</t>
+        </is>
+      </c>
+      <c r="D23" s="121" t="inlineStr">
+        <is>
+          <t>BUFFALO HIDE</t>
+        </is>
+      </c>
+      <c r="E23" s="128" t="n">
+        <v>142</v>
+      </c>
+      <c r="F23" s="123" t="n">
+        <v>7438.8</v>
+      </c>
+      <c r="G23" s="123" t="n">
+        <v>630.3649</v>
+      </c>
+      <c r="H23" s="123" t="n">
+        <v>587.1892</v>
+      </c>
+      <c r="I23" s="129" t="n">
+        <v>1.9757</v>
+      </c>
+    </row>
+    <row r="24" ht="27" customHeight="1">
+      <c r="A24" s="130" t="inlineStr">
+        <is>
+          <t>Des: LEATHER</t>
+        </is>
+      </c>
+      <c r="B24" s="121" t="inlineStr">
+        <is>
+          <t>9000619872</t>
+        </is>
+      </c>
+      <c r="C24" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U756033</t>
+        </is>
+      </c>
+      <c r="D24" s="121" t="inlineStr">
+        <is>
+          <t>BUFFALO HIDE</t>
+        </is>
+      </c>
+      <c r="E24" s="128" t="n">
+        <v>6</v>
+      </c>
+      <c r="F24" s="123" t="n">
+        <v>242.7</v>
+      </c>
+      <c r="G24" s="123" t="n">
+        <v>26.6351</v>
+      </c>
+      <c r="H24" s="123" t="n">
+        <v>24.8108</v>
+      </c>
+      <c r="I24" s="129" t="n">
+        <v>0.0835</v>
+      </c>
+    </row>
+    <row r="25" ht="27" customHeight="1">
+      <c r="A25" s="130" t="inlineStr">
+        <is>
+          <t>Case Qty:</t>
+        </is>
+      </c>
+      <c r="B25" s="121" t="inlineStr">
+        <is>
+          <t>9000691966</t>
+        </is>
+      </c>
+      <c r="C25" s="121" t="inlineStr">
+        <is>
+          <t>01.10.W653191</t>
+        </is>
+      </c>
+      <c r="D25" s="121" t="inlineStr">
+        <is>
+          <t>BUFFALO HIDE</t>
+        </is>
+      </c>
+      <c r="E25" s="128" t="n">
+        <v>105</v>
+      </c>
+      <c r="F25" s="123" t="n">
+        <v>5748.5</v>
+      </c>
+      <c r="G25" s="123" t="n">
+        <v>450</v>
+      </c>
+      <c r="H25" s="123" t="n">
+        <v>405</v>
+      </c>
+      <c r="I25" s="129" t="n">
+        <v>2.178</v>
+      </c>
+    </row>
+    <row r="26" ht="27" customHeight="1">
+      <c r="A26" s="130" t="inlineStr">
+        <is>
+          <t>MADE IN CAMBODIA</t>
+        </is>
+      </c>
+      <c r="B26" s="121" t="inlineStr">
+        <is>
+          <t>9000606101</t>
+        </is>
+      </c>
+      <c r="C26" s="121" t="inlineStr">
+        <is>
+          <t>01.10.W783049</t>
+        </is>
+      </c>
+      <c r="D26" s="121" t="inlineStr">
+        <is>
+          <t>BUFFALO HIDE</t>
+        </is>
+      </c>
+      <c r="E26" s="128" t="n">
+        <v>163</v>
+      </c>
+      <c r="F26" s="123" t="n">
+        <v>9263.5</v>
+      </c>
+      <c r="G26" s="123" t="n">
+        <v>972.1084</v>
+      </c>
+      <c r="H26" s="123" t="n">
+        <v>927.9217</v>
+      </c>
+      <c r="I26" s="129" t="n">
+        <v>2.7219</v>
+      </c>
+    </row>
+    <row r="27" ht="27" customHeight="1">
+      <c r="A27" s="130" t="n"/>
+      <c r="B27" s="121" t="inlineStr">
+        <is>
+          <t>9000606101</t>
+        </is>
+      </c>
+      <c r="C27" s="121" t="inlineStr">
+        <is>
+          <t>01.10.W783049</t>
+        </is>
+      </c>
+      <c r="D27" s="121" t="inlineStr">
+        <is>
+          <t>BUFFALO HIDE</t>
+        </is>
+      </c>
+      <c r="E27" s="128" t="n">
+        <v>3</v>
+      </c>
+      <c r="F27" s="123" t="n">
+        <v>112.5</v>
+      </c>
+      <c r="G27" s="123" t="n">
+        <v>17.8916</v>
+      </c>
+      <c r="H27" s="123" t="n">
+        <v>17.0783</v>
+      </c>
+      <c r="I27" s="129" t="n">
+        <v>0.0501</v>
+      </c>
+    </row>
+    <row r="28" ht="27" customHeight="1">
+      <c r="A28" s="130" t="n"/>
+      <c r="B28" s="121" t="inlineStr">
+        <is>
+          <t>9000678466</t>
+        </is>
+      </c>
+      <c r="C28" s="121" t="inlineStr">
+        <is>
+          <t>01.10.W783049</t>
+        </is>
+      </c>
+      <c r="D28" s="121" t="inlineStr">
+        <is>
+          <t>BUFFALO HIDE</t>
+        </is>
+      </c>
+      <c r="E28" s="128" t="n">
+        <v>180</v>
+      </c>
+      <c r="F28" s="123" t="n">
+        <v>10077.9</v>
+      </c>
+      <c r="G28" s="123" t="n">
+        <v>1075.5</v>
+      </c>
+      <c r="H28" s="123" t="n">
+        <v>1030.5</v>
+      </c>
+      <c r="I28" s="129" t="n">
+        <v>2.97</v>
+      </c>
+    </row>
+    <row r="29" ht="27" customHeight="1">
+      <c r="A29" s="130" t="n"/>
+      <c r="B29" s="121" t="n">
+        <v>9000707953</v>
+      </c>
+      <c r="C29" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U741023</t>
+        </is>
+      </c>
+      <c r="D29" s="121" t="inlineStr">
+        <is>
+          <t>BUFFALO HIDE</t>
+        </is>
+      </c>
+      <c r="E29" s="128" t="n">
+        <v>93</v>
+      </c>
+      <c r="F29" s="123" t="n">
+        <v>5423.2</v>
+      </c>
+      <c r="G29" s="123" t="n">
+        <v>594</v>
+      </c>
+      <c r="H29" s="123" t="n">
+        <v>549</v>
+      </c>
+      <c r="I29" s="129" t="n">
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="30" ht="27" customHeight="1">
+      <c r="A30" s="130" t="n"/>
+      <c r="B30" s="121" t="n">
+        <v>9000707953</v>
+      </c>
+      <c r="C30" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U741023</t>
+        </is>
+      </c>
+      <c r="D30" s="121" t="inlineStr">
+        <is>
+          <t>BUFFALO HIDE</t>
+        </is>
+      </c>
+      <c r="E30" s="128" t="n">
+        <v>97</v>
+      </c>
+      <c r="F30" s="123" t="n">
+        <v>5447.3</v>
+      </c>
+      <c r="G30" s="123" t="n">
+        <v>593.5</v>
+      </c>
+      <c r="H30" s="123" t="n">
+        <v>548.5</v>
+      </c>
+      <c r="I30" s="129" t="n">
+        <v>1.9404</v>
+      </c>
+    </row>
+    <row r="31" ht="27" customHeight="1">
+      <c r="A31" s="130" t="n"/>
+      <c r="B31" s="121" t="n">
+        <v>9000707953</v>
+      </c>
+      <c r="C31" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U741023</t>
+        </is>
+      </c>
+      <c r="D31" s="121" t="inlineStr">
+        <is>
+          <t>BUFFALO HIDE</t>
+        </is>
+      </c>
+      <c r="E31" s="128" t="n">
+        <v>94</v>
+      </c>
+      <c r="F31" s="123" t="n">
+        <v>5479.1</v>
+      </c>
+      <c r="G31" s="123" t="n">
+        <v>603.0842</v>
+      </c>
+      <c r="H31" s="123" t="n">
+        <v>558.5579</v>
+      </c>
+      <c r="I31" s="129" t="n">
+        <v>2.1943</v>
+      </c>
+    </row>
+    <row r="32" ht="27" customHeight="1">
+      <c r="A32" s="130" t="n"/>
+      <c r="B32" s="121" t="n">
+        <v>9000707953</v>
+      </c>
+      <c r="C32" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U741023</t>
+        </is>
+      </c>
+      <c r="D32" s="121" t="inlineStr">
+        <is>
+          <t>BUFFALO HIDE</t>
+        </is>
+      </c>
+      <c r="E32" s="128" t="n">
+        <v>1</v>
+      </c>
+      <c r="F32" s="123" t="n">
+        <v>56.5</v>
+      </c>
+      <c r="G32" s="123" t="n">
+        <v>6.4158</v>
+      </c>
+      <c r="H32" s="123" t="n">
+        <v>5.9421</v>
+      </c>
+      <c r="I32" s="129" t="n">
+        <v>0.0233</v>
+      </c>
+    </row>
+    <row r="33" ht="27" customHeight="1">
+      <c r="A33" s="130" t="n"/>
+      <c r="B33" s="121" t="n">
+        <v>9000707953</v>
+      </c>
+      <c r="C33" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U741023</t>
+        </is>
+      </c>
+      <c r="D33" s="121" t="inlineStr">
+        <is>
+          <t>BUFFALO HIDE</t>
+        </is>
+      </c>
+      <c r="E33" s="128" t="n">
+        <v>45</v>
+      </c>
+      <c r="F33" s="123" t="n">
+        <v>2603.6</v>
+      </c>
+      <c r="G33" s="123" t="n">
+        <v>283.4211</v>
+      </c>
+      <c r="H33" s="123" t="n">
+        <v>247.8947</v>
+      </c>
+      <c r="I33" s="129" t="n">
+        <v>1.2193</v>
+      </c>
+    </row>
+    <row r="34" ht="27" customHeight="1">
+      <c r="A34" s="130" t="n"/>
+      <c r="B34" s="121" t="n">
+        <v>9000707953</v>
+      </c>
+      <c r="C34" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U741023</t>
+        </is>
+      </c>
+      <c r="D34" s="121" t="inlineStr">
+        <is>
+          <t>BUFFALO HIDE</t>
+        </is>
+      </c>
+      <c r="E34" s="128" t="n">
+        <v>12</v>
+      </c>
+      <c r="F34" s="123" t="n">
+        <v>487.6</v>
+      </c>
+      <c r="G34" s="123" t="n">
+        <v>75.5789</v>
+      </c>
+      <c r="H34" s="123" t="n">
+        <v>66.1053</v>
+      </c>
+      <c r="I34" s="129" t="n">
+        <v>0.3251</v>
+      </c>
+    </row>
+    <row r="35" ht="27" customHeight="1">
+      <c r="A35" s="130" t="n"/>
+      <c r="B35" s="121" t="inlineStr">
+        <is>
+          <t>LEATHER (HS.CODE: 4107.12.00)</t>
+        </is>
+      </c>
+      <c r="C35" s="113" t="n"/>
+      <c r="D35" s="122" t="n"/>
+      <c r="E35" s="128" t="n"/>
+      <c r="F35" s="123" t="n"/>
+      <c r="G35" s="123" t="n"/>
+      <c r="H35" s="123" t="n"/>
+      <c r="I35" s="129" t="n"/>
+    </row>
+    <row r="36" ht="27" customHeight="1">
+      <c r="A36" s="112" t="n"/>
+      <c r="B36" s="112" t="inlineStr">
+        <is>
+          <t>TOTAL:</t>
+        </is>
+      </c>
+      <c r="C36" s="112" t="n"/>
+      <c r="D36" s="112" t="inlineStr">
+        <is>
+          <t>8 PALLETS</t>
+        </is>
+      </c>
+      <c r="E36" s="131">
+        <f>SUM(E23:E34)</f>
+        <v/>
+      </c>
+      <c r="F36" s="114">
+        <f>SUM(F23:F34)</f>
+        <v/>
+      </c>
+      <c r="G36" s="114">
+        <f>SUM(G23:G34)</f>
+        <v/>
+      </c>
+      <c r="H36" s="114">
+        <f>SUM(H23:H34)</f>
+        <v/>
+      </c>
+      <c r="I36" s="132">
+        <f>SUM(I23:I34)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" ht="27.75" customHeight="1"/>
+    <row r="38" ht="27.75" customHeight="1">
+      <c r="B38" s="133" t="inlineStr">
+        <is>
+          <t>TOTAL OF:</t>
+        </is>
+      </c>
+      <c r="D38" s="133" t="inlineStr">
+        <is>
+          <t>8 PALLETS</t>
+        </is>
+      </c>
+      <c r="E38" s="134">
+        <f>SUM(E23:E34)</f>
+        <v/>
+      </c>
+      <c r="F38" s="135">
+        <f>SUM(F23:F34)</f>
+        <v/>
+      </c>
+      <c r="G38" s="135">
+        <f>SUM(G23:G34)</f>
+        <v/>
+      </c>
+      <c r="H38" s="135">
+        <f>SUM(H23:H34)</f>
+        <v/>
+      </c>
+      <c r="I38" s="136">
+        <f>SUM(I23:I34)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" ht="27" customHeight="1">
+      <c r="A39" s="125" t="inlineStr">
+        <is>
+          <t>Mark &amp; Nº</t>
+        </is>
+      </c>
+      <c r="B39" s="125" t="inlineStr">
+        <is>
+          <t>P.O Nº</t>
+        </is>
+      </c>
+      <c r="C39" s="125" t="inlineStr">
+        <is>
+          <t>ITEM Nº</t>
+        </is>
+      </c>
+      <c r="D39" s="125" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="E39" s="125" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="F39" s="113" t="n"/>
+      <c r="G39" s="125" t="inlineStr">
+        <is>
+          <t>G.W (kgs)</t>
+        </is>
+      </c>
+      <c r="H39" s="125" t="inlineStr">
+        <is>
+          <t>N.W (kgs)</t>
+        </is>
+      </c>
+      <c r="I39" s="125" t="inlineStr">
+        <is>
+          <t>CBM</t>
+        </is>
+      </c>
+    </row>
+    <row r="40" ht="27" customHeight="1">
+      <c r="A40" s="126" t="n"/>
+      <c r="B40" s="126" t="n"/>
+      <c r="C40" s="126" t="n"/>
+      <c r="D40" s="126" t="n"/>
+      <c r="E40" s="125" t="inlineStr">
+        <is>
+          <t>PCS</t>
+        </is>
+      </c>
+      <c r="F40" s="125" t="inlineStr">
+        <is>
+          <t>SF</t>
+        </is>
+      </c>
+      <c r="G40" s="126" t="n"/>
+      <c r="H40" s="126" t="n"/>
+      <c r="I40" s="126" t="n"/>
+    </row>
+    <row r="41" ht="27" customHeight="1">
+      <c r="A41" s="127" t="inlineStr">
+        <is>
+          <t>VENDOR#:</t>
+        </is>
+      </c>
+      <c r="B41" s="121" t="n">
+        <v>9000719487</v>
+      </c>
+      <c r="C41" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U741023</t>
+        </is>
+      </c>
+      <c r="D41" s="121" t="inlineStr">
+        <is>
+          <t>BUFFALO HIDE</t>
+        </is>
+      </c>
+      <c r="E41" s="128" t="n">
+        <v>171</v>
+      </c>
+      <c r="F41" s="123" t="n">
+        <v>9892.700000000001</v>
+      </c>
+      <c r="G41" s="123" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" s="123" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" s="129" t="n">
+        <v>2.6928</v>
+      </c>
+    </row>
+    <row r="42" ht="27" customHeight="1">
+      <c r="A42" s="130" t="inlineStr">
+        <is>
+          <t>Des: LEATHER</t>
+        </is>
+      </c>
+      <c r="B42" s="121" t="n">
+        <v>9000719487</v>
+      </c>
+      <c r="C42" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U722233</t>
+        </is>
+      </c>
+      <c r="D42" s="121" t="inlineStr">
+        <is>
+          <t>BUFFALO HIDE</t>
+        </is>
+      </c>
+      <c r="E42" s="128" t="n">
+        <v>172</v>
+      </c>
+      <c r="F42" s="123" t="n">
+        <v>9198.4</v>
+      </c>
+      <c r="G42" s="123" t="n">
+        <v>610.234</v>
+      </c>
+      <c r="H42" s="123" t="n">
+        <v>569.0638</v>
+      </c>
+      <c r="I42" s="129" t="n">
+        <v>2.2462</v>
+      </c>
+    </row>
+    <row r="43" ht="27" customHeight="1">
+      <c r="A43" s="130" t="inlineStr">
+        <is>
+          <t>Case Qty:</t>
+        </is>
+      </c>
+      <c r="B43" s="121" t="n">
+        <v>9000719487</v>
+      </c>
+      <c r="C43" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U722233</t>
+        </is>
+      </c>
+      <c r="D43" s="121" t="inlineStr">
+        <is>
+          <t>BUFFALO HIDE</t>
+        </is>
+      </c>
+      <c r="E43" s="128" t="n">
+        <v>16</v>
+      </c>
+      <c r="F43" s="123" t="n">
+        <v>635.8</v>
+      </c>
+      <c r="G43" s="123" t="n">
+        <v>56.766</v>
+      </c>
+      <c r="H43" s="123" t="n">
+        <v>52.9362</v>
+      </c>
+      <c r="I43" s="129" t="n">
+        <v>0.209</v>
+      </c>
+    </row>
+    <row r="44" ht="27" customHeight="1">
+      <c r="A44" s="130" t="inlineStr">
+        <is>
+          <t>MADE IN CAMBODIA</t>
+        </is>
+      </c>
+      <c r="B44" s="121" t="n">
+        <v>9000719487</v>
+      </c>
+      <c r="C44" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U722233</t>
+        </is>
+      </c>
+      <c r="D44" s="121" t="inlineStr">
+        <is>
+          <t>cow lol</t>
+        </is>
+      </c>
+      <c r="E44" s="128" t="n">
+        <v>167</v>
+      </c>
+      <c r="F44" s="123" t="n">
+        <v>9074.200000000001</v>
+      </c>
+      <c r="G44" s="123" t="n">
+        <v>628.1919</v>
+      </c>
+      <c r="H44" s="123" t="n">
+        <v>584.5</v>
+      </c>
+      <c r="I44" s="129" t="n">
+        <v>2.3069</v>
+      </c>
+    </row>
+    <row r="45" ht="27" customHeight="1">
+      <c r="A45" s="130" t="n"/>
+      <c r="B45" s="121" t="n">
+        <v>9000719487</v>
+      </c>
+      <c r="C45" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U722233</t>
+        </is>
+      </c>
+      <c r="D45" s="121" t="inlineStr">
+        <is>
+          <t>cow lol</t>
+        </is>
+      </c>
+      <c r="E45" s="128" t="n">
+        <v>5</v>
+      </c>
+      <c r="F45" s="123" t="n">
+        <v>247</v>
+      </c>
+      <c r="G45" s="123" t="n">
+        <v>18.8081</v>
+      </c>
+      <c r="H45" s="123" t="n">
+        <v>17.5</v>
+      </c>
+      <c r="I45" s="129" t="n">
+        <v>0.06909999999999999</v>
+      </c>
+    </row>
+    <row r="46" ht="27" customHeight="1">
+      <c r="A46" s="130" t="n"/>
+      <c r="B46" s="121" t="n">
+        <v>9000707052</v>
+      </c>
+      <c r="C46" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U528110</t>
+        </is>
+      </c>
+      <c r="D46" s="121" t="inlineStr">
+        <is>
+          <t>cow lol</t>
+        </is>
+      </c>
+      <c r="E46" s="128" t="n">
+        <v>97</v>
+      </c>
+      <c r="F46" s="123" t="n">
+        <v>5048.7</v>
+      </c>
+      <c r="G46" s="123" t="n">
+        <v>455.5</v>
+      </c>
+      <c r="H46" s="123" t="n">
+        <v>410.5</v>
+      </c>
+      <c r="I46" s="129" t="n">
+        <v>1.782</v>
+      </c>
+    </row>
+    <row r="47" ht="27" customHeight="1">
+      <c r="A47" s="130" t="n"/>
+      <c r="B47" s="121" t="n">
+        <v>9000707052</v>
+      </c>
+      <c r="C47" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U528110</t>
+        </is>
+      </c>
+      <c r="D47" s="121" t="inlineStr">
+        <is>
+          <t>cow lol</t>
+        </is>
+      </c>
+      <c r="E47" s="128" t="n">
+        <v>94</v>
+      </c>
+      <c r="F47" s="123" t="n">
+        <v>5012.9</v>
+      </c>
+      <c r="G47" s="123" t="n">
+        <v>455.5</v>
+      </c>
+      <c r="H47" s="123" t="n">
+        <v>410.5</v>
+      </c>
+      <c r="I47" s="129" t="n">
+        <v>1.782</v>
+      </c>
+    </row>
+    <row r="48" ht="27" customHeight="1">
+      <c r="A48" s="130" t="n"/>
+      <c r="B48" s="121" t="n">
+        <v>9000707052</v>
+      </c>
+      <c r="C48" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U528110</t>
+        </is>
+      </c>
+      <c r="D48" s="121" t="inlineStr">
+        <is>
+          <t>cow lol</t>
+        </is>
+      </c>
+      <c r="E48" s="128" t="n">
+        <v>95</v>
+      </c>
+      <c r="F48" s="123" t="n">
+        <v>4996.9</v>
+      </c>
+      <c r="G48" s="123" t="n">
+        <v>452</v>
+      </c>
+      <c r="H48" s="123" t="n">
+        <v>407</v>
+      </c>
+      <c r="I48" s="129" t="n">
+        <v>1.7424</v>
+      </c>
+    </row>
+    <row r="49" ht="27" customHeight="1">
+      <c r="A49" s="130" t="n"/>
+      <c r="B49" s="121" t="n">
+        <v>9000707052</v>
+      </c>
+      <c r="C49" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U528110</t>
+        </is>
+      </c>
+      <c r="D49" s="121" t="inlineStr">
+        <is>
+          <t>cow lol</t>
+        </is>
+      </c>
+      <c r="E49" s="128" t="n">
+        <v>198</v>
+      </c>
+      <c r="F49" s="123" t="n">
+        <v>10511.4</v>
+      </c>
+      <c r="G49" s="123" t="n">
+        <v>876.6079</v>
+      </c>
+      <c r="H49" s="123" t="n">
+        <v>837.3568</v>
+      </c>
+      <c r="I49" s="129" t="n">
+        <v>2.4869</v>
+      </c>
+    </row>
+    <row r="50" ht="27" customHeight="1">
+      <c r="A50" s="130" t="n"/>
+      <c r="B50" s="121" t="n">
+        <v>9000707052</v>
+      </c>
+      <c r="C50" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U528110</t>
+        </is>
+      </c>
+      <c r="D50" s="121" t="inlineStr">
+        <is>
+          <t>cow lol</t>
+        </is>
+      </c>
+      <c r="E50" s="128" t="n">
+        <v>29</v>
+      </c>
+      <c r="F50" s="123" t="n">
+        <v>1162.8</v>
+      </c>
+      <c r="G50" s="123" t="n">
+        <v>128.3921</v>
+      </c>
+      <c r="H50" s="123" t="n">
+        <v>122.6432</v>
+      </c>
+      <c r="I50" s="129" t="n">
+        <v>0.3643</v>
+      </c>
+    </row>
+    <row r="51" ht="27" customHeight="1">
+      <c r="A51" s="130" t="n"/>
+      <c r="B51" s="121" t="n">
+        <v>9000707052</v>
+      </c>
+      <c r="C51" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U528103</t>
+        </is>
+      </c>
+      <c r="D51" s="121" t="inlineStr">
+        <is>
+          <t>cow lol</t>
+        </is>
+      </c>
+      <c r="E51" s="128" t="n">
+        <v>200</v>
+      </c>
+      <c r="F51" s="123" t="n">
+        <v>10017.2</v>
+      </c>
+      <c r="G51" s="123" t="n">
+        <v>858.5</v>
+      </c>
+      <c r="H51" s="123" t="n">
+        <v>813.5</v>
+      </c>
+      <c r="I51" s="129" t="n">
+        <v>2.5344</v>
+      </c>
+    </row>
+    <row r="52" ht="27" customHeight="1">
+      <c r="A52" s="130" t="n"/>
+      <c r="B52" s="121" t="n">
+        <v>9000707052</v>
+      </c>
+      <c r="C52" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U528103</t>
+        </is>
+      </c>
+      <c r="D52" s="121" t="inlineStr">
+        <is>
+          <t>cow lol</t>
+        </is>
+      </c>
+      <c r="E52" s="128" t="n">
+        <v>210</v>
+      </c>
+      <c r="F52" s="123" t="n">
+        <v>10534.2</v>
+      </c>
+      <c r="G52" s="123" t="n">
+        <v>865.4032</v>
+      </c>
+      <c r="H52" s="123" t="n">
+        <v>827.2984</v>
+      </c>
+      <c r="I52" s="129" t="n">
+        <v>2.5149</v>
+      </c>
+    </row>
+    <row r="53" ht="27" customHeight="1">
+      <c r="A53" s="130" t="n"/>
+      <c r="B53" s="121" t="n">
+        <v>9000707052</v>
+      </c>
+      <c r="C53" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U528103</t>
+        </is>
+      </c>
+      <c r="D53" s="121" t="inlineStr">
+        <is>
+          <t>cow lol</t>
+        </is>
+      </c>
+      <c r="E53" s="128" t="n">
+        <v>38</v>
+      </c>
+      <c r="F53" s="123" t="n">
+        <v>1513.7</v>
+      </c>
+      <c r="G53" s="123" t="n">
+        <v>156.5968</v>
+      </c>
+      <c r="H53" s="123" t="n">
+        <v>149.7016</v>
+      </c>
+      <c r="I53" s="129" t="n">
+        <v>0.4551</v>
+      </c>
+    </row>
+    <row r="54" ht="27" customFormat="1" customHeight="1" s="1">
+      <c r="A54" s="130" t="n"/>
+      <c r="B54" s="121" t="inlineStr">
+        <is>
+          <t>LEATHER (HS.CODE: 4107.12.00)</t>
+        </is>
+      </c>
+      <c r="C54" s="113" t="n"/>
+      <c r="D54" s="122" t="n"/>
+      <c r="E54" s="128" t="n"/>
+      <c r="F54" s="123" t="n"/>
+      <c r="G54" s="123" t="n"/>
+      <c r="H54" s="123" t="n"/>
+      <c r="I54" s="129" t="n"/>
+    </row>
+    <row r="55" ht="27" customHeight="1">
+      <c r="A55" s="112" t="n"/>
+      <c r="B55" s="112" t="inlineStr">
+        <is>
+          <t>TOTAL:</t>
+        </is>
+      </c>
+      <c r="C55" s="112" t="n"/>
+      <c r="D55" s="112" t="inlineStr">
+        <is>
+          <t>8 PALLETS</t>
+        </is>
+      </c>
+      <c r="E55" s="131">
+        <f>SUM(E41:E53)</f>
+        <v/>
+      </c>
+      <c r="F55" s="114">
+        <f>SUM(F41:F53)</f>
+        <v/>
+      </c>
+      <c r="G55" s="114">
+        <f>SUM(G41:G53)</f>
+        <v/>
+      </c>
+      <c r="H55" s="114">
+        <f>SUM(H41:H53)</f>
+        <v/>
+      </c>
+      <c r="I55" s="132">
+        <f>SUM(I41:I53)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" ht="24" customHeight="1">
+      <c r="B56" s="133" t="inlineStr">
+        <is>
+          <t>TOTAL OF:</t>
+        </is>
+      </c>
+      <c r="D56" s="133" t="inlineStr">
+        <is>
+          <t>16 PALLETS</t>
+        </is>
+      </c>
+      <c r="E56" s="134">
+        <f>SUM(E23:E34,E41:E53)</f>
+        <v/>
+      </c>
+      <c r="F56" s="135">
+        <f>SUM(F23:F34,F41:F53)</f>
+        <v/>
+      </c>
+      <c r="G56" s="135">
+        <f>SUM(G23:G34,G41:G53)</f>
+        <v/>
+      </c>
+      <c r="H56" s="135">
+        <f>SUM(H23:H34,H41:H53)</f>
+        <v/>
+      </c>
+      <c r="I56" s="136">
+        <f>SUM(I23:I34,I41:I53)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="57" ht="27" customHeight="1">
+      <c r="A57" s="137" t="n"/>
+      <c r="B57" s="138" t="inlineStr">
+        <is>
+          <t>TOTAL OF:</t>
+        </is>
+      </c>
+      <c r="C57" s="138" t="inlineStr">
+        <is>
+          <t>BUFFALO</t>
+        </is>
+      </c>
+      <c r="D57" s="138" t="inlineStr">
+        <is>
+          <t>9 PALLETS</t>
+        </is>
+      </c>
+      <c r="E57" s="139" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F57" s="140" t="n">
+        <v>72108.09999999999</v>
+      </c>
+      <c r="G57" s="140" t="n">
+        <v>5995.5</v>
+      </c>
+      <c r="H57" s="140" t="n">
+        <v>5590.5</v>
+      </c>
+      <c r="I57" s="141" t="n">
+        <v>22.8096</v>
+      </c>
+    </row>
+    <row r="58" ht="27" customHeight="1">
+      <c r="A58" s="137" t="n"/>
+      <c r="B58" s="138" t="inlineStr">
+        <is>
+          <t>TOTAL OF:</t>
+        </is>
+      </c>
+      <c r="C58" s="138" t="inlineStr">
         <is>
           <t>LEATHER</t>
         </is>
       </c>
-      <c r="E23" s="139" t="n">
-        <v>220</v>
-      </c>
-      <c r="F23" s="140" t="n">
-        <v>11723.6</v>
-      </c>
-      <c r="G23" s="140" t="n">
-        <v>985.5</v>
-      </c>
-      <c r="H23" s="140" t="n">
-        <v>940.5</v>
-      </c>
-      <c r="I23" s="141" t="n">
-        <v>2.574</v>
-      </c>
-    </row>
-    <row r="24" ht="27" customHeight="1">
-      <c r="A24" s="142" t="inlineStr">
-        <is>
-          <t>Des: LEATHER</t>
-        </is>
-      </c>
-      <c r="B24" s="127" t="inlineStr">
-        <is>
-          <t>RB0604</t>
-        </is>
-      </c>
-      <c r="C24" s="127" t="inlineStr">
-        <is>
-          <t>1.23.07.0154J</t>
-        </is>
-      </c>
-      <c r="D24" s="117" t="n"/>
-      <c r="E24" s="139" t="n">
-        <v>185</v>
-      </c>
-      <c r="F24" s="140" t="n">
-        <v>10157.8</v>
-      </c>
-      <c r="G24" s="140" t="n">
-        <v>848.5</v>
-      </c>
-      <c r="H24" s="140" t="n">
-        <v>803.5</v>
-      </c>
-      <c r="I24" s="141" t="n">
-        <v>2.4948</v>
-      </c>
-    </row>
-    <row r="25" ht="27" customHeight="1">
-      <c r="A25" s="142" t="inlineStr">
-        <is>
-          <t>Case Qty:</t>
-        </is>
-      </c>
-      <c r="B25" s="127" t="inlineStr">
-        <is>
-          <t>RB0604</t>
-        </is>
-      </c>
-      <c r="C25" s="127" t="inlineStr">
-        <is>
-          <t>1.23.07.0154J</t>
-        </is>
-      </c>
-      <c r="D25" s="117" t="n"/>
-      <c r="E25" s="139" t="n">
-        <v>185</v>
-      </c>
-      <c r="F25" s="140" t="n">
-        <v>10043.7</v>
-      </c>
-      <c r="G25" s="140" t="n">
-        <v>844.5</v>
-      </c>
-      <c r="H25" s="140" t="n">
-        <v>799.5</v>
-      </c>
-      <c r="I25" s="141" t="n">
-        <v>2.376</v>
-      </c>
-    </row>
-    <row r="26" ht="27" customHeight="1">
-      <c r="A26" s="142" t="inlineStr">
-        <is>
-          <t>MADE IN CAMBODIA</t>
-        </is>
-      </c>
-      <c r="B26" s="127" t="inlineStr">
-        <is>
-          <t>RB3358</t>
-        </is>
-      </c>
-      <c r="C26" s="127" t="inlineStr">
-        <is>
-          <t>1.23.07.0157J</t>
-        </is>
-      </c>
-      <c r="D26" s="117" t="n"/>
-      <c r="E26" s="139" t="n">
-        <v>190</v>
-      </c>
-      <c r="F26" s="140" t="n">
-        <v>11067.7</v>
-      </c>
-      <c r="G26" s="140" t="n">
-        <v>888.5</v>
-      </c>
-      <c r="H26" s="140" t="n">
-        <v>843.5</v>
-      </c>
-      <c r="I26" s="141" t="n">
-        <v>2.97</v>
-      </c>
-    </row>
-    <row r="27" ht="27" customHeight="1">
-      <c r="A27" s="142" t="n"/>
-      <c r="B27" s="127" t="inlineStr">
-        <is>
-          <t>SJ0B-317</t>
-        </is>
-      </c>
-      <c r="C27" s="127" t="inlineStr">
-        <is>
-          <t>1.23.07.0220D</t>
-        </is>
-      </c>
-      <c r="D27" s="117" t="n"/>
-      <c r="E27" s="139" t="n">
-        <v>185</v>
-      </c>
-      <c r="F27" s="140" t="n">
-        <v>10308</v>
-      </c>
-      <c r="G27" s="140" t="n">
-        <v>787</v>
-      </c>
-      <c r="H27" s="140" t="n">
-        <v>742</v>
-      </c>
-      <c r="I27" s="141" t="n">
-        <v>2.6532</v>
-      </c>
-    </row>
-    <row r="28" ht="27" customHeight="1">
-      <c r="A28" s="142" t="n"/>
-      <c r="B28" s="127" t="inlineStr">
-        <is>
-          <t>SJ0B-317</t>
-        </is>
-      </c>
-      <c r="C28" s="127" t="inlineStr">
-        <is>
-          <t>1.23.07.0220D</t>
-        </is>
-      </c>
-      <c r="D28" s="117" t="n"/>
-      <c r="E28" s="139" t="n">
-        <v>183</v>
-      </c>
-      <c r="F28" s="140" t="n">
-        <v>10162.2</v>
-      </c>
-      <c r="G28" s="140" t="n">
-        <v>778.5</v>
-      </c>
-      <c r="H28" s="140" t="n">
-        <v>733.5</v>
-      </c>
-      <c r="I28" s="141" t="n">
-        <v>2.5344</v>
-      </c>
-    </row>
-    <row r="29" ht="27" customHeight="1">
-      <c r="A29" s="142" t="n"/>
-      <c r="B29" s="127" t="inlineStr">
-        <is>
-          <t>SJ0B-317</t>
-        </is>
-      </c>
-      <c r="C29" s="127" t="inlineStr">
-        <is>
-          <t>1.23.07.0220D</t>
-        </is>
-      </c>
-      <c r="D29" s="117" t="n"/>
-      <c r="E29" s="139" t="n">
-        <v>190</v>
-      </c>
-      <c r="F29" s="140" t="n">
-        <v>10120.6</v>
-      </c>
-      <c r="G29" s="140" t="n">
-        <v>776.5</v>
-      </c>
-      <c r="H29" s="140" t="n">
-        <v>731.5</v>
-      </c>
-      <c r="I29" s="141" t="n">
-        <v>3.0492</v>
-      </c>
-    </row>
-    <row r="30" ht="27" customHeight="1">
-      <c r="A30" s="142" t="n"/>
-      <c r="B30" s="127" t="inlineStr">
-        <is>
-          <t>SJ0B-317</t>
-        </is>
-      </c>
-      <c r="C30" s="127" t="inlineStr">
-        <is>
-          <t>1.23.07.0220D</t>
-        </is>
-      </c>
-      <c r="D30" s="117" t="n"/>
-      <c r="E30" s="139" t="n">
-        <v>190</v>
-      </c>
-      <c r="F30" s="140" t="n">
-        <v>10093.7</v>
-      </c>
-      <c r="G30" s="140" t="n">
-        <v>774.5</v>
-      </c>
-      <c r="H30" s="140" t="n">
-        <v>729.5</v>
-      </c>
-      <c r="I30" s="141" t="n">
-        <v>3.0492</v>
-      </c>
-    </row>
-    <row r="31" ht="27" customHeight="1">
-      <c r="A31" s="142" t="n"/>
-      <c r="B31" s="127" t="inlineStr">
-        <is>
-          <t>SJ0B-317</t>
-        </is>
-      </c>
-      <c r="C31" s="127" t="inlineStr">
-        <is>
-          <t>1.23.07.0220D</t>
-        </is>
-      </c>
-      <c r="D31" s="117" t="n"/>
-      <c r="E31" s="139" t="n">
-        <v>190</v>
-      </c>
-      <c r="F31" s="140" t="n">
-        <v>10178.8</v>
-      </c>
-      <c r="G31" s="140" t="n">
-        <v>780</v>
-      </c>
-      <c r="H31" s="140" t="n">
-        <v>735</v>
-      </c>
-      <c r="I31" s="141" t="n">
-        <v>3.0492</v>
-      </c>
-    </row>
-    <row r="32" ht="27" customHeight="1">
-      <c r="A32" s="142" t="n"/>
-      <c r="B32" s="127" t="inlineStr">
-        <is>
-          <t>SJ0B-317</t>
-        </is>
-      </c>
-      <c r="C32" s="127" t="inlineStr">
-        <is>
-          <t>1.23.07.0220D</t>
-        </is>
-      </c>
-      <c r="D32" s="117" t="n"/>
-      <c r="E32" s="139" t="n">
-        <v>190</v>
-      </c>
-      <c r="F32" s="140" t="n">
-        <v>10150.7</v>
-      </c>
-      <c r="G32" s="140" t="n">
-        <v>778</v>
-      </c>
-      <c r="H32" s="140" t="n">
-        <v>733</v>
-      </c>
-      <c r="I32" s="141" t="n">
-        <v>3.0492</v>
-      </c>
-    </row>
-    <row r="33" ht="27" customHeight="1">
-      <c r="A33" s="142" t="n"/>
-      <c r="B33" s="127" t="inlineStr">
-        <is>
-          <t>SJ0B-317</t>
-        </is>
-      </c>
-      <c r="C33" s="127" t="inlineStr">
-        <is>
-          <t>1.23.07.0220D</t>
-        </is>
-      </c>
-      <c r="D33" s="117" t="n"/>
-      <c r="E33" s="139" t="n">
-        <v>190</v>
-      </c>
-      <c r="F33" s="140" t="n">
-        <v>10239.9</v>
-      </c>
-      <c r="G33" s="140" t="n">
-        <v>784</v>
-      </c>
-      <c r="H33" s="140" t="n">
-        <v>739</v>
-      </c>
-      <c r="I33" s="141" t="n">
-        <v>3.0492</v>
-      </c>
-    </row>
-    <row r="34" ht="27" customHeight="1">
-      <c r="A34" s="142" t="n"/>
-      <c r="B34" s="127" t="inlineStr">
-        <is>
-          <t>SJ0B-317</t>
-        </is>
-      </c>
-      <c r="C34" s="127" t="inlineStr">
-        <is>
-          <t>1.23.07.0220D</t>
-        </is>
-      </c>
-      <c r="D34" s="117" t="n"/>
-      <c r="E34" s="139" t="n">
-        <v>142</v>
-      </c>
-      <c r="F34" s="140" t="n">
-        <v>7362.9</v>
-      </c>
-      <c r="G34" s="140" t="n">
-        <v>566.7759</v>
-      </c>
-      <c r="H34" s="140" t="n">
-        <v>530.0517</v>
-      </c>
-      <c r="I34" s="141" t="n">
-        <v>2.4884</v>
-      </c>
-    </row>
-    <row r="35" ht="27" customHeight="1">
-      <c r="A35" s="142" t="n"/>
-      <c r="B35" s="127" t="inlineStr">
-        <is>
-          <t>SJ0B-317</t>
-        </is>
-      </c>
-      <c r="C35" s="127" t="inlineStr">
-        <is>
-          <t>1.23.07.0220D</t>
-        </is>
-      </c>
-      <c r="D35" s="111" t="n"/>
-      <c r="E35" s="139" t="n">
-        <v>32</v>
-      </c>
-      <c r="F35" s="140" t="n">
-        <v>1588.2</v>
-      </c>
-      <c r="G35" s="140" t="n">
-        <v>127.7241</v>
-      </c>
-      <c r="H35" s="140" t="n">
-        <v>119.4483</v>
-      </c>
-      <c r="I35" s="141" t="n">
-        <v>0.5608</v>
-      </c>
-    </row>
-    <row r="36" ht="27" customHeight="1">
-      <c r="A36" s="142" t="n"/>
-      <c r="B36" s="127" t="inlineStr">
-        <is>
-          <t>LEATHER (HS.CODE: 4107.12.00)</t>
-        </is>
-      </c>
-      <c r="C36" s="110" t="n"/>
-      <c r="D36" s="138" t="n"/>
-      <c r="E36" s="139" t="n"/>
-      <c r="F36" s="140" t="n"/>
-      <c r="G36" s="140" t="n"/>
-      <c r="H36" s="140" t="n"/>
-      <c r="I36" s="141" t="n"/>
-    </row>
-    <row r="37" ht="27" customHeight="1">
-      <c r="A37" s="143" t="n"/>
-      <c r="B37" s="125" t="inlineStr">
-        <is>
-          <t xml:space="preserve">TOTAL OF: </t>
-        </is>
-      </c>
-      <c r="C37" s="121" t="n"/>
-      <c r="D37" s="125" t="inlineStr">
-        <is>
-          <t>0 PALLETS</t>
-        </is>
-      </c>
-      <c r="E37" s="125">
-        <f>SUM(E23:E35)</f>
-        <v/>
-      </c>
-      <c r="F37" s="125">
-        <f>SUM(F23:F35)</f>
-        <v/>
-      </c>
-      <c r="G37" s="125">
-        <f>SUM(G23:G35)</f>
-        <v/>
-      </c>
-      <c r="H37" s="125">
-        <f>SUM(H23:H35)</f>
-        <v/>
-      </c>
-      <c r="I37" s="125">
-        <f>SUM(I23:I35)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="38" ht="27.75" customHeight="1">
-      <c r="A38" s="20" t="n"/>
-      <c r="B38" s="65" t="n"/>
-    </row>
-    <row r="39" ht="27.75" customHeight="1">
-      <c r="A39" s="13" t="inlineStr">
+      <c r="D58" s="138" t="inlineStr">
+        <is>
+          <t>7 PALLETS</t>
+        </is>
+      </c>
+      <c r="E58" s="139" t="n">
+        <v>1133</v>
+      </c>
+      <c r="F58" s="140" t="n">
+        <v>58119</v>
+      </c>
+      <c r="G58" s="140" t="n">
+        <v>4895.5</v>
+      </c>
+      <c r="H58" s="140" t="n">
+        <v>4580.5</v>
+      </c>
+      <c r="I58" s="141" t="n">
+        <v>16.038</v>
+      </c>
+    </row>
+    <row r="59" ht="53.1" customHeight="1">
+      <c r="A59" s="13" t="inlineStr">
         <is>
           <t>Country of Original Cambodia</t>
         </is>
       </c>
-      <c r="B39" s="13" t="n"/>
-      <c r="C39" s="13" t="n"/>
-      <c r="D39" s="101" t="n"/>
-      <c r="E39" s="27" t="n"/>
-      <c r="F39" s="96" t="n"/>
-      <c r="G39" s="96" t="n"/>
-      <c r="H39" s="96" t="n"/>
-    </row>
-    <row r="40" ht="65.25" customHeight="1">
-      <c r="A40" s="28" t="inlineStr">
+      <c r="B59" s="13" t="n"/>
+      <c r="C59" s="13" t="n"/>
+      <c r="D59" s="101" t="n"/>
+      <c r="E59" s="27" t="n"/>
+      <c r="F59" s="96" t="n"/>
+      <c r="G59" s="96" t="n"/>
+      <c r="H59" s="96" t="n"/>
+    </row>
+    <row r="60" ht="65.25" customHeight="1">
+      <c r="A60" s="28" t="inlineStr">
         <is>
           <t>Manufacture:</t>
         </is>
       </c>
-      <c r="B40" s="104" t="inlineStr">
+      <c r="B60" s="104" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
 XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="E40" s="31" t="n"/>
-      <c r="F40" s="31" t="n"/>
-      <c r="G40" s="31" t="n"/>
-      <c r="H40" s="96" t="n"/>
-    </row>
-    <row r="41" ht="51.75" customHeight="1">
-      <c r="A41" s="104" t="inlineStr">
+      <c r="E60" s="31" t="n"/>
+      <c r="F60" s="31" t="n"/>
+      <c r="G60" s="31" t="n"/>
+      <c r="H60" s="96" t="n"/>
+    </row>
+    <row r="61" ht="51.75" customHeight="1">
+      <c r="A61" s="104" t="inlineStr">
         <is>
           <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED  PHNOM PENH BRANCH
                                           /BANK OF CHINA PHNOM PENH BRANCH</t>
         </is>
       </c>
-      <c r="E41" s="31" t="n"/>
-      <c r="F41" s="31" t="n"/>
-      <c r="G41" s="31" t="n"/>
-      <c r="H41" s="31" t="n"/>
-    </row>
-    <row r="42" ht="27.75" customHeight="1">
-      <c r="A42" s="99" t="inlineStr">
+      <c r="E61" s="31" t="n"/>
+      <c r="F61" s="31" t="n"/>
+      <c r="G61" s="31" t="n"/>
+      <c r="H61" s="31" t="n"/>
+    </row>
+    <row r="62" ht="27.75" customHeight="1">
+      <c r="A62" s="99" t="inlineStr">
         <is>
           <t>A/C NO:100001100764430</t>
         </is>
       </c>
-      <c r="B42" s="99" t="n"/>
-      <c r="C42" s="99" t="n"/>
-      <c r="D42" s="99" t="n"/>
-      <c r="E42" s="16" t="n"/>
-      <c r="F42" s="16" t="n"/>
-      <c r="G42" s="16" t="n"/>
-      <c r="H42" s="16" t="n"/>
-    </row>
-    <row r="43" ht="27.75" customHeight="1">
-      <c r="A43" s="99" t="inlineStr">
+      <c r="B62" s="99" t="n"/>
+      <c r="C62" s="99" t="n"/>
+      <c r="D62" s="99" t="n"/>
+      <c r="E62" s="16" t="n"/>
+      <c r="F62" s="16" t="n"/>
+      <c r="G62" s="16" t="n"/>
+      <c r="H62" s="16" t="n"/>
+    </row>
+    <row r="63" ht="24.75" customHeight="1">
+      <c r="A63" s="99" t="inlineStr">
         <is>
           <t>SWIFT CODE  ：BKCHKHPPXXX</t>
         </is>
       </c>
-      <c r="B43" s="99" t="n"/>
-      <c r="C43" s="99" t="n"/>
-      <c r="D43" s="99" t="n"/>
-      <c r="E43" s="16" t="n"/>
-      <c r="F43" s="16" t="n"/>
-      <c r="G43" s="16" t="n"/>
-      <c r="H43" s="16" t="n"/>
-    </row>
-    <row r="44" ht="27.75" customHeight="1">
-      <c r="A44" s="82" t="n"/>
-      <c r="B44" s="83" t="n"/>
-      <c r="C44" s="82" t="n"/>
-      <c r="D44" s="82" t="n"/>
-      <c r="E44" s="84" t="n"/>
-      <c r="F44" s="96" t="inlineStr">
+      <c r="B63" s="99" t="n"/>
+      <c r="C63" s="99" t="n"/>
+      <c r="D63" s="99" t="n"/>
+      <c r="E63" s="16" t="n"/>
+      <c r="F63" s="16" t="n"/>
+      <c r="G63" s="16" t="n"/>
+      <c r="H63" s="16" t="n"/>
+    </row>
+    <row r="64" ht="21" customHeight="1">
+      <c r="A64" s="82" t="n"/>
+      <c r="B64" s="83" t="n"/>
+      <c r="C64" s="82" t="n"/>
+      <c r="D64" s="82" t="n"/>
+      <c r="E64" s="84" t="n"/>
+      <c r="F64" s="96" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
       </c>
-      <c r="G44" s="96" t="n"/>
-      <c r="H44" s="84" t="n"/>
-    </row>
-    <row r="45" ht="27.75" customHeight="1"/>
-    <row r="46" ht="27.75" customHeight="1"/>
-    <row r="47" ht="27.75" customHeight="1"/>
-    <row r="48" ht="27.75" customHeight="1"/>
-    <row r="49" ht="42" customHeight="1"/>
-    <row r="50" ht="42" customHeight="1"/>
-    <row r="51" ht="74.09999999999999" customHeight="1"/>
-    <row r="52" ht="44.1" customHeight="1"/>
-    <row r="53" ht="24.75" customHeight="1"/>
-    <row r="54" ht="27" customFormat="1" customHeight="1" s="1"/>
-    <row r="55" ht="42" customHeight="1"/>
-    <row r="56" ht="24" customHeight="1"/>
-    <row r="57" ht="69.75" customHeight="1">
-      <c r="A57" s="71" t="n"/>
-      <c r="B57" s="67" t="n"/>
-      <c r="C57" s="52" t="n"/>
-      <c r="D57" s="53" t="n"/>
-      <c r="E57" s="54" t="n"/>
-      <c r="F57" s="55" t="n"/>
-      <c r="G57" s="55" t="n"/>
-      <c r="H57" s="55" t="n"/>
-      <c r="I57" s="55" t="n"/>
-    </row>
-    <row r="58" ht="42" customHeight="1">
-      <c r="A58" s="21" t="n"/>
-      <c r="B58" s="67" t="n"/>
-      <c r="C58" s="52" t="n"/>
-      <c r="D58" s="53" t="n"/>
-      <c r="E58" s="54" t="n"/>
-      <c r="F58" s="55" t="n"/>
-      <c r="G58" s="55" t="n"/>
-      <c r="H58" s="55" t="n"/>
-      <c r="I58" s="55" t="n"/>
-    </row>
-    <row r="59" ht="53.1" customHeight="1">
-      <c r="A59" s="21" t="n"/>
-      <c r="B59" s="67" t="n"/>
-      <c r="C59" s="52" t="n"/>
-      <c r="D59" s="53" t="n"/>
-      <c r="E59" s="54" t="n"/>
-      <c r="F59" s="55" t="n"/>
-      <c r="G59" s="55" t="n"/>
-      <c r="H59" s="55" t="n"/>
-      <c r="I59" s="55" t="n"/>
-    </row>
-    <row r="60" ht="27.75" customHeight="1">
-      <c r="A60" s="21" t="n"/>
-      <c r="B60" s="67" t="n"/>
-      <c r="C60" s="52" t="n"/>
-      <c r="D60" s="53" t="n"/>
-      <c r="E60" s="54" t="n"/>
-      <c r="F60" s="55" t="n"/>
-      <c r="G60" s="55" t="n"/>
-      <c r="H60" s="55" t="n"/>
-      <c r="I60" s="55" t="n"/>
-    </row>
-    <row r="61" ht="27.75" customHeight="1">
-      <c r="A61" s="21" t="n"/>
-      <c r="B61" s="67" t="n"/>
-      <c r="C61" s="52" t="n"/>
-      <c r="D61" s="53" t="n"/>
-      <c r="E61" s="54" t="n"/>
-      <c r="F61" s="55" t="n"/>
-      <c r="G61" s="55" t="n"/>
-      <c r="H61" s="55" t="n"/>
-      <c r="I61" s="55" t="n"/>
-    </row>
-    <row r="62" ht="27.75" customHeight="1">
-      <c r="A62" s="21" t="n"/>
-      <c r="B62" s="67" t="n"/>
-      <c r="C62" s="52" t="n"/>
-      <c r="D62" s="53" t="n"/>
-      <c r="E62" s="54" t="n"/>
-      <c r="F62" s="55" t="n"/>
-      <c r="G62" s="55" t="n"/>
-      <c r="H62" s="55" t="n"/>
-      <c r="I62" s="55" t="n"/>
-    </row>
-    <row r="63" ht="24.75" customHeight="1">
-      <c r="A63" s="21" t="n"/>
-      <c r="B63" s="67" t="n"/>
-      <c r="C63" s="52" t="n"/>
-      <c r="D63" s="53" t="n"/>
-      <c r="E63" s="54" t="n"/>
-      <c r="F63" s="55" t="n"/>
-      <c r="G63" s="55" t="n"/>
-      <c r="H63" s="55" t="n"/>
-      <c r="I63" s="55" t="n"/>
-    </row>
-    <row r="64" ht="21" customHeight="1">
-      <c r="A64" s="21" t="n"/>
-      <c r="B64" s="67" t="n"/>
-      <c r="C64" s="52" t="n"/>
-      <c r="D64" s="53" t="n"/>
-      <c r="E64" s="54" t="n"/>
-      <c r="F64" s="55" t="n"/>
-      <c r="G64" s="55" t="n"/>
-      <c r="H64" s="55" t="n"/>
-      <c r="I64" s="55" t="n"/>
-    </row>
-    <row r="65" ht="21" customHeight="1">
-      <c r="A65" s="21" t="n"/>
-      <c r="B65" s="67" t="n"/>
-      <c r="C65" s="52" t="n"/>
-      <c r="D65" s="53" t="n"/>
-      <c r="E65" s="54" t="n"/>
-      <c r="F65" s="55" t="n"/>
-      <c r="G65" s="55" t="n"/>
-      <c r="H65" s="55" t="n"/>
-      <c r="I65" s="55" t="n"/>
-    </row>
-    <row r="66" ht="21" customHeight="1">
-      <c r="A66" s="101" t="n"/>
-      <c r="B66" s="68" t="n"/>
-      <c r="C66" s="24" t="n"/>
-      <c r="D66" s="101" t="n"/>
-      <c r="E66" s="25" t="n"/>
-      <c r="F66" s="26" t="n"/>
-      <c r="G66" s="26" t="n"/>
-      <c r="H66" s="26" t="n"/>
-      <c r="I66" s="26" t="n"/>
-    </row>
+      <c r="G64" s="96" t="n"/>
+      <c r="H64" s="84" t="n"/>
+    </row>
+    <row r="65" ht="21" customHeight="1"/>
+    <row r="66" ht="21" customHeight="1"/>
     <row r="67" ht="21" customHeight="1"/>
     <row r="68" ht="21" customHeight="1"/>
     <row r="69" ht="21" customHeight="1"/>
     <row r="70" ht="21" customHeight="1"/>
-    <row r="71" ht="21" customHeight="1">
-      <c r="B71" s="69" t="n"/>
-    </row>
+    <row r="71" ht="21" customHeight="1"/>
     <row r="72" ht="25.5" customHeight="1"/>
     <row r="73" ht="21" customHeight="1"/>
-    <row r="74" ht="21" customHeight="1">
-      <c r="F74" s="96" t="n"/>
-      <c r="G74" s="96" t="n"/>
-      <c r="H74" s="96" t="n"/>
-    </row>
-    <row r="75" ht="21" customHeight="1">
-      <c r="F75" s="96" t="n"/>
-      <c r="G75" s="96" t="n"/>
-      <c r="H75" s="96" t="n"/>
-    </row>
-    <row r="76" ht="21" customHeight="1">
-      <c r="F76" s="96" t="n"/>
-      <c r="G76" s="96" t="n"/>
-      <c r="H76" s="96" t="n"/>
-      <c r="I76" s="96" t="n"/>
-    </row>
-    <row r="77" ht="21" customHeight="1"/>
-    <row r="78" ht="17.25" customHeight="1"/>
-    <row r="79"/>
-    <row r="80"/>
-    <row r="81"/>
-    <row r="82"/>
-    <row r="83"/>
-    <row r="84"/>
-    <row r="85"/>
-    <row r="86"/>
+    <row r="74" ht="21" customHeight="1"/>
+    <row r="75" ht="21" customHeight="1"/>
+    <row r="76" ht="21" customHeight="1"/>
+    <row r="77" ht="21" customHeight="1">
+      <c r="A77" s="71" t="n"/>
+      <c r="B77" s="67" t="n"/>
+      <c r="C77" s="52" t="n"/>
+      <c r="D77" s="53" t="n"/>
+      <c r="E77" s="54" t="n"/>
+      <c r="F77" s="55" t="n"/>
+      <c r="G77" s="55" t="n"/>
+      <c r="H77" s="55" t="n"/>
+      <c r="I77" s="55" t="n"/>
+    </row>
+    <row r="78" ht="17.25" customHeight="1">
+      <c r="A78" s="21" t="n"/>
+      <c r="B78" s="67" t="n"/>
+      <c r="C78" s="52" t="n"/>
+      <c r="D78" s="53" t="n"/>
+      <c r="E78" s="54" t="n"/>
+      <c r="F78" s="55" t="n"/>
+      <c r="G78" s="55" t="n"/>
+      <c r="H78" s="55" t="n"/>
+      <c r="I78" s="55" t="n"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="21" t="n"/>
+      <c r="B79" s="67" t="n"/>
+      <c r="C79" s="52" t="n"/>
+      <c r="D79" s="53" t="n"/>
+      <c r="E79" s="54" t="n"/>
+      <c r="F79" s="55" t="n"/>
+      <c r="G79" s="55" t="n"/>
+      <c r="H79" s="55" t="n"/>
+      <c r="I79" s="55" t="n"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="21" t="n"/>
+      <c r="B80" s="67" t="n"/>
+      <c r="C80" s="52" t="n"/>
+      <c r="D80" s="53" t="n"/>
+      <c r="E80" s="54" t="n"/>
+      <c r="F80" s="55" t="n"/>
+      <c r="G80" s="55" t="n"/>
+      <c r="H80" s="55" t="n"/>
+      <c r="I80" s="55" t="n"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="21" t="n"/>
+      <c r="B81" s="67" t="n"/>
+      <c r="C81" s="52" t="n"/>
+      <c r="D81" s="53" t="n"/>
+      <c r="E81" s="54" t="n"/>
+      <c r="F81" s="55" t="n"/>
+      <c r="G81" s="55" t="n"/>
+      <c r="H81" s="55" t="n"/>
+      <c r="I81" s="55" t="n"/>
+    </row>
+    <row r="82">
+      <c r="A82" s="21" t="n"/>
+      <c r="B82" s="67" t="n"/>
+      <c r="C82" s="52" t="n"/>
+      <c r="D82" s="53" t="n"/>
+      <c r="E82" s="54" t="n"/>
+      <c r="F82" s="55" t="n"/>
+      <c r="G82" s="55" t="n"/>
+      <c r="H82" s="55" t="n"/>
+      <c r="I82" s="55" t="n"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="21" t="n"/>
+      <c r="B83" s="67" t="n"/>
+      <c r="C83" s="52" t="n"/>
+      <c r="D83" s="53" t="n"/>
+      <c r="E83" s="54" t="n"/>
+      <c r="F83" s="55" t="n"/>
+      <c r="G83" s="55" t="n"/>
+      <c r="H83" s="55" t="n"/>
+      <c r="I83" s="55" t="n"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="21" t="n"/>
+      <c r="B84" s="67" t="n"/>
+      <c r="C84" s="52" t="n"/>
+      <c r="D84" s="53" t="n"/>
+      <c r="E84" s="54" t="n"/>
+      <c r="F84" s="55" t="n"/>
+      <c r="G84" s="55" t="n"/>
+      <c r="H84" s="55" t="n"/>
+      <c r="I84" s="55" t="n"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="21" t="n"/>
+      <c r="B85" s="67" t="n"/>
+      <c r="C85" s="52" t="n"/>
+      <c r="D85" s="53" t="n"/>
+      <c r="E85" s="54" t="n"/>
+      <c r="F85" s="55" t="n"/>
+      <c r="G85" s="55" t="n"/>
+      <c r="H85" s="55" t="n"/>
+      <c r="I85" s="55" t="n"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="101" t="n"/>
+      <c r="B86" s="68" t="n"/>
+      <c r="C86" s="24" t="n"/>
+      <c r="D86" s="101" t="n"/>
+      <c r="E86" s="25" t="n"/>
+      <c r="F86" s="26" t="n"/>
+      <c r="G86" s="26" t="n"/>
+      <c r="H86" s="26" t="n"/>
+      <c r="I86" s="26" t="n"/>
+    </row>
     <row r="87"/>
     <row r="88"/>
     <row r="89"/>
     <row r="90" ht="15" customHeight="1"/>
-    <row r="91"/>
+    <row r="91">
+      <c r="B91" s="69" t="n"/>
+    </row>
     <row r="92"/>
     <row r="93"/>
-    <row r="94"/>
-    <row r="95"/>
-    <row r="96"/>
+    <row r="94">
+      <c r="F94" s="96" t="n"/>
+      <c r="G94" s="96" t="n"/>
+      <c r="H94" s="96" t="n"/>
+    </row>
+    <row r="95">
+      <c r="F95" s="96" t="n"/>
+      <c r="G95" s="96" t="n"/>
+      <c r="H95" s="96" t="n"/>
+    </row>
+    <row r="96">
+      <c r="F96" s="96" t="n"/>
+      <c r="G96" s="96" t="n"/>
+      <c r="H96" s="96" t="n"/>
+      <c r="I96" s="96" t="n"/>
+    </row>
     <row r="97"/>
     <row r="98" ht="115.7" customHeight="1"/>
     <row r="99" ht="113.65" customHeight="1"/>
@@ -4128,24 +5297,12 @@
     <row r="111"/>
     <row r="112"/>
     <row r="113"/>
-    <row r="114">
-      <c r="I114" s="96" t="n"/>
-    </row>
-    <row r="115">
-      <c r="I115" s="96" t="n"/>
-    </row>
-    <row r="116">
-      <c r="I116" s="96" t="n"/>
-    </row>
-    <row r="117">
-      <c r="I117" s="16" t="n"/>
-    </row>
-    <row r="118">
-      <c r="I118" s="16" t="n"/>
-    </row>
-    <row r="119">
-      <c r="I119" s="96" t="n"/>
-    </row>
+    <row r="114"/>
+    <row r="115"/>
+    <row r="116"/>
+    <row r="117"/>
+    <row r="118"/>
+    <row r="119"/>
     <row r="120"/>
     <row r="121"/>
     <row r="122"/>
@@ -4160,12 +5317,24 @@
     <row r="131"/>
     <row r="132"/>
     <row r="133"/>
-    <row r="134"/>
-    <row r="135"/>
-    <row r="136"/>
-    <row r="137"/>
-    <row r="138"/>
-    <row r="139"/>
+    <row r="134">
+      <c r="I134" s="96" t="n"/>
+    </row>
+    <row r="135">
+      <c r="I135" s="96" t="n"/>
+    </row>
+    <row r="136">
+      <c r="I136" s="96" t="n"/>
+    </row>
+    <row r="137">
+      <c r="I137" s="16" t="n"/>
+    </row>
+    <row r="138">
+      <c r="I138" s="16" t="n"/>
+    </row>
+    <row r="139">
+      <c r="I139" s="96" t="n"/>
+    </row>
     <row r="140"/>
     <row r="141"/>
     <row r="142"/>
@@ -4228,24 +5397,37 @@
     <row r="199"/>
     <row r="200"/>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="31">
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="B55"/>
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="H21:H22"/>
     <mergeCell ref="A3:I3"/>
+    <mergeCell ref="B36"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="H39:H40"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A5:I5"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="I21:I22"/>
-    <mergeCell ref="B40:D40"/>
     <mergeCell ref="A4:I4"/>
     <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="D23:D35"/>
+    <mergeCell ref="I39:I40"/>
+    <mergeCell ref="B56"/>
+    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="A37"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="A39:A40"/>
     <mergeCell ref="A1:I1"/>
+    <mergeCell ref="B38"/>
     <mergeCell ref="G21:G22"/>
-    <mergeCell ref="B36:C36"/>
     <mergeCell ref="A6:I6"/>
-    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B35:C35"/>
     <mergeCell ref="E21:F21"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
fix grand footer bug where it appear every table
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -450,7 +450,7 @@
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
@@ -816,21 +816,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="38" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="38" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="38" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="38" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="38" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4388,104 +4373,107 @@
       </c>
     </row>
     <row r="37" ht="27.75" customHeight="1"/>
-    <row r="38" ht="27.75" customHeight="1">
-      <c r="B38" s="133" t="inlineStr">
-        <is>
-          <t>TOTAL OF:</t>
-        </is>
-      </c>
-      <c r="D38" s="133" t="inlineStr">
-        <is>
-          <t>8 PALLETS</t>
-        </is>
-      </c>
-      <c r="E38" s="134">
-        <f>SUM(E23:E34)</f>
-        <v/>
-      </c>
-      <c r="F38" s="135">
-        <f>SUM(F23:F34)</f>
-        <v/>
-      </c>
-      <c r="G38" s="135">
-        <f>SUM(G23:G34)</f>
-        <v/>
-      </c>
-      <c r="H38" s="135">
-        <f>SUM(H23:H34)</f>
-        <v/>
-      </c>
-      <c r="I38" s="136">
-        <f>SUM(I23:I34)</f>
-        <v/>
+    <row r="38" ht="27" customHeight="1">
+      <c r="A38" s="125" t="inlineStr">
+        <is>
+          <t>Mark &amp; Nº</t>
+        </is>
+      </c>
+      <c r="B38" s="125" t="inlineStr">
+        <is>
+          <t>P.O Nº</t>
+        </is>
+      </c>
+      <c r="C38" s="125" t="inlineStr">
+        <is>
+          <t>ITEM Nº</t>
+        </is>
+      </c>
+      <c r="D38" s="125" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="E38" s="125" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="F38" s="113" t="n"/>
+      <c r="G38" s="125" t="inlineStr">
+        <is>
+          <t>G.W (kgs)</t>
+        </is>
+      </c>
+      <c r="H38" s="125" t="inlineStr">
+        <is>
+          <t>N.W (kgs)</t>
+        </is>
+      </c>
+      <c r="I38" s="125" t="inlineStr">
+        <is>
+          <t>CBM</t>
+        </is>
       </c>
     </row>
     <row r="39" ht="27" customHeight="1">
-      <c r="A39" s="125" t="inlineStr">
-        <is>
-          <t>Mark &amp; Nº</t>
-        </is>
-      </c>
-      <c r="B39" s="125" t="inlineStr">
-        <is>
-          <t>P.O Nº</t>
-        </is>
-      </c>
-      <c r="C39" s="125" t="inlineStr">
-        <is>
-          <t>ITEM Nº</t>
-        </is>
-      </c>
-      <c r="D39" s="125" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
+      <c r="A39" s="126" t="n"/>
+      <c r="B39" s="126" t="n"/>
+      <c r="C39" s="126" t="n"/>
+      <c r="D39" s="126" t="n"/>
       <c r="E39" s="125" t="inlineStr">
         <is>
-          <t>Quantity</t>
-        </is>
-      </c>
-      <c r="F39" s="113" t="n"/>
-      <c r="G39" s="125" t="inlineStr">
-        <is>
-          <t>G.W (kgs)</t>
-        </is>
-      </c>
-      <c r="H39" s="125" t="inlineStr">
-        <is>
-          <t>N.W (kgs)</t>
-        </is>
-      </c>
-      <c r="I39" s="125" t="inlineStr">
-        <is>
-          <t>CBM</t>
-        </is>
-      </c>
+          <t>PCS</t>
+        </is>
+      </c>
+      <c r="F39" s="125" t="inlineStr">
+        <is>
+          <t>SF</t>
+        </is>
+      </c>
+      <c r="G39" s="126" t="n"/>
+      <c r="H39" s="126" t="n"/>
+      <c r="I39" s="126" t="n"/>
     </row>
     <row r="40" ht="27" customHeight="1">
-      <c r="A40" s="126" t="n"/>
-      <c r="B40" s="126" t="n"/>
-      <c r="C40" s="126" t="n"/>
-      <c r="D40" s="126" t="n"/>
-      <c r="E40" s="125" t="inlineStr">
-        <is>
-          <t>PCS</t>
-        </is>
-      </c>
-      <c r="F40" s="125" t="inlineStr">
-        <is>
-          <t>SF</t>
-        </is>
-      </c>
-      <c r="G40" s="126" t="n"/>
-      <c r="H40" s="126" t="n"/>
-      <c r="I40" s="126" t="n"/>
+      <c r="A40" s="127" t="inlineStr">
+        <is>
+          <t>VENDOR#:</t>
+        </is>
+      </c>
+      <c r="B40" s="121" t="n">
+        <v>9000719487</v>
+      </c>
+      <c r="C40" s="121" t="inlineStr">
+        <is>
+          <t>01.10.U741023</t>
+        </is>
+      </c>
+      <c r="D40" s="121" t="inlineStr">
+        <is>
+          <t>BUFFALO HIDE</t>
+        </is>
+      </c>
+      <c r="E40" s="128" t="n">
+        <v>171</v>
+      </c>
+      <c r="F40" s="123" t="n">
+        <v>9892.700000000001</v>
+      </c>
+      <c r="G40" s="123" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" s="123" t="n">
+        <v>0</v>
+      </c>
+      <c r="I40" s="129" t="n">
+        <v>2.6928</v>
+      </c>
     </row>
     <row r="41" ht="27" customHeight="1">
-      <c r="A41" s="127" t="inlineStr">
-        <is>
-          <t>VENDOR#:</t>
+      <c r="A41" s="130" t="inlineStr">
+        <is>
+          <t>Des: LEATHER</t>
         </is>
       </c>
       <c r="B41" s="121" t="n">
@@ -4493,7 +4481,7 @@
       </c>
       <c r="C41" s="121" t="inlineStr">
         <is>
-          <t>01.10.U741023</t>
+          <t>01.10.U722233</t>
         </is>
       </c>
       <c r="D41" s="121" t="inlineStr">
@@ -4502,25 +4490,25 @@
         </is>
       </c>
       <c r="E41" s="128" t="n">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F41" s="123" t="n">
-        <v>9892.700000000001</v>
+        <v>9198.4</v>
       </c>
       <c r="G41" s="123" t="n">
-        <v>0</v>
+        <v>610.234</v>
       </c>
       <c r="H41" s="123" t="n">
-        <v>0</v>
+        <v>569.0638</v>
       </c>
       <c r="I41" s="129" t="n">
-        <v>2.6928</v>
+        <v>2.2462</v>
       </c>
     </row>
     <row r="42" ht="27" customHeight="1">
       <c r="A42" s="130" t="inlineStr">
         <is>
-          <t>Des: LEATHER</t>
+          <t>Case Qty:</t>
         </is>
       </c>
       <c r="B42" s="121" t="n">
@@ -4537,25 +4525,25 @@
         </is>
       </c>
       <c r="E42" s="128" t="n">
-        <v>172</v>
+        <v>16</v>
       </c>
       <c r="F42" s="123" t="n">
-        <v>9198.4</v>
+        <v>635.8</v>
       </c>
       <c r="G42" s="123" t="n">
-        <v>610.234</v>
+        <v>56.766</v>
       </c>
       <c r="H42" s="123" t="n">
-        <v>569.0638</v>
+        <v>52.9362</v>
       </c>
       <c r="I42" s="129" t="n">
-        <v>2.2462</v>
+        <v>0.209</v>
       </c>
     </row>
     <row r="43" ht="27" customHeight="1">
       <c r="A43" s="130" t="inlineStr">
         <is>
-          <t>Case Qty:</t>
+          <t>MADE IN CAMBODIA</t>
         </is>
       </c>
       <c r="B43" s="121" t="n">
@@ -4568,31 +4556,27 @@
       </c>
       <c r="D43" s="121" t="inlineStr">
         <is>
-          <t>BUFFALO HIDE</t>
+          <t>cow lol</t>
         </is>
       </c>
       <c r="E43" s="128" t="n">
-        <v>16</v>
+        <v>167</v>
       </c>
       <c r="F43" s="123" t="n">
-        <v>635.8</v>
+        <v>9074.200000000001</v>
       </c>
       <c r="G43" s="123" t="n">
-        <v>56.766</v>
+        <v>628.1919</v>
       </c>
       <c r="H43" s="123" t="n">
-        <v>52.9362</v>
+        <v>584.5</v>
       </c>
       <c r="I43" s="129" t="n">
-        <v>0.209</v>
+        <v>2.3069</v>
       </c>
     </row>
     <row r="44" ht="27" customHeight="1">
-      <c r="A44" s="130" t="inlineStr">
-        <is>
-          <t>MADE IN CAMBODIA</t>
-        </is>
-      </c>
+      <c r="A44" s="130" t="n"/>
       <c r="B44" s="121" t="n">
         <v>9000719487</v>
       </c>
@@ -4607,29 +4591,29 @@
         </is>
       </c>
       <c r="E44" s="128" t="n">
-        <v>167</v>
+        <v>5</v>
       </c>
       <c r="F44" s="123" t="n">
-        <v>9074.200000000001</v>
+        <v>247</v>
       </c>
       <c r="G44" s="123" t="n">
-        <v>628.1919</v>
+        <v>18.8081</v>
       </c>
       <c r="H44" s="123" t="n">
-        <v>584.5</v>
+        <v>17.5</v>
       </c>
       <c r="I44" s="129" t="n">
-        <v>2.3069</v>
+        <v>0.06909999999999999</v>
       </c>
     </row>
     <row r="45" ht="27" customHeight="1">
       <c r="A45" s="130" t="n"/>
       <c r="B45" s="121" t="n">
-        <v>9000719487</v>
+        <v>9000707052</v>
       </c>
       <c r="C45" s="121" t="inlineStr">
         <is>
-          <t>01.10.U722233</t>
+          <t>01.10.U528110</t>
         </is>
       </c>
       <c r="D45" s="121" t="inlineStr">
@@ -4638,19 +4622,19 @@
         </is>
       </c>
       <c r="E45" s="128" t="n">
-        <v>5</v>
+        <v>97</v>
       </c>
       <c r="F45" s="123" t="n">
-        <v>247</v>
+        <v>5048.7</v>
       </c>
       <c r="G45" s="123" t="n">
-        <v>18.8081</v>
+        <v>455.5</v>
       </c>
       <c r="H45" s="123" t="n">
-        <v>17.5</v>
+        <v>410.5</v>
       </c>
       <c r="I45" s="129" t="n">
-        <v>0.06909999999999999</v>
+        <v>1.782</v>
       </c>
     </row>
     <row r="46" ht="27" customHeight="1">
@@ -4669,10 +4653,10 @@
         </is>
       </c>
       <c r="E46" s="128" t="n">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F46" s="123" t="n">
-        <v>5048.7</v>
+        <v>5012.9</v>
       </c>
       <c r="G46" s="123" t="n">
         <v>455.5</v>
@@ -4700,19 +4684,19 @@
         </is>
       </c>
       <c r="E47" s="128" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F47" s="123" t="n">
-        <v>5012.9</v>
+        <v>4996.9</v>
       </c>
       <c r="G47" s="123" t="n">
-        <v>455.5</v>
+        <v>452</v>
       </c>
       <c r="H47" s="123" t="n">
-        <v>410.5</v>
+        <v>407</v>
       </c>
       <c r="I47" s="129" t="n">
-        <v>1.782</v>
+        <v>1.7424</v>
       </c>
     </row>
     <row r="48" ht="27" customHeight="1">
@@ -4731,19 +4715,19 @@
         </is>
       </c>
       <c r="E48" s="128" t="n">
-        <v>95</v>
+        <v>198</v>
       </c>
       <c r="F48" s="123" t="n">
-        <v>4996.9</v>
+        <v>10511.4</v>
       </c>
       <c r="G48" s="123" t="n">
-        <v>452</v>
+        <v>876.6079</v>
       </c>
       <c r="H48" s="123" t="n">
-        <v>407</v>
+        <v>837.3568</v>
       </c>
       <c r="I48" s="129" t="n">
-        <v>1.7424</v>
+        <v>2.4869</v>
       </c>
     </row>
     <row r="49" ht="27" customHeight="1">
@@ -4762,19 +4746,19 @@
         </is>
       </c>
       <c r="E49" s="128" t="n">
-        <v>198</v>
+        <v>29</v>
       </c>
       <c r="F49" s="123" t="n">
-        <v>10511.4</v>
+        <v>1162.8</v>
       </c>
       <c r="G49" s="123" t="n">
-        <v>876.6079</v>
+        <v>128.3921</v>
       </c>
       <c r="H49" s="123" t="n">
-        <v>837.3568</v>
+        <v>122.6432</v>
       </c>
       <c r="I49" s="129" t="n">
-        <v>2.4869</v>
+        <v>0.3643</v>
       </c>
     </row>
     <row r="50" ht="27" customHeight="1">
@@ -4784,7 +4768,7 @@
       </c>
       <c r="C50" s="121" t="inlineStr">
         <is>
-          <t>01.10.U528110</t>
+          <t>01.10.U528103</t>
         </is>
       </c>
       <c r="D50" s="121" t="inlineStr">
@@ -4793,19 +4777,19 @@
         </is>
       </c>
       <c r="E50" s="128" t="n">
-        <v>29</v>
+        <v>200</v>
       </c>
       <c r="F50" s="123" t="n">
-        <v>1162.8</v>
+        <v>10017.2</v>
       </c>
       <c r="G50" s="123" t="n">
-        <v>128.3921</v>
+        <v>858.5</v>
       </c>
       <c r="H50" s="123" t="n">
-        <v>122.6432</v>
+        <v>813.5</v>
       </c>
       <c r="I50" s="129" t="n">
-        <v>0.3643</v>
+        <v>2.5344</v>
       </c>
     </row>
     <row r="51" ht="27" customHeight="1">
@@ -4824,19 +4808,19 @@
         </is>
       </c>
       <c r="E51" s="128" t="n">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="F51" s="123" t="n">
-        <v>10017.2</v>
+        <v>10534.2</v>
       </c>
       <c r="G51" s="123" t="n">
-        <v>858.5</v>
+        <v>865.4032</v>
       </c>
       <c r="H51" s="123" t="n">
-        <v>813.5</v>
+        <v>827.2984</v>
       </c>
       <c r="I51" s="129" t="n">
-        <v>2.5344</v>
+        <v>2.5149</v>
       </c>
     </row>
     <row r="52" ht="27" customHeight="1">
@@ -4855,198 +4839,107 @@
         </is>
       </c>
       <c r="E52" s="128" t="n">
-        <v>210</v>
+        <v>38</v>
       </c>
       <c r="F52" s="123" t="n">
-        <v>10534.2</v>
+        <v>1513.7</v>
       </c>
       <c r="G52" s="123" t="n">
-        <v>865.4032</v>
+        <v>156.5968</v>
       </c>
       <c r="H52" s="123" t="n">
-        <v>827.2984</v>
+        <v>149.7016</v>
       </c>
       <c r="I52" s="129" t="n">
-        <v>2.5149</v>
+        <v>0.4551</v>
       </c>
     </row>
     <row r="53" ht="27" customHeight="1">
       <c r="A53" s="130" t="n"/>
-      <c r="B53" s="121" t="n">
-        <v>9000707052</v>
-      </c>
-      <c r="C53" s="121" t="inlineStr">
-        <is>
-          <t>01.10.U528103</t>
-        </is>
-      </c>
-      <c r="D53" s="121" t="inlineStr">
-        <is>
-          <t>cow lol</t>
-        </is>
-      </c>
-      <c r="E53" s="128" t="n">
-        <v>38</v>
-      </c>
-      <c r="F53" s="123" t="n">
-        <v>1513.7</v>
-      </c>
-      <c r="G53" s="123" t="n">
-        <v>156.5968</v>
-      </c>
-      <c r="H53" s="123" t="n">
-        <v>149.7016</v>
-      </c>
-      <c r="I53" s="129" t="n">
-        <v>0.4551</v>
-      </c>
+      <c r="B53" s="121" t="inlineStr">
+        <is>
+          <t>LEATHER (HS.CODE: 4107.12.00)</t>
+        </is>
+      </c>
+      <c r="C53" s="113" t="n"/>
+      <c r="D53" s="122" t="n"/>
+      <c r="E53" s="128" t="n"/>
+      <c r="F53" s="123" t="n"/>
+      <c r="G53" s="123" t="n"/>
+      <c r="H53" s="123" t="n"/>
+      <c r="I53" s="129" t="n"/>
     </row>
     <row r="54" ht="27" customFormat="1" customHeight="1" s="1">
-      <c r="A54" s="130" t="n"/>
-      <c r="B54" s="121" t="inlineStr">
-        <is>
-          <t>LEATHER (HS.CODE: 4107.12.00)</t>
-        </is>
-      </c>
-      <c r="C54" s="113" t="n"/>
-      <c r="D54" s="122" t="n"/>
-      <c r="E54" s="128" t="n"/>
-      <c r="F54" s="123" t="n"/>
-      <c r="G54" s="123" t="n"/>
-      <c r="H54" s="123" t="n"/>
-      <c r="I54" s="129" t="n"/>
-    </row>
-    <row r="55" ht="27" customHeight="1">
-      <c r="A55" s="112" t="n"/>
-      <c r="B55" s="112" t="inlineStr">
+      <c r="A54" s="112" t="n"/>
+      <c r="B54" s="112" t="inlineStr">
         <is>
           <t>TOTAL:</t>
         </is>
       </c>
-      <c r="C55" s="112" t="n"/>
-      <c r="D55" s="112" t="inlineStr">
+      <c r="C54" s="112" t="n"/>
+      <c r="D54" s="112" t="inlineStr">
         <is>
           <t>8 PALLETS</t>
         </is>
       </c>
-      <c r="E55" s="131">
-        <f>SUM(E41:E53)</f>
-        <v/>
-      </c>
-      <c r="F55" s="114">
-        <f>SUM(F41:F53)</f>
-        <v/>
-      </c>
-      <c r="G55" s="114">
-        <f>SUM(G41:G53)</f>
-        <v/>
-      </c>
-      <c r="H55" s="114">
-        <f>SUM(H41:H53)</f>
-        <v/>
-      </c>
-      <c r="I55" s="132">
-        <f>SUM(I41:I53)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="56" ht="24" customHeight="1">
-      <c r="B56" s="133" t="inlineStr">
+      <c r="E54" s="131">
+        <f>SUM(E40:E52)</f>
+        <v/>
+      </c>
+      <c r="F54" s="114">
+        <f>SUM(F40:F52)</f>
+        <v/>
+      </c>
+      <c r="G54" s="114">
+        <f>SUM(G40:G52)</f>
+        <v/>
+      </c>
+      <c r="H54" s="114">
+        <f>SUM(H40:H52)</f>
+        <v/>
+      </c>
+      <c r="I54" s="132">
+        <f>SUM(I40:I52)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="55" ht="42" customHeight="1">
+      <c r="B55" s="133" t="inlineStr">
         <is>
           <t>TOTAL OF:</t>
         </is>
       </c>
-      <c r="D56" s="133" t="inlineStr">
+      <c r="D55" s="133" t="inlineStr">
         <is>
           <t>16 PALLETS</t>
         </is>
       </c>
-      <c r="E56" s="134">
-        <f>SUM(E23:E34,E41:E53)</f>
-        <v/>
-      </c>
-      <c r="F56" s="135">
-        <f>SUM(F23:F34,F41:F53)</f>
-        <v/>
-      </c>
-      <c r="G56" s="135">
-        <f>SUM(G23:G34,G41:G53)</f>
-        <v/>
-      </c>
-      <c r="H56" s="135">
-        <f>SUM(H23:H34,H41:H53)</f>
-        <v/>
-      </c>
-      <c r="I56" s="136">
-        <f>SUM(I23:I34,I41:I53)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="57" ht="27" customHeight="1">
-      <c r="A57" s="137" t="n"/>
-      <c r="B57" s="138" t="inlineStr">
-        <is>
-          <t>TOTAL OF:</t>
-        </is>
-      </c>
-      <c r="C57" s="138" t="inlineStr">
-        <is>
-          <t>BUFFALO</t>
-        </is>
-      </c>
-      <c r="D57" s="138" t="inlineStr">
-        <is>
-          <t>9 PALLETS</t>
-        </is>
-      </c>
-      <c r="E57" s="139" t="n">
-        <v>1300</v>
-      </c>
-      <c r="F57" s="140" t="n">
-        <v>72108.09999999999</v>
-      </c>
-      <c r="G57" s="140" t="n">
-        <v>5995.5</v>
-      </c>
-      <c r="H57" s="140" t="n">
-        <v>5590.5</v>
-      </c>
-      <c r="I57" s="141" t="n">
-        <v>22.8096</v>
-      </c>
-    </row>
-    <row r="58" ht="27" customHeight="1">
-      <c r="A58" s="137" t="n"/>
-      <c r="B58" s="138" t="inlineStr">
-        <is>
-          <t>TOTAL OF:</t>
-        </is>
-      </c>
-      <c r="C58" s="138" t="inlineStr">
-        <is>
-          <t>LEATHER</t>
-        </is>
-      </c>
-      <c r="D58" s="138" t="inlineStr">
-        <is>
-          <t>7 PALLETS</t>
-        </is>
-      </c>
-      <c r="E58" s="139" t="n">
-        <v>1133</v>
-      </c>
-      <c r="F58" s="140" t="n">
-        <v>58119</v>
-      </c>
-      <c r="G58" s="140" t="n">
-        <v>4895.5</v>
-      </c>
-      <c r="H58" s="140" t="n">
-        <v>4580.5</v>
-      </c>
-      <c r="I58" s="141" t="n">
-        <v>16.038</v>
-      </c>
+      <c r="E55" s="134">
+        <f>SUM(E23:E34,E40:E52)</f>
+        <v/>
+      </c>
+      <c r="F55" s="135">
+        <f>SUM(F23:F34,F40:F52)</f>
+        <v/>
+      </c>
+      <c r="G55" s="135">
+        <f>SUM(G23:G34,G40:G52)</f>
+        <v/>
+      </c>
+      <c r="H55" s="135">
+        <f>SUM(H23:H34,H40:H52)</f>
+        <v/>
+      </c>
+      <c r="I55" s="136">
+        <f>SUM(I23:I34,I40:I52)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" ht="24" customHeight="1"/>
+    <row r="57" ht="69.75" customHeight="1"/>
+    <row r="58" ht="42" customHeight="1">
+      <c r="A58" s="20" t="n"/>
+      <c r="B58" s="65" t="n"/>
     </row>
     <row r="59" ht="53.1" customHeight="1">
       <c r="A59" s="13" t="inlineStr">
@@ -5397,34 +5290,33 @@
     <row r="199"/>
     <row r="200"/>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="B54:C54"/>
+  <mergeCells count="30">
     <mergeCell ref="B60:D60"/>
+    <mergeCell ref="H38:H39"/>
     <mergeCell ref="B55"/>
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="H21:H22"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="B36"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="B38:B39"/>
     <mergeCell ref="B21:B22"/>
-    <mergeCell ref="H39:H40"/>
     <mergeCell ref="A2:I2"/>
+    <mergeCell ref="E38:F38"/>
     <mergeCell ref="A5:I5"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="I21:I22"/>
+    <mergeCell ref="B54"/>
     <mergeCell ref="A4:I4"/>
+    <mergeCell ref="B53:C53"/>
     <mergeCell ref="A21:A22"/>
-    <mergeCell ref="I39:I40"/>
-    <mergeCell ref="B56"/>
     <mergeCell ref="A61:D61"/>
-    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="I38:I39"/>
     <mergeCell ref="A37"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="B38"/>
     <mergeCell ref="G21:G22"/>
     <mergeCell ref="A6:I6"/>
     <mergeCell ref="B35:C35"/>

</xml_diff>

<commit_message>
fixing fob, custom mode not filling value
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -450,7 +450,7 @@
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
@@ -804,18 +804,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="38" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="38" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="38" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="38" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1652,14 +1640,14 @@
         </is>
       </c>
       <c r="C16" s="111" t="n">
-        <v>7438.8</v>
-      </c>
-      <c r="D16" s="111" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="E16" s="111">
-        <f>D16 * C16</f>
+        <v>7681.5</v>
+      </c>
+      <c r="D16" s="111">
+        <f>E16/C16</f>
         <v/>
+      </c>
+      <c r="E16" s="111" t="n">
+        <v>9572.751</v>
       </c>
     </row>
     <row r="17" ht="30" customFormat="1" customHeight="1" s="36">
@@ -1668,18 +1656,18 @@
       </c>
       <c r="B17" s="110" t="inlineStr">
         <is>
-          <t>01.10.U756033</t>
+          <t>01.10.W653191</t>
         </is>
       </c>
       <c r="C17" s="111" t="n">
-        <v>242.7</v>
-      </c>
-      <c r="D17" s="111" t="n">
-        <v>1.13</v>
-      </c>
-      <c r="E17" s="111">
-        <f>D17 * C17</f>
+        <v>5748.5</v>
+      </c>
+      <c r="D17" s="111">
+        <f>E17/C17</f>
         <v/>
+      </c>
+      <c r="E17" s="111" t="n">
+        <v>7473.05</v>
       </c>
     </row>
     <row r="18" ht="30" customFormat="1" customHeight="1" s="36">
@@ -1688,18 +1676,18 @@
       </c>
       <c r="B18" s="110" t="inlineStr">
         <is>
-          <t>01.10.W653191</t>
+          <t>01.10.W783049</t>
         </is>
       </c>
       <c r="C18" s="111" t="n">
-        <v>5748.5</v>
-      </c>
-      <c r="D18" s="111" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="E18" s="111">
-        <f>D18 * C18</f>
+        <v>9376</v>
+      </c>
+      <c r="D18" s="111">
+        <f>E18/C18</f>
         <v/>
+      </c>
+      <c r="E18" s="111" t="n">
+        <v>14140.885</v>
       </c>
     </row>
     <row r="19" ht="30" customFormat="1" customHeight="1" s="36">
@@ -1712,14 +1700,14 @@
         </is>
       </c>
       <c r="C19" s="111" t="n">
-        <v>9263.5</v>
-      </c>
-      <c r="D19" s="111" t="n">
-        <v>1.51</v>
-      </c>
-      <c r="E19" s="111">
-        <f>D19 * C19</f>
+        <v>10077.9</v>
+      </c>
+      <c r="D19" s="111">
+        <f>E19/C19</f>
         <v/>
+      </c>
+      <c r="E19" s="111" t="n">
+        <v>15217.629</v>
       </c>
     </row>
     <row r="20" ht="30" customFormat="1" customHeight="1" s="36">
@@ -1728,18 +1716,18 @@
       </c>
       <c r="B20" s="110" t="inlineStr">
         <is>
-          <t>01.10.W783049</t>
+          <t>01.10.U741023</t>
         </is>
       </c>
       <c r="C20" s="111" t="n">
-        <v>112.5</v>
-      </c>
-      <c r="D20" s="111" t="n">
-        <v>1.36</v>
-      </c>
-      <c r="E20" s="111">
-        <f>D20 * C20</f>
+        <v>19497.3</v>
+      </c>
+      <c r="D20" s="111">
+        <f>E20/C20</f>
         <v/>
+      </c>
+      <c r="E20" s="111" t="n">
+        <v>25661.748</v>
       </c>
     </row>
     <row r="21" ht="30" customFormat="1" customHeight="1" s="36">
@@ -1748,18 +1736,18 @@
       </c>
       <c r="B21" s="110" t="inlineStr">
         <is>
-          <t>01.10.W783049</t>
+          <t>01.10.U741023</t>
         </is>
       </c>
       <c r="C21" s="111" t="n">
-        <v>10077.9</v>
-      </c>
-      <c r="D21" s="111" t="n">
-        <v>1.51</v>
-      </c>
-      <c r="E21" s="111">
-        <f>D21 * C21</f>
+        <v>9892.700000000001</v>
+      </c>
+      <c r="D21" s="111">
+        <f>E21/C21</f>
         <v/>
+      </c>
+      <c r="E21" s="111" t="n">
+        <v>13058.364</v>
       </c>
     </row>
     <row r="22" ht="30" customFormat="1" customHeight="1" s="36">
@@ -1768,18 +1756,18 @@
       </c>
       <c r="B22" s="110" t="inlineStr">
         <is>
-          <t>01.10.U741023</t>
+          <t>01.10.U722233</t>
         </is>
       </c>
       <c r="C22" s="111" t="n">
-        <v>18953.2</v>
-      </c>
-      <c r="D22" s="111" t="n">
-        <v>1.32</v>
-      </c>
-      <c r="E22" s="111">
-        <f>D22 * C22</f>
+        <v>9834.200000000001</v>
+      </c>
+      <c r="D22" s="111">
+        <f>E22/C22</f>
         <v/>
+      </c>
+      <c r="E22" s="111" t="n">
+        <v>12019.77</v>
       </c>
     </row>
     <row r="23" ht="30" customFormat="1" customHeight="1" s="36">
@@ -1788,18 +1776,18 @@
       </c>
       <c r="B23" s="110" t="inlineStr">
         <is>
-          <t>01.10.U741023</t>
+          <t>01.10.U722233</t>
         </is>
       </c>
       <c r="C23" s="111" t="n">
-        <v>56.5</v>
-      </c>
-      <c r="D23" s="111" t="n">
-        <v>1.12</v>
-      </c>
-      <c r="E23" s="111">
-        <f>D23 * C23</f>
+        <v>9321.200000000001</v>
+      </c>
+      <c r="D23" s="111">
+        <f>E23/C23</f>
         <v/>
+      </c>
+      <c r="E23" s="111" t="n">
+        <v>11420.616</v>
       </c>
     </row>
     <row r="24" ht="30" customFormat="1" customHeight="1" s="36">
@@ -1808,18 +1796,18 @@
       </c>
       <c r="B24" s="110" t="inlineStr">
         <is>
-          <t>01.10.U741023</t>
+          <t>01.10.U528110</t>
         </is>
       </c>
       <c r="C24" s="111" t="n">
-        <v>487.6</v>
-      </c>
-      <c r="D24" s="111" t="n">
-        <v>1.19</v>
-      </c>
-      <c r="E24" s="111">
-        <f>D24 * C24</f>
+        <v>26732.7</v>
+      </c>
+      <c r="D24" s="111">
+        <f>E24/C24</f>
         <v/>
+      </c>
+      <c r="E24" s="111" t="n">
+        <v>33799.365</v>
       </c>
     </row>
     <row r="25" ht="30" customFormat="1" customHeight="1" s="36">
@@ -1828,346 +1816,194 @@
       </c>
       <c r="B25" s="110" t="inlineStr">
         <is>
-          <t>01.10.U741023</t>
+          <t>01.10.U528103</t>
         </is>
       </c>
       <c r="C25" s="111" t="n">
-        <v>9892.700000000001</v>
-      </c>
-      <c r="D25" s="111" t="n">
-        <v>1.32</v>
-      </c>
-      <c r="E25" s="111">
-        <f>D25 * C25</f>
+        <v>22065.1</v>
+      </c>
+      <c r="D25" s="111">
+        <f>E25/C25</f>
         <v/>
       </c>
-    </row>
-    <row r="26" ht="30" customFormat="1" customHeight="1" s="37">
-      <c r="A26" s="110" t="n">
-        <v>11</v>
-      </c>
-      <c r="B26" s="110" t="inlineStr">
-        <is>
-          <t>01.10.U722233</t>
-        </is>
-      </c>
-      <c r="C26" s="111" t="n">
-        <v>9198.4</v>
-      </c>
-      <c r="D26" s="111" t="n">
-        <v>1.23</v>
-      </c>
-      <c r="E26" s="111">
-        <f>D26 * C26</f>
+      <c r="E25" s="111" t="n">
+        <v>27825.896</v>
+      </c>
+    </row>
+    <row r="26" ht="36" customFormat="1" customHeight="1" s="37">
+      <c r="A26" s="112" t="inlineStr">
+        <is>
+          <t>TOTAL:</t>
+        </is>
+      </c>
+      <c r="B26" s="113" t="n"/>
+      <c r="C26" s="114">
+        <f>SUM(C16:C25)</f>
         <v/>
       </c>
-    </row>
-    <row r="27" ht="30" customFormat="1" customHeight="1" s="37">
-      <c r="A27" s="110" t="n">
-        <v>12</v>
-      </c>
-      <c r="B27" s="110" t="inlineStr">
-        <is>
-          <t>01.10.U722233</t>
-        </is>
-      </c>
-      <c r="C27" s="111" t="n">
-        <v>635.8</v>
-      </c>
-      <c r="D27" s="111" t="n">
-        <v>1.11</v>
-      </c>
-      <c r="E27" s="111">
-        <f>D27 * C27</f>
+      <c r="D26" s="112" t="n"/>
+      <c r="E26" s="114">
+        <f>SUM(E16:E25)</f>
         <v/>
       </c>
     </row>
-    <row r="28" ht="30" customHeight="1">
-      <c r="A28" s="110" t="n">
-        <v>13</v>
-      </c>
-      <c r="B28" s="110" t="inlineStr">
-        <is>
-          <t>01.10.U722233</t>
-        </is>
-      </c>
-      <c r="C28" s="111" t="n">
-        <v>9074.200000000001</v>
-      </c>
-      <c r="D28" s="111" t="n">
-        <v>1.23</v>
-      </c>
-      <c r="E28" s="111">
-        <f>D28 * C28</f>
-        <v/>
-      </c>
-    </row>
-    <row r="29" ht="30" customHeight="1">
-      <c r="A29" s="110" t="n">
-        <v>14</v>
-      </c>
-      <c r="B29" s="110" t="inlineStr">
-        <is>
-          <t>01.10.U722233</t>
-        </is>
-      </c>
-      <c r="C29" s="111" t="n">
-        <v>247</v>
-      </c>
-      <c r="D29" s="111" t="n">
-        <v>1.05</v>
-      </c>
-      <c r="E29" s="111">
-        <f>D29 * C29</f>
-        <v/>
-      </c>
-    </row>
-    <row r="30" ht="30" customHeight="1">
-      <c r="A30" s="110" t="n">
-        <v>15</v>
-      </c>
-      <c r="B30" s="110" t="inlineStr">
-        <is>
-          <t>01.10.U528110</t>
-        </is>
-      </c>
-      <c r="C30" s="111" t="n">
-        <v>25569.9</v>
-      </c>
-      <c r="D30" s="111" t="n">
-        <v>1.27</v>
-      </c>
-      <c r="E30" s="111">
-        <f>D30 * C30</f>
-        <v/>
-      </c>
-    </row>
-    <row r="31" ht="30" customHeight="1">
-      <c r="A31" s="110" t="n">
-        <v>16</v>
-      </c>
-      <c r="B31" s="110" t="inlineStr">
-        <is>
-          <t>01.10.U528110</t>
-        </is>
-      </c>
-      <c r="C31" s="111" t="n">
-        <v>1162.8</v>
-      </c>
-      <c r="D31" s="111" t="n">
-        <v>1.14</v>
-      </c>
-      <c r="E31" s="111">
-        <f>D31 * C31</f>
-        <v/>
-      </c>
-    </row>
-    <row r="32" ht="30" customHeight="1">
-      <c r="A32" s="110" t="n">
-        <v>17</v>
-      </c>
-      <c r="B32" s="110" t="inlineStr">
-        <is>
-          <t>01.10.U528103</t>
-        </is>
-      </c>
-      <c r="C32" s="111" t="n">
-        <v>20551.4</v>
-      </c>
-      <c r="D32" s="111" t="n">
-        <v>1.27</v>
-      </c>
-      <c r="E32" s="111">
-        <f>D32 * C32</f>
-        <v/>
-      </c>
-    </row>
-    <row r="33" ht="30" customHeight="1">
-      <c r="A33" s="110" t="n">
-        <v>18</v>
-      </c>
-      <c r="B33" s="110" t="inlineStr">
-        <is>
-          <t>01.10.U528103</t>
-        </is>
-      </c>
-      <c r="C33" s="111" t="n">
-        <v>1513.7</v>
-      </c>
-      <c r="D33" s="111" t="n">
-        <v>1.14</v>
-      </c>
-      <c r="E33" s="111">
-        <f>D33 * C33</f>
-        <v/>
-      </c>
-    </row>
-    <row r="34" ht="36" customHeight="1">
-      <c r="A34" s="112" t="inlineStr">
-        <is>
-          <t>TOTAL:</t>
-        </is>
-      </c>
-      <c r="B34" s="113" t="n"/>
-      <c r="C34" s="114">
-        <f>SUM(C16:C33)</f>
-        <v/>
-      </c>
-      <c r="D34" s="112" t="n"/>
-      <c r="E34" s="114">
-        <f>SUM(E16:E33)</f>
-        <v/>
+    <row r="27" ht="57" customFormat="1" customHeight="1" s="37">
+      <c r="A27" s="94" t="n"/>
+      <c r="C27" s="115" t="n"/>
+      <c r="D27" s="115" t="n"/>
+      <c r="E27" s="115" t="n"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="45" t="inlineStr">
+        <is>
+          <t>FCA:</t>
+        </is>
+      </c>
+      <c r="B28" s="46" t="inlineStr">
+        <is>
+          <t>BAVET, SVAY RIENG</t>
+        </is>
+      </c>
+      <c r="C28" s="41" t="n"/>
+      <c r="D28" s="41" t="n"/>
+      <c r="E28" s="41" t="n"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="41" t="inlineStr">
+        <is>
+          <t>Term of Payment: 100% TT after shipment</t>
+        </is>
+      </c>
+      <c r="B29" s="41" t="n"/>
+      <c r="C29" s="41" t="n"/>
+      <c r="D29" s="41" t="n"/>
+      <c r="E29" s="41" t="n"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="41" t="inlineStr">
+        <is>
+          <t>Transaction method: FCA(USD)</t>
+        </is>
+      </c>
+      <c r="B30" s="41" t="n"/>
+      <c r="C30" s="41" t="n"/>
+      <c r="D30" s="41" t="n"/>
+      <c r="E30" s="41" t="n"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beneficiary bank information: </t>
+        </is>
+      </c>
+      <c r="B31" s="41" t="n"/>
+      <c r="C31" s="41" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO.,LTD.</t>
+        </is>
+      </c>
+      <c r="D31" s="41" t="n"/>
+      <c r="E31" s="41" t="n"/>
+    </row>
+    <row r="32" ht="45.95" customHeight="1">
+      <c r="A32" s="41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beneficiary Bank' s Name: </t>
+        </is>
+      </c>
+      <c r="B32" s="41" t="n"/>
+      <c r="C32" s="91" t="inlineStr">
+        <is>
+          <t>BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
+ /BANK OF CHINA PHNOM PENH BRANCH</t>
+        </is>
+      </c>
+    </row>
+    <row r="33" ht="41.1" customHeight="1">
+      <c r="A33" s="41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bank Address:  </t>
+        </is>
+      </c>
+      <c r="B33" s="41" t="n"/>
+      <c r="C33" s="91" t="inlineStr">
+        <is>
+          <t>1st AND 2nd FLOOR,CANADIA TOWER,No.315 ANDDUONG ST.
+PHNOM PEMH,CAMBODIA.</t>
+        </is>
+      </c>
+    </row>
+    <row r="34" ht="29.1" customHeight="1">
+      <c r="A34" s="41" t="inlineStr">
+        <is>
+          <t>Bank account :</t>
+        </is>
+      </c>
+      <c r="B34" s="41" t="n"/>
+      <c r="C34" s="92" t="inlineStr">
+        <is>
+          <t>100001100764430</t>
+        </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="94" t="n"/>
-      <c r="C35" s="115" t="n"/>
-      <c r="D35" s="115" t="n"/>
-      <c r="E35" s="115" t="n"/>
+      <c r="A35" s="41" t="inlineStr">
+        <is>
+          <t>SWIFT CODE  ：</t>
+        </is>
+      </c>
+      <c r="B35" s="41" t="n"/>
+      <c r="C35" s="41" t="inlineStr">
+        <is>
+          <t>BKCHKHPPXXX</t>
+        </is>
+      </c>
+      <c r="D35" s="41" t="n"/>
+      <c r="E35" s="41" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="45" t="inlineStr">
-        <is>
-          <t>FCA:</t>
-        </is>
-      </c>
-      <c r="B36" s="46" t="inlineStr">
-        <is>
-          <t>BAVET, SVAY RIENG</t>
-        </is>
-      </c>
+      <c r="A36" s="41" t="n"/>
+      <c r="B36" s="41" t="n"/>
       <c r="C36" s="41" t="n"/>
       <c r="D36" s="41" t="n"/>
       <c r="E36" s="41" t="n"/>
+      <c r="F36" s="41" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="41" t="inlineStr">
-        <is>
-          <t>Term of Payment: 100% TT after shipment</t>
-        </is>
-      </c>
-      <c r="B37" s="41" t="n"/>
-      <c r="C37" s="41" t="n"/>
-      <c r="D37" s="41" t="n"/>
-      <c r="E37" s="41" t="n"/>
+      <c r="A37" s="37" t="inlineStr">
+        <is>
+          <t>The Buyer:</t>
+        </is>
+      </c>
+      <c r="D37" s="47" t="inlineStr">
+        <is>
+          <t>The Seller:</t>
+        </is>
+      </c>
     </row>
     <row r="38">
-      <c r="A38" s="41" t="inlineStr">
-        <is>
-          <t>Transaction method: FCA(USD)</t>
-        </is>
-      </c>
-      <c r="B38" s="41" t="n"/>
-      <c r="C38" s="41" t="n"/>
-      <c r="D38" s="41" t="n"/>
-      <c r="E38" s="41" t="n"/>
-    </row>
-    <row r="39">
-      <c r="A39" s="41" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Beneficiary bank information: </t>
-        </is>
-      </c>
-      <c r="B39" s="41" t="n"/>
-      <c r="C39" s="41" t="inlineStr">
+      <c r="A38" s="73" t="inlineStr">
+        <is>
+          <t>JASON FURNITURE VIET NAM COMPANY LIMITED</t>
+        </is>
+      </c>
+      <c r="B38" s="72" t="n"/>
+      <c r="C38" s="48" t="n"/>
+      <c r="D38" s="73" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO.,LTD.</t>
         </is>
       </c>
-      <c r="D39" s="41" t="n"/>
-      <c r="E39" s="41" t="n"/>
-    </row>
-    <row r="40" ht="45.95" customHeight="1">
-      <c r="A40" s="41" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Beneficiary Bank' s Name: </t>
-        </is>
-      </c>
-      <c r="B40" s="41" t="n"/>
-      <c r="C40" s="91" t="inlineStr">
-        <is>
-          <t>BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
- /BANK OF CHINA PHNOM PENH BRANCH</t>
-        </is>
-      </c>
-    </row>
-    <row r="41" ht="41.1" customHeight="1">
-      <c r="A41" s="41" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Bank Address:  </t>
-        </is>
-      </c>
-      <c r="B41" s="41" t="n"/>
-      <c r="C41" s="91" t="inlineStr">
-        <is>
-          <t>1st AND 2nd FLOOR,CANADIA TOWER,No.315 ANDDUONG ST.
-PHNOM PEMH,CAMBODIA.</t>
-        </is>
-      </c>
-    </row>
-    <row r="42" ht="29.1" customHeight="1">
-      <c r="A42" s="41" t="inlineStr">
-        <is>
-          <t>Bank account :</t>
-        </is>
-      </c>
-      <c r="B42" s="41" t="n"/>
-      <c r="C42" s="92" t="inlineStr">
-        <is>
-          <t>100001100764430</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="41" t="inlineStr">
-        <is>
-          <t>SWIFT CODE  ：</t>
-        </is>
-      </c>
-      <c r="B43" s="41" t="n"/>
-      <c r="C43" s="41" t="inlineStr">
-        <is>
-          <t>BKCHKHPPXXX</t>
-        </is>
-      </c>
-      <c r="D43" s="41" t="n"/>
-      <c r="E43" s="41" t="n"/>
-    </row>
-    <row r="44">
-      <c r="A44" s="41" t="n"/>
-      <c r="B44" s="41" t="n"/>
-      <c r="C44" s="41" t="n"/>
-      <c r="D44" s="41" t="n"/>
-      <c r="E44" s="41" t="n"/>
-      <c r="F44" s="41" t="n"/>
-    </row>
-    <row r="45">
-      <c r="A45" s="37" t="inlineStr">
-        <is>
-          <t>The Buyer:</t>
-        </is>
-      </c>
-      <c r="D45" s="47" t="inlineStr">
-        <is>
-          <t>The Seller:</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="73" t="inlineStr">
-        <is>
-          <t>JASON FURNITURE VIET NAM COMPANY LIMITED</t>
-        </is>
-      </c>
-      <c r="B46" s="72" t="n"/>
-      <c r="C46" s="48" t="n"/>
-      <c r="D46" s="73" t="inlineStr">
-        <is>
-          <t>CALIFOR UPHOLSTERY MATERIALS CO.,LTD.</t>
-        </is>
-      </c>
-      <c r="E46" s="73" t="n"/>
-    </row>
+      <c r="E38" s="73" t="n"/>
+    </row>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
+    <row r="42"/>
+    <row r="43"/>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46"/>
     <row r="47"/>
     <row r="48"/>
     <row r="49"/>
@@ -2324,16 +2160,16 @@
     <row r="200" ht="27.95" customHeight="1"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C33:E33"/>
     <mergeCell ref="A12:D12"/>
-    <mergeCell ref="C40:E40"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="B10:E10"/>
-    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="C32:E32"/>
     <mergeCell ref="A200:B200"/>
   </mergeCells>
   <pageMargins left="0.432638888888889" right="0.314583333333333" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2669,14 +2505,14 @@
         </is>
       </c>
       <c r="E22" s="123" t="n">
-        <v>7438.8</v>
-      </c>
-      <c r="F22" s="123" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="G22" s="123">
-        <f>F22 * E22</f>
+        <v>7681.5</v>
+      </c>
+      <c r="F22" s="123">
+        <f>G22/E22</f>
         <v/>
+      </c>
+      <c r="G22" s="123" t="n">
+        <v>9572.751</v>
       </c>
     </row>
     <row r="23" ht="35" customHeight="1">
@@ -2687,12 +2523,12 @@
       </c>
       <c r="B23" s="121" t="inlineStr">
         <is>
-          <t>9000619872</t>
+          <t>9000691966</t>
         </is>
       </c>
       <c r="C23" s="121" t="inlineStr">
         <is>
-          <t>01.10.U756033</t>
+          <t>01.10.W653191</t>
         </is>
       </c>
       <c r="D23" s="122" t="inlineStr">
@@ -2701,14 +2537,14 @@
         </is>
       </c>
       <c r="E23" s="123" t="n">
-        <v>242.7</v>
-      </c>
-      <c r="F23" s="123" t="n">
-        <v>1.13</v>
-      </c>
-      <c r="G23" s="123">
-        <f>F23 * E23</f>
+        <v>5748.5</v>
+      </c>
+      <c r="F23" s="123">
+        <f>G23/E23</f>
         <v/>
+      </c>
+      <c r="G23" s="123" t="n">
+        <v>7473.05</v>
       </c>
     </row>
     <row r="24" ht="35" customHeight="1">
@@ -2719,12 +2555,12 @@
       </c>
       <c r="B24" s="121" t="inlineStr">
         <is>
-          <t>9000691966</t>
+          <t>9000606101</t>
         </is>
       </c>
       <c r="C24" s="121" t="inlineStr">
         <is>
-          <t>01.10.W653191</t>
+          <t>01.10.W783049</t>
         </is>
       </c>
       <c r="D24" s="122" t="inlineStr">
@@ -2733,21 +2569,21 @@
         </is>
       </c>
       <c r="E24" s="123" t="n">
-        <v>5748.5</v>
-      </c>
-      <c r="F24" s="123" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="G24" s="123">
-        <f>F24 * E24</f>
+        <v>9376</v>
+      </c>
+      <c r="F24" s="123">
+        <f>G24/E24</f>
         <v/>
+      </c>
+      <c r="G24" s="123" t="n">
+        <v>14140.885</v>
       </c>
     </row>
     <row r="25" ht="35" customHeight="1">
       <c r="A25" s="124" t="n"/>
       <c r="B25" s="121" t="inlineStr">
         <is>
-          <t>9000606101</t>
+          <t>9000678466</t>
         </is>
       </c>
       <c r="C25" s="121" t="inlineStr">
@@ -2761,26 +2597,26 @@
         </is>
       </c>
       <c r="E25" s="123" t="n">
-        <v>9263.5</v>
-      </c>
-      <c r="F25" s="123" t="n">
-        <v>1.51</v>
-      </c>
-      <c r="G25" s="123">
-        <f>F25 * E25</f>
+        <v>10077.9</v>
+      </c>
+      <c r="F25" s="123">
+        <f>G25/E25</f>
         <v/>
+      </c>
+      <c r="G25" s="123" t="n">
+        <v>15217.629</v>
       </c>
     </row>
     <row r="26" ht="35" customHeight="1">
       <c r="A26" s="124" t="n"/>
       <c r="B26" s="121" t="inlineStr">
         <is>
-          <t>9000606101</t>
+          <t>9000707953</t>
         </is>
       </c>
       <c r="C26" s="121" t="inlineStr">
         <is>
-          <t>01.10.W783049</t>
+          <t>01.10.U741023</t>
         </is>
       </c>
       <c r="D26" s="122" t="inlineStr">
@@ -2789,26 +2625,26 @@
         </is>
       </c>
       <c r="E26" s="123" t="n">
-        <v>112.5</v>
-      </c>
-      <c r="F26" s="123" t="n">
-        <v>1.36</v>
-      </c>
-      <c r="G26" s="123">
-        <f>F26 * E26</f>
+        <v>19497.3</v>
+      </c>
+      <c r="F26" s="123">
+        <f>G26/E26</f>
         <v/>
+      </c>
+      <c r="G26" s="123" t="n">
+        <v>25661.748</v>
       </c>
     </row>
     <row r="27" ht="35" customFormat="1" customHeight="1" s="1">
       <c r="A27" s="124" t="n"/>
       <c r="B27" s="121" t="inlineStr">
         <is>
-          <t>9000678466</t>
+          <t>9000719487</t>
         </is>
       </c>
       <c r="C27" s="121" t="inlineStr">
         <is>
-          <t>01.10.W783049</t>
+          <t>01.10.U741023</t>
         </is>
       </c>
       <c r="D27" s="122" t="inlineStr">
@@ -2817,26 +2653,26 @@
         </is>
       </c>
       <c r="E27" s="123" t="n">
-        <v>10077.9</v>
-      </c>
-      <c r="F27" s="123" t="n">
-        <v>1.51</v>
-      </c>
-      <c r="G27" s="123">
-        <f>F27 * E27</f>
+        <v>9892.700000000001</v>
+      </c>
+      <c r="F27" s="123">
+        <f>G27/E27</f>
         <v/>
+      </c>
+      <c r="G27" s="123" t="n">
+        <v>13058.364</v>
       </c>
     </row>
     <row r="28" ht="35" customHeight="1">
       <c r="A28" s="124" t="n"/>
       <c r="B28" s="121" t="inlineStr">
         <is>
-          <t>9000707953</t>
+          <t>9000719487</t>
         </is>
       </c>
       <c r="C28" s="121" t="inlineStr">
         <is>
-          <t>01.10.U741023</t>
+          <t>01.10.U722233</t>
         </is>
       </c>
       <c r="D28" s="122" t="inlineStr">
@@ -2845,495 +2681,319 @@
         </is>
       </c>
       <c r="E28" s="123" t="n">
-        <v>18953.2</v>
-      </c>
-      <c r="F28" s="123" t="n">
-        <v>1.32</v>
-      </c>
-      <c r="G28" s="123">
-        <f>F28 * E28</f>
+        <v>9834.200000000001</v>
+      </c>
+      <c r="F28" s="123">
+        <f>G28/E28</f>
         <v/>
+      </c>
+      <c r="G28" s="123" t="n">
+        <v>12019.77</v>
       </c>
     </row>
     <row r="29" ht="35" customHeight="1">
       <c r="A29" s="124" t="n"/>
       <c r="B29" s="121" t="inlineStr">
         <is>
-          <t>9000707953</t>
+          <t>9000719487</t>
         </is>
       </c>
       <c r="C29" s="121" t="inlineStr">
         <is>
-          <t>01.10.U741023</t>
+          <t>01.10.U722233</t>
         </is>
       </c>
       <c r="D29" s="122" t="inlineStr">
         <is>
-          <t>BUFFALO HIDE</t>
+          <t>cow lol</t>
         </is>
       </c>
       <c r="E29" s="123" t="n">
-        <v>56.5</v>
-      </c>
-      <c r="F29" s="123" t="n">
-        <v>1.12</v>
-      </c>
-      <c r="G29" s="123">
-        <f>F29 * E29</f>
+        <v>9321.200000000001</v>
+      </c>
+      <c r="F29" s="123">
+        <f>G29/E29</f>
         <v/>
+      </c>
+      <c r="G29" s="123" t="n">
+        <v>11420.616</v>
       </c>
     </row>
     <row r="30" ht="35" customHeight="1">
       <c r="A30" s="124" t="n"/>
       <c r="B30" s="121" t="inlineStr">
         <is>
-          <t>9000707953</t>
+          <t>9000707052</t>
         </is>
       </c>
       <c r="C30" s="121" t="inlineStr">
         <is>
-          <t>01.10.U741023</t>
+          <t>01.10.U528110</t>
         </is>
       </c>
       <c r="D30" s="122" t="inlineStr">
         <is>
-          <t>BUFFALO HIDE</t>
+          <t>cow lol</t>
         </is>
       </c>
       <c r="E30" s="123" t="n">
-        <v>487.6</v>
-      </c>
-      <c r="F30" s="123" t="n">
-        <v>1.19</v>
-      </c>
-      <c r="G30" s="123">
-        <f>F30 * E30</f>
+        <v>26732.7</v>
+      </c>
+      <c r="F30" s="123">
+        <f>G30/E30</f>
         <v/>
+      </c>
+      <c r="G30" s="123" t="n">
+        <v>33799.365</v>
       </c>
     </row>
     <row r="31" ht="35" customHeight="1">
       <c r="A31" s="124" t="n"/>
       <c r="B31" s="121" t="inlineStr">
         <is>
-          <t>9000719487</t>
+          <t>9000707052</t>
         </is>
       </c>
       <c r="C31" s="121" t="inlineStr">
         <is>
-          <t>01.10.U741023</t>
+          <t>01.10.U528103</t>
         </is>
       </c>
       <c r="D31" s="122" t="inlineStr">
         <is>
-          <t>BUFFALO HIDE</t>
+          <t>cow lol</t>
         </is>
       </c>
       <c r="E31" s="123" t="n">
-        <v>9892.700000000001</v>
-      </c>
-      <c r="F31" s="123" t="n">
-        <v>1.32</v>
-      </c>
-      <c r="G31" s="123">
-        <f>F31 * E31</f>
+        <v>22065.1</v>
+      </c>
+      <c r="F31" s="123">
+        <f>G31/E31</f>
         <v/>
       </c>
+      <c r="G31" s="123" t="n">
+        <v>27825.896</v>
+      </c>
     </row>
     <row r="32" ht="35" customHeight="1">
-      <c r="A32" s="124" t="n"/>
-      <c r="B32" s="121" t="inlineStr">
-        <is>
-          <t>9000719487</t>
-        </is>
-      </c>
-      <c r="C32" s="121" t="inlineStr">
-        <is>
-          <t>01.10.U722233</t>
-        </is>
-      </c>
-      <c r="D32" s="122" t="inlineStr">
-        <is>
-          <t>BUFFALO HIDE</t>
-        </is>
-      </c>
-      <c r="E32" s="123" t="n">
-        <v>9198.4</v>
-      </c>
-      <c r="F32" s="123" t="n">
-        <v>1.23</v>
-      </c>
-      <c r="G32" s="123">
-        <f>F32 * E32</f>
+      <c r="A32" s="112" t="n"/>
+      <c r="B32" s="112" t="inlineStr">
+        <is>
+          <t>TOTAL:</t>
+        </is>
+      </c>
+      <c r="C32" s="112" t="n"/>
+      <c r="D32" s="112" t="inlineStr">
+        <is>
+          <t>16 PALLETS</t>
+        </is>
+      </c>
+      <c r="E32" s="114">
+        <f>SUM(E22:E31)</f>
         <v/>
       </c>
-    </row>
-    <row r="33" ht="35" customHeight="1">
-      <c r="A33" s="124" t="n"/>
-      <c r="B33" s="121" t="inlineStr">
-        <is>
-          <t>9000719487</t>
-        </is>
-      </c>
-      <c r="C33" s="121" t="inlineStr">
-        <is>
-          <t>01.10.U722233</t>
-        </is>
-      </c>
-      <c r="D33" s="122" t="inlineStr">
-        <is>
-          <t>BUFFALO HIDE</t>
-        </is>
-      </c>
-      <c r="E33" s="123" t="n">
-        <v>635.8</v>
-      </c>
-      <c r="F33" s="123" t="n">
-        <v>1.11</v>
-      </c>
-      <c r="G33" s="123">
-        <f>F33 * E33</f>
+      <c r="F32" s="112" t="n"/>
+      <c r="G32" s="114">
+        <f>SUM(G22:G31)</f>
         <v/>
       </c>
     </row>
-    <row r="34" ht="35" customHeight="1">
-      <c r="A34" s="124" t="n"/>
-      <c r="B34" s="121" t="inlineStr">
-        <is>
-          <t>9000719487</t>
-        </is>
-      </c>
-      <c r="C34" s="121" t="inlineStr">
-        <is>
-          <t>01.10.U722233</t>
-        </is>
-      </c>
-      <c r="D34" s="122" t="inlineStr">
-        <is>
-          <t>cow lol</t>
-        </is>
-      </c>
-      <c r="E34" s="123" t="n">
-        <v>9074.200000000001</v>
-      </c>
-      <c r="F34" s="123" t="n">
-        <v>1.23</v>
-      </c>
-      <c r="G34" s="123">
-        <f>F34 * E34</f>
-        <v/>
-      </c>
-    </row>
-    <row r="35" ht="35" customHeight="1">
-      <c r="A35" s="124" t="n"/>
-      <c r="B35" s="121" t="inlineStr">
-        <is>
-          <t>9000719487</t>
-        </is>
-      </c>
-      <c r="C35" s="121" t="inlineStr">
-        <is>
-          <t>01.10.U722233</t>
-        </is>
-      </c>
-      <c r="D35" s="122" t="inlineStr">
-        <is>
-          <t>cow lol</t>
-        </is>
-      </c>
-      <c r="E35" s="123" t="n">
-        <v>247</v>
-      </c>
-      <c r="F35" s="123" t="n">
-        <v>1.05</v>
-      </c>
-      <c r="G35" s="123">
-        <f>F35 * E35</f>
-        <v/>
-      </c>
-    </row>
-    <row r="36" ht="35" customHeight="1">
-      <c r="A36" s="124" t="n"/>
-      <c r="B36" s="121" t="inlineStr">
-        <is>
-          <t>9000707052</t>
-        </is>
-      </c>
-      <c r="C36" s="121" t="inlineStr">
-        <is>
-          <t>01.10.U528110</t>
-        </is>
-      </c>
-      <c r="D36" s="122" t="inlineStr">
-        <is>
-          <t>cow lol</t>
-        </is>
-      </c>
-      <c r="E36" s="123" t="n">
-        <v>25569.9</v>
-      </c>
-      <c r="F36" s="123" t="n">
-        <v>1.27</v>
-      </c>
-      <c r="G36" s="123">
-        <f>F36 * E36</f>
-        <v/>
-      </c>
-    </row>
-    <row r="37" ht="35" customHeight="1">
-      <c r="A37" s="124" t="n"/>
-      <c r="B37" s="121" t="inlineStr">
-        <is>
-          <t>9000707052</t>
-        </is>
-      </c>
-      <c r="C37" s="121" t="inlineStr">
-        <is>
-          <t>01.10.U528110</t>
-        </is>
-      </c>
-      <c r="D37" s="122" t="inlineStr">
-        <is>
-          <t>cow lol</t>
-        </is>
-      </c>
-      <c r="E37" s="123" t="n">
-        <v>1162.8</v>
-      </c>
-      <c r="F37" s="123" t="n">
-        <v>1.14</v>
-      </c>
-      <c r="G37" s="123">
-        <f>F37 * E37</f>
-        <v/>
-      </c>
-    </row>
-    <row r="38" ht="35" customHeight="1">
-      <c r="A38" s="124" t="n"/>
-      <c r="B38" s="121" t="inlineStr">
-        <is>
-          <t>9000707052</t>
-        </is>
-      </c>
-      <c r="C38" s="121" t="inlineStr">
-        <is>
-          <t>01.10.U528103</t>
-        </is>
-      </c>
-      <c r="D38" s="122" t="inlineStr">
-        <is>
-          <t>cow lol</t>
-        </is>
-      </c>
-      <c r="E38" s="123" t="n">
-        <v>20551.4</v>
-      </c>
-      <c r="F38" s="123" t="n">
-        <v>1.27</v>
-      </c>
-      <c r="G38" s="123">
-        <f>F38 * E38</f>
-        <v/>
-      </c>
-    </row>
-    <row r="39" ht="35" customHeight="1">
-      <c r="A39" s="124" t="n"/>
-      <c r="B39" s="121" t="inlineStr">
-        <is>
-          <t>9000707052</t>
-        </is>
-      </c>
-      <c r="C39" s="121" t="inlineStr">
-        <is>
-          <t>01.10.U528103</t>
-        </is>
-      </c>
-      <c r="D39" s="122" t="inlineStr">
-        <is>
-          <t>cow lol</t>
-        </is>
-      </c>
-      <c r="E39" s="123" t="n">
-        <v>1513.7</v>
-      </c>
-      <c r="F39" s="123" t="n">
-        <v>1.14</v>
-      </c>
-      <c r="G39" s="123">
-        <f>F39 * E39</f>
-        <v/>
-      </c>
-    </row>
-    <row r="40" ht="35" customHeight="1">
-      <c r="A40" s="112" t="n"/>
-      <c r="B40" s="112" t="inlineStr">
-        <is>
-          <t>TOTAL:</t>
-        </is>
-      </c>
-      <c r="C40" s="112" t="n"/>
-      <c r="D40" s="112" t="inlineStr">
-        <is>
-          <t>16 PALLETS</t>
-        </is>
-      </c>
-      <c r="E40" s="112">
-        <f>SUM(E22:E39)</f>
-        <v/>
-      </c>
-      <c r="F40" s="112" t="n"/>
-      <c r="G40" s="112">
-        <f>SUM(G22:G39)</f>
-        <v/>
-      </c>
+    <row r="33" ht="27.75" customHeight="1">
+      <c r="A33" s="21" t="n"/>
+      <c r="B33" s="21" t="n"/>
+      <c r="C33" s="22" t="n"/>
+      <c r="D33" s="22" t="n"/>
+      <c r="E33" s="22" t="n"/>
+      <c r="F33" s="22" t="n"/>
+      <c r="G33" s="18" t="n"/>
+      <c r="L33" s="49" t="n"/>
+      <c r="M33" s="50" t="n"/>
+      <c r="N33" s="51" t="n"/>
+      <c r="O33" s="51" t="n"/>
+    </row>
+    <row r="34" ht="42" customHeight="1">
+      <c r="A34" s="101" t="inlineStr">
+        <is>
+          <t>Country of Original Cambodia</t>
+        </is>
+      </c>
+      <c r="D34" s="101" t="n"/>
+      <c r="E34" s="4" t="n"/>
+      <c r="F34" s="33" t="n"/>
+      <c r="G34" s="96" t="n"/>
+      <c r="L34" s="49" t="n"/>
+      <c r="M34" s="50" t="n"/>
+      <c r="N34" s="51" t="n"/>
+      <c r="O34" s="51" t="n"/>
+    </row>
+    <row r="35" ht="61.5" customHeight="1">
+      <c r="A35" s="28" t="inlineStr">
+        <is>
+          <t>Manufacture:</t>
+        </is>
+      </c>
+      <c r="B35" s="102" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
+XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
+        </is>
+      </c>
+      <c r="D35" s="102" t="n"/>
+      <c r="E35" s="102" t="n"/>
+      <c r="F35" s="4" t="n"/>
+      <c r="G35" s="96" t="n"/>
+      <c r="L35" s="49" t="n"/>
+      <c r="M35" s="50" t="n"/>
+      <c r="N35" s="51" t="n"/>
+      <c r="O35" s="51" t="n"/>
+    </row>
+    <row r="36" ht="42" customHeight="1">
+      <c r="A36" s="103" t="inlineStr">
+        <is>
+          <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
+                                                  /BANK OF CHINA PHNOM PENH BRANCH</t>
+        </is>
+      </c>
+      <c r="D36" s="103" t="n"/>
+      <c r="E36" s="103" t="n"/>
+      <c r="F36" s="103" t="n"/>
+      <c r="G36" s="96" t="n"/>
+      <c r="L36" s="49" t="n"/>
+      <c r="M36" s="50" t="n"/>
+      <c r="N36" s="51" t="n"/>
+      <c r="O36" s="51" t="n"/>
+    </row>
+    <row r="37" ht="24.75" customHeight="1">
+      <c r="A37" s="99" t="inlineStr">
+        <is>
+          <t>A/C NO:100001100764430</t>
+        </is>
+      </c>
+      <c r="L37" s="49" t="n"/>
+      <c r="M37" s="50" t="n"/>
+      <c r="N37" s="51" t="n"/>
+      <c r="O37" s="51" t="n"/>
+    </row>
+    <row r="38" ht="27" customHeight="1">
+      <c r="A38" s="99" t="inlineStr">
+        <is>
+          <t>SWIFT CODE  ：BKCHKHPPXXX</t>
+        </is>
+      </c>
+      <c r="L38" s="49" t="n"/>
+      <c r="M38" s="50" t="n"/>
+      <c r="N38" s="51" t="n"/>
+      <c r="O38" s="51" t="n"/>
+    </row>
+    <row r="39" ht="21" customHeight="1">
+      <c r="E39" s="81" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
+        </is>
+      </c>
+      <c r="F39" s="81" t="n"/>
+      <c r="G39" s="81" t="n"/>
+      <c r="H39" s="81" t="n"/>
+      <c r="L39" s="49" t="n"/>
+      <c r="M39" s="50" t="n"/>
+      <c r="N39" s="51" t="n"/>
+      <c r="O39" s="51" t="n"/>
+    </row>
+    <row r="40" ht="21" customHeight="1">
+      <c r="D40" s="78" t="n"/>
+      <c r="E40" s="76" t="n"/>
+      <c r="F40" s="79" t="inlineStr">
+        <is>
+          <t>Sign &amp; Stamp</t>
+        </is>
+      </c>
+      <c r="G40" s="80" t="n"/>
+      <c r="L40" s="49" t="n"/>
+      <c r="M40" s="50" t="n"/>
+      <c r="N40" s="51" t="n"/>
+      <c r="O40" s="51" t="n"/>
     </row>
     <row r="41" ht="21" customHeight="1">
-      <c r="A41" s="21" t="n"/>
-      <c r="B41" s="21" t="n"/>
-      <c r="C41" s="22" t="n"/>
-      <c r="D41" s="22" t="n"/>
-      <c r="E41" s="22" t="n"/>
-      <c r="F41" s="22" t="n"/>
-      <c r="G41" s="18" t="n"/>
+      <c r="D41" s="78" t="n"/>
+      <c r="E41" s="76" t="n"/>
+      <c r="F41" s="76" t="n"/>
+      <c r="G41" s="80" t="n"/>
       <c r="L41" s="49" t="n"/>
       <c r="M41" s="50" t="n"/>
       <c r="N41" s="51" t="n"/>
       <c r="O41" s="51" t="n"/>
     </row>
-    <row r="42" ht="42" customHeight="1">
-      <c r="A42" s="101" t="inlineStr">
-        <is>
-          <t>Country of Original Cambodia</t>
-        </is>
-      </c>
-      <c r="D42" s="101" t="n"/>
-      <c r="E42" s="4" t="n"/>
-      <c r="F42" s="33" t="n"/>
-      <c r="G42" s="96" t="n"/>
+    <row r="42" ht="21" customHeight="1">
+      <c r="D42" s="78" t="n"/>
+      <c r="E42" s="76" t="n"/>
+      <c r="F42" s="76" t="n"/>
+      <c r="G42" s="80" t="n"/>
       <c r="L42" s="49" t="n"/>
       <c r="M42" s="50" t="n"/>
       <c r="N42" s="51" t="n"/>
       <c r="O42" s="51" t="n"/>
     </row>
-    <row r="43" ht="61.5" customHeight="1">
-      <c r="A43" s="28" t="inlineStr">
-        <is>
-          <t>Manufacture:</t>
-        </is>
-      </c>
-      <c r="B43" s="102" t="inlineStr">
-        <is>
-          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
-XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
-        </is>
-      </c>
-      <c r="D43" s="102" t="n"/>
-      <c r="E43" s="102" t="n"/>
-      <c r="F43" s="4" t="n"/>
-      <c r="G43" s="96" t="n"/>
+    <row r="43" ht="21" customHeight="1">
+      <c r="D43" s="78" t="n"/>
+      <c r="E43" s="76" t="n"/>
+      <c r="F43" s="77" t="inlineStr">
+        <is>
+          <t>ZENG XUELI</t>
+        </is>
+      </c>
+      <c r="G43" s="77" t="n"/>
       <c r="L43" s="49" t="n"/>
       <c r="M43" s="50" t="n"/>
       <c r="N43" s="51" t="n"/>
       <c r="O43" s="51" t="n"/>
     </row>
-    <row r="44" ht="42" customHeight="1">
-      <c r="A44" s="103" t="inlineStr">
-        <is>
-          <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
-                                                  /BANK OF CHINA PHNOM PENH BRANCH</t>
-        </is>
-      </c>
-      <c r="D44" s="103" t="n"/>
-      <c r="E44" s="103" t="n"/>
-      <c r="F44" s="103" t="n"/>
-      <c r="G44" s="96" t="n"/>
-      <c r="L44" s="49" t="n"/>
-      <c r="M44" s="50" t="n"/>
-      <c r="N44" s="51" t="n"/>
-      <c r="O44" s="51" t="n"/>
-    </row>
-    <row r="45" ht="24.75" customHeight="1">
-      <c r="A45" s="99" t="inlineStr">
-        <is>
-          <t>A/C NO:100001100764430</t>
-        </is>
-      </c>
-      <c r="L45" s="49" t="n"/>
-      <c r="M45" s="50" t="n"/>
-      <c r="N45" s="51" t="n"/>
-      <c r="O45" s="51" t="n"/>
-    </row>
-    <row r="46" ht="27" customHeight="1">
-      <c r="A46" s="99" t="inlineStr">
-        <is>
-          <t>SWIFT CODE  ：BKCHKHPPXXX</t>
-        </is>
-      </c>
-      <c r="L46" s="49" t="n"/>
-      <c r="M46" s="50" t="n"/>
-      <c r="N46" s="51" t="n"/>
-      <c r="O46" s="51" t="n"/>
+    <row r="44" ht="21" customHeight="1">
+      <c r="D44" s="74" t="n"/>
+      <c r="E44" s="74" t="n"/>
+      <c r="F44" s="74" t="n"/>
+      <c r="G44" s="75" t="n"/>
+    </row>
+    <row r="45" ht="25.5" customHeight="1">
+      <c r="D45" s="74" t="n"/>
+      <c r="E45" s="74" t="n"/>
+      <c r="F45" s="74" t="n"/>
+      <c r="G45" s="75" t="n"/>
+    </row>
+    <row r="46" ht="21" customHeight="1">
+      <c r="D46" s="74" t="n"/>
+      <c r="E46" s="74" t="n"/>
+      <c r="F46" s="74" t="n"/>
+      <c r="G46" s="75" t="n"/>
     </row>
     <row r="47" ht="21" customHeight="1">
-      <c r="E47" s="81" t="inlineStr">
-        <is>
-          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
-        </is>
-      </c>
-      <c r="F47" s="81" t="n"/>
-      <c r="G47" s="81" t="n"/>
-      <c r="H47" s="81" t="n"/>
-      <c r="L47" s="49" t="n"/>
-      <c r="M47" s="50" t="n"/>
-      <c r="N47" s="51" t="n"/>
-      <c r="O47" s="51" t="n"/>
+      <c r="D47" s="74" t="n"/>
+      <c r="E47" s="74" t="n"/>
+      <c r="F47" s="74" t="n"/>
+      <c r="G47" s="75" t="n"/>
     </row>
     <row r="48" ht="21" customHeight="1">
-      <c r="D48" s="78" t="n"/>
-      <c r="E48" s="76" t="n"/>
-      <c r="F48" s="79" t="inlineStr">
-        <is>
-          <t>Sign &amp; Stamp</t>
-        </is>
-      </c>
-      <c r="G48" s="80" t="n"/>
-      <c r="L48" s="49" t="n"/>
-      <c r="M48" s="50" t="n"/>
-      <c r="N48" s="51" t="n"/>
-      <c r="O48" s="51" t="n"/>
+      <c r="D48" s="74" t="n"/>
+      <c r="E48" s="74" t="n"/>
+      <c r="F48" s="74" t="n"/>
+      <c r="G48" s="75" t="n"/>
     </row>
     <row r="49" ht="21" customHeight="1">
-      <c r="D49" s="78" t="n"/>
-      <c r="E49" s="76" t="n"/>
-      <c r="F49" s="76" t="n"/>
-      <c r="G49" s="80" t="n"/>
-      <c r="L49" s="49" t="n"/>
-      <c r="M49" s="50" t="n"/>
-      <c r="N49" s="51" t="n"/>
-      <c r="O49" s="51" t="n"/>
+      <c r="D49" s="74" t="n"/>
+      <c r="E49" s="74" t="n"/>
+      <c r="F49" s="74" t="n"/>
+      <c r="G49" s="75" t="n"/>
     </row>
     <row r="50" ht="21" customHeight="1">
-      <c r="D50" s="78" t="n"/>
-      <c r="E50" s="76" t="n"/>
-      <c r="F50" s="76" t="n"/>
-      <c r="G50" s="80" t="n"/>
-      <c r="L50" s="49" t="n"/>
-      <c r="M50" s="50" t="n"/>
-      <c r="N50" s="51" t="n"/>
-      <c r="O50" s="51" t="n"/>
+      <c r="D50" s="74" t="n"/>
+      <c r="E50" s="74" t="n"/>
+      <c r="F50" s="74" t="n"/>
+      <c r="G50" s="75" t="n"/>
     </row>
     <row r="51" ht="17.25" customHeight="1">
-      <c r="D51" s="78" t="n"/>
-      <c r="E51" s="76" t="n"/>
-      <c r="F51" s="77" t="inlineStr">
-        <is>
-          <t>ZENG XUELI</t>
-        </is>
-      </c>
-      <c r="G51" s="77" t="n"/>
-      <c r="L51" s="49" t="n"/>
-      <c r="M51" s="50" t="n"/>
-      <c r="N51" s="51" t="n"/>
-      <c r="O51" s="51" t="n"/>
+      <c r="D51" s="74" t="n"/>
+      <c r="E51" s="74" t="n"/>
+      <c r="F51" s="74" t="n"/>
+      <c r="G51" s="75" t="n"/>
     </row>
     <row r="52">
       <c r="D52" s="74" t="n"/>
@@ -3359,54 +3019,14 @@
       <c r="F55" s="74" t="n"/>
       <c r="G55" s="75" t="n"/>
     </row>
-    <row r="56">
-      <c r="D56" s="74" t="n"/>
-      <c r="E56" s="74" t="n"/>
-      <c r="F56" s="74" t="n"/>
-      <c r="G56" s="75" t="n"/>
-    </row>
-    <row r="57">
-      <c r="D57" s="74" t="n"/>
-      <c r="E57" s="74" t="n"/>
-      <c r="F57" s="74" t="n"/>
-      <c r="G57" s="75" t="n"/>
-    </row>
-    <row r="58">
-      <c r="D58" s="74" t="n"/>
-      <c r="E58" s="74" t="n"/>
-      <c r="F58" s="74" t="n"/>
-      <c r="G58" s="75" t="n"/>
-    </row>
-    <row r="59">
-      <c r="D59" s="74" t="n"/>
-      <c r="E59" s="74" t="n"/>
-      <c r="F59" s="74" t="n"/>
-      <c r="G59" s="75" t="n"/>
-    </row>
-    <row r="60">
-      <c r="D60" s="74" t="n"/>
-      <c r="E60" s="74" t="n"/>
-      <c r="F60" s="74" t="n"/>
-      <c r="G60" s="75" t="n"/>
-    </row>
-    <row r="61">
-      <c r="D61" s="74" t="n"/>
-      <c r="E61" s="74" t="n"/>
-      <c r="F61" s="74" t="n"/>
-      <c r="G61" s="75" t="n"/>
-    </row>
-    <row r="62">
-      <c r="D62" s="74" t="n"/>
-      <c r="E62" s="74" t="n"/>
-      <c r="F62" s="74" t="n"/>
-      <c r="G62" s="75" t="n"/>
-    </row>
-    <row r="63" ht="15" customHeight="1">
-      <c r="D63" s="74" t="n"/>
-      <c r="E63" s="74" t="n"/>
-      <c r="F63" s="74" t="n"/>
-      <c r="G63" s="75" t="n"/>
-    </row>
+    <row r="56"/>
+    <row r="57"/>
+    <row r="58"/>
+    <row r="59"/>
+    <row r="60"/>
+    <row r="61"/>
+    <row r="62"/>
+    <row r="63" ht="15" customHeight="1"/>
     <row r="64"/>
     <row r="65"/>
     <row r="66"/>
@@ -3546,18 +3166,18 @@
     <row r="200"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="B32"/>
+    <mergeCell ref="A36:C36"/>
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B40"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A45:G45"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A6:G6"/>
     <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="A38:G38"/>
     <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="B35:C35"/>
     <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A46:G46"/>
+    <mergeCell ref="A37:G37"/>
   </mergeCells>
   <conditionalFormatting sqref="J23:J35">
     <cfRule type="duplicateValues" priority="1" stopIfTrue="1"/>
@@ -3670,7 +3290,7 @@
       </c>
       <c r="I7" s="87" t="inlineStr">
         <is>
-          <t>CLF2025-171</t>
+          <t>JFREF</t>
         </is>
       </c>
     </row>
@@ -3694,7 +3314,7 @@
       </c>
       <c r="I8" s="85" t="inlineStr">
         <is>
-          <t>JF25030</t>
+          <t>JFINV</t>
         </is>
       </c>
     </row>
@@ -3712,8 +3332,10 @@
           <t>Date:</t>
         </is>
       </c>
-      <c r="I9" s="118" t="n">
-        <v>45819</v>
+      <c r="I9" s="88" t="inlineStr">
+        <is>
+          <t>JFTIME</t>
+        </is>
       </c>
     </row>
     <row r="10" ht="22.5" customHeight="1">
@@ -4903,38 +4525,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" ht="42" customHeight="1">
-      <c r="B55" s="133" t="inlineStr">
-        <is>
-          <t>TOTAL OF:</t>
-        </is>
-      </c>
-      <c r="D55" s="133" t="inlineStr">
-        <is>
-          <t>16 PALLETS</t>
-        </is>
-      </c>
-      <c r="E55" s="134">
-        <f>SUM(E23:E34,E40:E52)</f>
-        <v/>
-      </c>
-      <c r="F55" s="135">
-        <f>SUM(F23:F34,F40:F52)</f>
-        <v/>
-      </c>
-      <c r="G55" s="135">
-        <f>SUM(G23:G34,G40:G52)</f>
-        <v/>
-      </c>
-      <c r="H55" s="135">
-        <f>SUM(H23:H34,H40:H52)</f>
-        <v/>
-      </c>
-      <c r="I55" s="136">
-        <f>SUM(I23:I34,I40:I52)</f>
-        <v/>
-      </c>
-    </row>
+    <row r="55" ht="42" customHeight="1"/>
     <row r="56" ht="24" customHeight="1"/>
     <row r="57" ht="69.75" customHeight="1"/>
     <row r="58" ht="42" customHeight="1">
@@ -5290,10 +4881,9 @@
     <row r="199"/>
     <row r="200"/>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="29">
     <mergeCell ref="B60:D60"/>
     <mergeCell ref="H38:H39"/>
-    <mergeCell ref="B55"/>
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="H21:H22"/>
     <mergeCell ref="A3:I3"/>

</xml_diff>

<commit_message>
fixing grand footer height inconcistance
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -21,12 +21,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="[$-409]dd\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="#,##0.00;[Red]#,##0.00"/>
     <numFmt numFmtId="166" formatCode="###0;###0"/>
     <numFmt numFmtId="167" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="168" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="168" formatCode="##0.00"/>
+    <numFmt numFmtId="169" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="42">
     <font>
@@ -450,7 +451,7 @@
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
@@ -739,7 +740,7 @@
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="36" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="169" fontId="36" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="40" fillId="4" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -755,7 +756,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="4" fontId="38" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="168" fontId="38" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="35" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -763,7 +764,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -803,7 +804,37 @@
     <xf numFmtId="3" fontId="38" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="4" fontId="38" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="38" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="38" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="38" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="38" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="38" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="38" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="38" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="38" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1636,18 +1667,20 @@
       </c>
       <c r="B16" s="110" t="inlineStr">
         <is>
-          <t>01.10.U756033</t>
+          <t>01.10.U722233/01.10.U741023
+01.10.U756033/01.10.W653191
+01.10.W783049</t>
         </is>
       </c>
       <c r="C16" s="111" t="n">
-        <v>7681.5</v>
+        <v>72108.10000000001</v>
       </c>
       <c r="D16" s="111">
         <f>E16/C16</f>
         <v/>
       </c>
       <c r="E16" s="111" t="n">
-        <v>9572.751</v>
+        <v>97144.197</v>
       </c>
     </row>
     <row r="17" ht="30" customFormat="1" customHeight="1" s="36">
@@ -1656,346 +1689,195 @@
       </c>
       <c r="B17" s="110" t="inlineStr">
         <is>
-          <t>01.10.W653191</t>
+          <t>01.10.U528103/01.10.U528110
+01.10.U722233</t>
         </is>
       </c>
       <c r="C17" s="111" t="n">
-        <v>5748.5</v>
+        <v>58119</v>
       </c>
       <c r="D17" s="111">
         <f>E17/C17</f>
         <v/>
       </c>
       <c r="E17" s="111" t="n">
-        <v>7473.05</v>
-      </c>
-    </row>
-    <row r="18" ht="30" customFormat="1" customHeight="1" s="36">
-      <c r="A18" s="110" t="n">
-        <v>3</v>
-      </c>
-      <c r="B18" s="110" t="inlineStr">
-        <is>
-          <t>01.10.W783049</t>
-        </is>
-      </c>
-      <c r="C18" s="111" t="n">
-        <v>9376</v>
-      </c>
-      <c r="D18" s="111">
-        <f>E18/C18</f>
+        <v>73045.87700000001</v>
+      </c>
+    </row>
+    <row r="18" ht="36" customFormat="1" customHeight="1" s="36">
+      <c r="A18" s="112" t="inlineStr">
+        <is>
+          <t>TOTAL:</t>
+        </is>
+      </c>
+      <c r="B18" s="113" t="n"/>
+      <c r="C18" s="114">
+        <f>SUM(C16:C17)</f>
         <v/>
       </c>
-      <c r="E18" s="111" t="n">
-        <v>14140.885</v>
-      </c>
-    </row>
-    <row r="19" ht="30" customFormat="1" customHeight="1" s="36">
-      <c r="A19" s="110" t="n">
-        <v>4</v>
-      </c>
-      <c r="B19" s="110" t="inlineStr">
-        <is>
-          <t>01.10.W783049</t>
-        </is>
-      </c>
-      <c r="C19" s="111" t="n">
-        <v>10077.9</v>
-      </c>
-      <c r="D19" s="111">
-        <f>E19/C19</f>
+      <c r="D18" s="112" t="n"/>
+      <c r="E18" s="114">
+        <f>SUM(E16:E17)</f>
         <v/>
       </c>
-      <c r="E19" s="111" t="n">
-        <v>15217.629</v>
-      </c>
-    </row>
-    <row r="20" ht="30" customFormat="1" customHeight="1" s="36">
-      <c r="A20" s="110" t="n">
-        <v>5</v>
-      </c>
-      <c r="B20" s="110" t="inlineStr">
-        <is>
-          <t>01.10.U741023</t>
-        </is>
-      </c>
-      <c r="C20" s="111" t="n">
-        <v>19497.3</v>
-      </c>
-      <c r="D20" s="111">
-        <f>E20/C20</f>
-        <v/>
-      </c>
-      <c r="E20" s="111" t="n">
-        <v>25661.748</v>
-      </c>
-    </row>
-    <row r="21" ht="30" customFormat="1" customHeight="1" s="36">
-      <c r="A21" s="110" t="n">
-        <v>6</v>
-      </c>
-      <c r="B21" s="110" t="inlineStr">
-        <is>
-          <t>01.10.U741023</t>
-        </is>
-      </c>
-      <c r="C21" s="111" t="n">
-        <v>9892.700000000001</v>
-      </c>
-      <c r="D21" s="111">
-        <f>E21/C21</f>
-        <v/>
-      </c>
-      <c r="E21" s="111" t="n">
-        <v>13058.364</v>
-      </c>
-    </row>
-    <row r="22" ht="30" customFormat="1" customHeight="1" s="36">
-      <c r="A22" s="110" t="n">
-        <v>7</v>
-      </c>
-      <c r="B22" s="110" t="inlineStr">
-        <is>
-          <t>01.10.U722233</t>
-        </is>
-      </c>
-      <c r="C22" s="111" t="n">
-        <v>9834.200000000001</v>
-      </c>
-      <c r="D22" s="111">
-        <f>E22/C22</f>
-        <v/>
-      </c>
-      <c r="E22" s="111" t="n">
-        <v>12019.77</v>
-      </c>
-    </row>
-    <row r="23" ht="30" customFormat="1" customHeight="1" s="36">
-      <c r="A23" s="110" t="n">
-        <v>8</v>
-      </c>
-      <c r="B23" s="110" t="inlineStr">
-        <is>
-          <t>01.10.U722233</t>
-        </is>
-      </c>
-      <c r="C23" s="111" t="n">
-        <v>9321.200000000001</v>
-      </c>
-      <c r="D23" s="111">
-        <f>E23/C23</f>
-        <v/>
-      </c>
-      <c r="E23" s="111" t="n">
-        <v>11420.616</v>
-      </c>
-    </row>
-    <row r="24" ht="30" customFormat="1" customHeight="1" s="36">
-      <c r="A24" s="110" t="n">
-        <v>9</v>
-      </c>
-      <c r="B24" s="110" t="inlineStr">
-        <is>
-          <t>01.10.U528110</t>
-        </is>
-      </c>
-      <c r="C24" s="111" t="n">
-        <v>26732.7</v>
-      </c>
-      <c r="D24" s="111">
-        <f>E24/C24</f>
-        <v/>
-      </c>
-      <c r="E24" s="111" t="n">
-        <v>33799.365</v>
-      </c>
-    </row>
-    <row r="25" ht="30" customFormat="1" customHeight="1" s="36">
-      <c r="A25" s="110" t="n">
-        <v>10</v>
-      </c>
-      <c r="B25" s="110" t="inlineStr">
-        <is>
-          <t>01.10.U528103</t>
-        </is>
-      </c>
-      <c r="C25" s="111" t="n">
-        <v>22065.1</v>
-      </c>
-      <c r="D25" s="111">
-        <f>E25/C25</f>
-        <v/>
-      </c>
-      <c r="E25" s="111" t="n">
-        <v>27825.896</v>
-      </c>
-    </row>
-    <row r="26" ht="36" customFormat="1" customHeight="1" s="37">
-      <c r="A26" s="112" t="inlineStr">
-        <is>
-          <t>TOTAL:</t>
-        </is>
-      </c>
-      <c r="B26" s="113" t="n"/>
-      <c r="C26" s="114">
-        <f>SUM(C16:C25)</f>
-        <v/>
-      </c>
-      <c r="D26" s="112" t="n"/>
-      <c r="E26" s="114">
-        <f>SUM(E16:E25)</f>
-        <v/>
+    </row>
+    <row r="19" ht="29.1" customFormat="1" customHeight="1" s="36">
+      <c r="A19" s="94" t="n"/>
+      <c r="C19" s="115" t="n"/>
+      <c r="D19" s="115" t="n"/>
+      <c r="E19" s="115" t="n"/>
+    </row>
+    <row r="20" ht="29.1" customFormat="1" customHeight="1" s="36">
+      <c r="A20" s="45" t="inlineStr">
+        <is>
+          <t>FOB:</t>
+        </is>
+      </c>
+      <c r="B20" s="46" t="inlineStr">
+        <is>
+          <t>BAVET</t>
+        </is>
+      </c>
+      <c r="C20" s="41" t="n"/>
+      <c r="D20" s="41" t="n"/>
+      <c r="E20" s="41" t="n"/>
+    </row>
+    <row r="21" ht="45.95" customFormat="1" customHeight="1" s="36">
+      <c r="A21" s="41" t="inlineStr">
+        <is>
+          <t>Term of Payment: 100% TT after shipment</t>
+        </is>
+      </c>
+      <c r="B21" s="41" t="n"/>
+      <c r="C21" s="41" t="n"/>
+      <c r="D21" s="41" t="n"/>
+      <c r="E21" s="41" t="n"/>
+    </row>
+    <row r="22" ht="41.1" customFormat="1" customHeight="1" s="36">
+      <c r="A22" s="41" t="inlineStr">
+        <is>
+          <t>Transaction method: FOB(USD)</t>
+        </is>
+      </c>
+      <c r="B22" s="41" t="n"/>
+      <c r="C22" s="41" t="n"/>
+      <c r="D22" s="41" t="n"/>
+      <c r="E22" s="41" t="n"/>
+    </row>
+    <row r="23" ht="29.1" customFormat="1" customHeight="1" s="36">
+      <c r="A23" s="41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beneficiary bank information: </t>
+        </is>
+      </c>
+      <c r="B23" s="41" t="n"/>
+      <c r="C23" s="41" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO.,LTD.</t>
+        </is>
+      </c>
+      <c r="D23" s="41" t="n"/>
+      <c r="E23" s="41" t="n"/>
+    </row>
+    <row r="24" ht="45.95" customFormat="1" customHeight="1" s="36">
+      <c r="A24" s="41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beneficiary Bank' s Name: </t>
+        </is>
+      </c>
+      <c r="B24" s="41" t="n"/>
+      <c r="C24" s="91" t="inlineStr">
+        <is>
+          <t>BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
+ /BANK OF CHINA PHNOM PENH BRANCH</t>
+        </is>
+      </c>
+    </row>
+    <row r="25" ht="41.1" customFormat="1" customHeight="1" s="36">
+      <c r="A25" s="41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bank Address:  </t>
+        </is>
+      </c>
+      <c r="B25" s="41" t="n"/>
+      <c r="C25" s="91" t="inlineStr">
+        <is>
+          <t>1st AND 2nd FLOOR,CANADIA TOWER,No.315 ANDDUONG ST.
+PHNOM PEMH,CAMBODIA.</t>
+        </is>
+      </c>
+    </row>
+    <row r="26" ht="29.1" customFormat="1" customHeight="1" s="37">
+      <c r="A26" s="41" t="inlineStr">
+        <is>
+          <t>Bank account :</t>
+        </is>
+      </c>
+      <c r="B26" s="41" t="n"/>
+      <c r="C26" s="92" t="inlineStr">
+        <is>
+          <t>100001100764430</t>
+        </is>
       </c>
     </row>
     <row r="27" ht="57" customFormat="1" customHeight="1" s="37">
-      <c r="A27" s="94" t="n"/>
-      <c r="C27" s="115" t="n"/>
-      <c r="D27" s="115" t="n"/>
-      <c r="E27" s="115" t="n"/>
+      <c r="A27" s="41" t="inlineStr">
+        <is>
+          <t>SWIFT CODE  ：</t>
+        </is>
+      </c>
+      <c r="B27" s="41" t="n"/>
+      <c r="C27" s="41" t="inlineStr">
+        <is>
+          <t>BKCHKHPPXXX</t>
+        </is>
+      </c>
+      <c r="D27" s="41" t="n"/>
+      <c r="E27" s="41" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" s="45" t="inlineStr">
-        <is>
-          <t>FCA:</t>
-        </is>
-      </c>
-      <c r="B28" s="46" t="inlineStr">
-        <is>
-          <t>BAVET, SVAY RIENG</t>
-        </is>
-      </c>
+      <c r="A28" s="41" t="n"/>
+      <c r="B28" s="41" t="n"/>
       <c r="C28" s="41" t="n"/>
       <c r="D28" s="41" t="n"/>
       <c r="E28" s="41" t="n"/>
+      <c r="F28" s="41" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" s="41" t="inlineStr">
-        <is>
-          <t>Term of Payment: 100% TT after shipment</t>
-        </is>
-      </c>
-      <c r="B29" s="41" t="n"/>
-      <c r="C29" s="41" t="n"/>
-      <c r="D29" s="41" t="n"/>
-      <c r="E29" s="41" t="n"/>
+      <c r="A29" s="37" t="inlineStr">
+        <is>
+          <t>The Buyer:</t>
+        </is>
+      </c>
+      <c r="D29" s="47" t="inlineStr">
+        <is>
+          <t>The Seller:</t>
+        </is>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" s="41" t="inlineStr">
-        <is>
-          <t>Transaction method: FCA(USD)</t>
-        </is>
-      </c>
-      <c r="B30" s="41" t="n"/>
-      <c r="C30" s="41" t="n"/>
-      <c r="D30" s="41" t="n"/>
-      <c r="E30" s="41" t="n"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="41" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Beneficiary bank information: </t>
-        </is>
-      </c>
-      <c r="B31" s="41" t="n"/>
-      <c r="C31" s="41" t="inlineStr">
+      <c r="A30" s="73" t="inlineStr">
+        <is>
+          <t>JASON FURNITURE VIET NAM COMPANY LIMITED</t>
+        </is>
+      </c>
+      <c r="B30" s="72" t="n"/>
+      <c r="C30" s="48" t="n"/>
+      <c r="D30" s="73" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO.,LTD.</t>
         </is>
       </c>
-      <c r="D31" s="41" t="n"/>
-      <c r="E31" s="41" t="n"/>
-    </row>
-    <row r="32" ht="45.95" customHeight="1">
-      <c r="A32" s="41" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Beneficiary Bank' s Name: </t>
-        </is>
-      </c>
-      <c r="B32" s="41" t="n"/>
-      <c r="C32" s="91" t="inlineStr">
-        <is>
-          <t>BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
- /BANK OF CHINA PHNOM PENH BRANCH</t>
-        </is>
-      </c>
-    </row>
-    <row r="33" ht="41.1" customHeight="1">
-      <c r="A33" s="41" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Bank Address:  </t>
-        </is>
-      </c>
-      <c r="B33" s="41" t="n"/>
-      <c r="C33" s="91" t="inlineStr">
-        <is>
-          <t>1st AND 2nd FLOOR,CANADIA TOWER,No.315 ANDDUONG ST.
-PHNOM PEMH,CAMBODIA.</t>
-        </is>
-      </c>
-    </row>
-    <row r="34" ht="29.1" customHeight="1">
-      <c r="A34" s="41" t="inlineStr">
-        <is>
-          <t>Bank account :</t>
-        </is>
-      </c>
-      <c r="B34" s="41" t="n"/>
-      <c r="C34" s="92" t="inlineStr">
-        <is>
-          <t>100001100764430</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="41" t="inlineStr">
-        <is>
-          <t>SWIFT CODE  ：</t>
-        </is>
-      </c>
-      <c r="B35" s="41" t="n"/>
-      <c r="C35" s="41" t="inlineStr">
-        <is>
-          <t>BKCHKHPPXXX</t>
-        </is>
-      </c>
-      <c r="D35" s="41" t="n"/>
-      <c r="E35" s="41" t="n"/>
-    </row>
-    <row r="36">
-      <c r="A36" s="41" t="n"/>
-      <c r="B36" s="41" t="n"/>
-      <c r="C36" s="41" t="n"/>
-      <c r="D36" s="41" t="n"/>
-      <c r="E36" s="41" t="n"/>
-      <c r="F36" s="41" t="n"/>
-    </row>
-    <row r="37">
-      <c r="A37" s="37" t="inlineStr">
-        <is>
-          <t>The Buyer:</t>
-        </is>
-      </c>
-      <c r="D37" s="47" t="inlineStr">
-        <is>
-          <t>The Seller:</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="73" t="inlineStr">
-        <is>
-          <t>JASON FURNITURE VIET NAM COMPANY LIMITED</t>
-        </is>
-      </c>
-      <c r="B38" s="72" t="n"/>
-      <c r="C38" s="48" t="n"/>
-      <c r="D38" s="73" t="inlineStr">
-        <is>
-          <t>CALIFOR UPHOLSTERY MATERIALS CO.,LTD.</t>
-        </is>
-      </c>
-      <c r="E38" s="73" t="n"/>
-    </row>
+      <c r="E30" s="73" t="n"/>
+    </row>
+    <row r="31"/>
+    <row r="32"/>
+    <row r="33"/>
+    <row r="34"/>
+    <row r="35"/>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="38"/>
     <row r="39"/>
     <row r="40"/>
     <row r="41"/>
@@ -2159,17 +2041,20 @@
     <row r="199"/>
     <row r="200" ht="27.95" customHeight="1"/>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C33:E33"/>
+  <mergeCells count="14">
+    <mergeCell ref="C24:E24"/>
     <mergeCell ref="A12:D12"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C22:E22"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="B11:E11"/>
+    <mergeCell ref="C26:E26"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A14:E14"/>
+    <mergeCell ref="C21:E21"/>
     <mergeCell ref="B10:E10"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C25:E25"/>
     <mergeCell ref="A200:B200"/>
   </mergeCells>
   <pageMargins left="0.432638888888889" right="0.314583333333333" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2325,7 +2210,7 @@
       <c r="E10" s="4" t="n"/>
       <c r="F10" s="9" t="inlineStr">
         <is>
-          <t>FCA :</t>
+          <t>FOB :</t>
         </is>
       </c>
       <c r="G10" s="106" t="inlineStr">
@@ -2491,12 +2376,16 @@
       </c>
       <c r="B22" s="121" t="inlineStr">
         <is>
-          <t>9000619872</t>
+          <t>9000606101/9000619872
+9000678466/9000691966
+9000707953/9000719487</t>
         </is>
       </c>
       <c r="C22" s="121" t="inlineStr">
         <is>
-          <t>01.10.U756033</t>
+          <t>01.10.U722233/01.10.U741023
+01.10.U756033/01.10.W653191
+01.10.W783049</t>
         </is>
       </c>
       <c r="D22" s="122" t="inlineStr">
@@ -2505,14 +2394,14 @@
         </is>
       </c>
       <c r="E22" s="123" t="n">
-        <v>7681.5</v>
+        <v>72108.10000000001</v>
       </c>
       <c r="F22" s="123">
         <f>G22/E22</f>
         <v/>
       </c>
       <c r="G22" s="123" t="n">
-        <v>9572.751</v>
+        <v>97144.197</v>
       </c>
     </row>
     <row r="23" ht="35" customHeight="1">
@@ -2523,28 +2412,29 @@
       </c>
       <c r="B23" s="121" t="inlineStr">
         <is>
-          <t>9000691966</t>
+          <t>9000707052/9000719487</t>
         </is>
       </c>
       <c r="C23" s="121" t="inlineStr">
         <is>
-          <t>01.10.W653191</t>
+          <t>01.10.U528103/01.10.U528110
+01.10.U722233</t>
         </is>
       </c>
       <c r="D23" s="122" t="inlineStr">
         <is>
-          <t>BUFFALO HIDE</t>
+          <t>cow lol</t>
         </is>
       </c>
       <c r="E23" s="123" t="n">
-        <v>5748.5</v>
+        <v>58119</v>
       </c>
       <c r="F23" s="123">
         <f>G23/E23</f>
         <v/>
       </c>
       <c r="G23" s="123" t="n">
-        <v>7473.05</v>
+        <v>73045.87700000001</v>
       </c>
     </row>
     <row r="24" ht="35" customHeight="1">
@@ -2553,399 +2443,222 @@
           <t>MADE IN CAMBODIA</t>
         </is>
       </c>
-      <c r="B24" s="121" t="inlineStr">
-        <is>
-          <t>9000606101</t>
-        </is>
-      </c>
-      <c r="C24" s="121" t="inlineStr">
-        <is>
-          <t>01.10.W783049</t>
-        </is>
-      </c>
-      <c r="D24" s="122" t="inlineStr">
-        <is>
-          <t>BUFFALO HIDE</t>
-        </is>
-      </c>
-      <c r="E24" s="123" t="n">
-        <v>9376</v>
-      </c>
-      <c r="F24" s="123">
-        <f>G24/E24</f>
+      <c r="B24" s="121" t="n"/>
+      <c r="C24" s="121" t="n"/>
+      <c r="D24" s="122" t="n"/>
+      <c r="E24" s="123" t="n"/>
+      <c r="F24" s="123" t="n"/>
+      <c r="G24" s="123" t="n"/>
+    </row>
+    <row r="25" ht="35" customHeight="1">
+      <c r="A25" s="112" t="n"/>
+      <c r="B25" s="112" t="inlineStr">
+        <is>
+          <t>TOTAL:</t>
+        </is>
+      </c>
+      <c r="C25" s="112" t="n"/>
+      <c r="D25" s="112" t="inlineStr">
+        <is>
+          <t>16 PALLETS</t>
+        </is>
+      </c>
+      <c r="E25" s="114">
+        <f>SUM(E22:E24)</f>
         <v/>
       </c>
-      <c r="G24" s="123" t="n">
-        <v>14140.885</v>
-      </c>
-    </row>
-    <row r="25" ht="35" customHeight="1">
-      <c r="A25" s="124" t="n"/>
-      <c r="B25" s="121" t="inlineStr">
-        <is>
-          <t>9000678466</t>
-        </is>
-      </c>
-      <c r="C25" s="121" t="inlineStr">
-        <is>
-          <t>01.10.W783049</t>
-        </is>
-      </c>
-      <c r="D25" s="122" t="inlineStr">
-        <is>
-          <t>BUFFALO HIDE</t>
-        </is>
-      </c>
-      <c r="E25" s="123" t="n">
-        <v>10077.9</v>
-      </c>
-      <c r="F25" s="123">
-        <f>G25/E25</f>
+      <c r="F25" s="112" t="n"/>
+      <c r="G25" s="114">
+        <f>SUM(G22:G24)</f>
         <v/>
       </c>
-      <c r="G25" s="123" t="n">
-        <v>15217.629</v>
-      </c>
-    </row>
-    <row r="26" ht="35" customHeight="1">
-      <c r="A26" s="124" t="n"/>
-      <c r="B26" s="121" t="inlineStr">
-        <is>
-          <t>9000707953</t>
-        </is>
-      </c>
-      <c r="C26" s="121" t="inlineStr">
-        <is>
-          <t>01.10.U741023</t>
-        </is>
-      </c>
-      <c r="D26" s="122" t="inlineStr">
-        <is>
-          <t>BUFFALO HIDE</t>
-        </is>
-      </c>
-      <c r="E26" s="123" t="n">
-        <v>19497.3</v>
-      </c>
-      <c r="F26" s="123">
-        <f>G26/E26</f>
-        <v/>
-      </c>
-      <c r="G26" s="123" t="n">
-        <v>25661.748</v>
-      </c>
-    </row>
-    <row r="27" ht="35" customFormat="1" customHeight="1" s="1">
-      <c r="A27" s="124" t="n"/>
-      <c r="B27" s="121" t="inlineStr">
-        <is>
-          <t>9000719487</t>
-        </is>
-      </c>
-      <c r="C27" s="121" t="inlineStr">
-        <is>
-          <t>01.10.U741023</t>
-        </is>
-      </c>
-      <c r="D27" s="122" t="inlineStr">
-        <is>
-          <t>BUFFALO HIDE</t>
-        </is>
-      </c>
-      <c r="E27" s="123" t="n">
-        <v>9892.700000000001</v>
-      </c>
-      <c r="F27" s="123">
-        <f>G27/E27</f>
-        <v/>
-      </c>
-      <c r="G27" s="123" t="n">
-        <v>13058.364</v>
-      </c>
-    </row>
-    <row r="28" ht="35" customHeight="1">
-      <c r="A28" s="124" t="n"/>
-      <c r="B28" s="121" t="inlineStr">
-        <is>
-          <t>9000719487</t>
-        </is>
-      </c>
-      <c r="C28" s="121" t="inlineStr">
-        <is>
-          <t>01.10.U722233</t>
-        </is>
-      </c>
-      <c r="D28" s="122" t="inlineStr">
-        <is>
-          <t>BUFFALO HIDE</t>
-        </is>
-      </c>
-      <c r="E28" s="123" t="n">
-        <v>9834.200000000001</v>
-      </c>
-      <c r="F28" s="123">
-        <f>G28/E28</f>
-        <v/>
-      </c>
-      <c r="G28" s="123" t="n">
-        <v>12019.77</v>
-      </c>
-    </row>
-    <row r="29" ht="35" customHeight="1">
-      <c r="A29" s="124" t="n"/>
-      <c r="B29" s="121" t="inlineStr">
-        <is>
-          <t>9000719487</t>
-        </is>
-      </c>
-      <c r="C29" s="121" t="inlineStr">
-        <is>
-          <t>01.10.U722233</t>
-        </is>
-      </c>
-      <c r="D29" s="122" t="inlineStr">
-        <is>
-          <t>cow lol</t>
-        </is>
-      </c>
-      <c r="E29" s="123" t="n">
-        <v>9321.200000000001</v>
-      </c>
-      <c r="F29" s="123">
-        <f>G29/E29</f>
-        <v/>
-      </c>
-      <c r="G29" s="123" t="n">
-        <v>11420.616</v>
-      </c>
-    </row>
-    <row r="30" ht="35" customHeight="1">
-      <c r="A30" s="124" t="n"/>
-      <c r="B30" s="121" t="inlineStr">
-        <is>
-          <t>9000707052</t>
-        </is>
-      </c>
-      <c r="C30" s="121" t="inlineStr">
-        <is>
-          <t>01.10.U528110</t>
-        </is>
-      </c>
-      <c r="D30" s="122" t="inlineStr">
-        <is>
-          <t>cow lol</t>
-        </is>
-      </c>
-      <c r="E30" s="123" t="n">
-        <v>26732.7</v>
-      </c>
-      <c r="F30" s="123">
-        <f>G30/E30</f>
-        <v/>
-      </c>
-      <c r="G30" s="123" t="n">
-        <v>33799.365</v>
-      </c>
-    </row>
-    <row r="31" ht="35" customHeight="1">
-      <c r="A31" s="124" t="n"/>
-      <c r="B31" s="121" t="inlineStr">
-        <is>
-          <t>9000707052</t>
-        </is>
-      </c>
-      <c r="C31" s="121" t="inlineStr">
-        <is>
-          <t>01.10.U528103</t>
-        </is>
-      </c>
-      <c r="D31" s="122" t="inlineStr">
-        <is>
-          <t>cow lol</t>
-        </is>
-      </c>
-      <c r="E31" s="123" t="n">
-        <v>22065.1</v>
-      </c>
-      <c r="F31" s="123">
-        <f>G31/E31</f>
-        <v/>
-      </c>
-      <c r="G31" s="123" t="n">
-        <v>27825.896</v>
-      </c>
-    </row>
-    <row r="32" ht="35" customHeight="1">
-      <c r="A32" s="112" t="n"/>
-      <c r="B32" s="112" t="inlineStr">
-        <is>
-          <t>TOTAL:</t>
-        </is>
-      </c>
-      <c r="C32" s="112" t="n"/>
-      <c r="D32" s="112" t="inlineStr">
-        <is>
-          <t>16 PALLETS</t>
-        </is>
-      </c>
-      <c r="E32" s="114">
-        <f>SUM(E22:E31)</f>
-        <v/>
-      </c>
-      <c r="F32" s="112" t="n"/>
-      <c r="G32" s="114">
-        <f>SUM(G22:G31)</f>
-        <v/>
-      </c>
+    </row>
+    <row r="26" ht="24.75" customHeight="1">
+      <c r="A26" s="21" t="n"/>
+      <c r="B26" s="21" t="n"/>
+      <c r="C26" s="22" t="n"/>
+      <c r="D26" s="22" t="n"/>
+      <c r="E26" s="22" t="n"/>
+      <c r="F26" s="22" t="n"/>
+      <c r="G26" s="18" t="n"/>
+      <c r="L26" s="49" t="n"/>
+      <c r="M26" s="50" t="n"/>
+      <c r="N26" s="51" t="n"/>
+      <c r="O26" s="51" t="n"/>
+    </row>
+    <row r="27" ht="42" customFormat="1" customHeight="1" s="1">
+      <c r="A27" s="101" t="inlineStr">
+        <is>
+          <t>Country of Original Cambodia</t>
+        </is>
+      </c>
+      <c r="L27" s="49" t="n"/>
+      <c r="M27" s="50" t="n"/>
+      <c r="N27" s="51" t="n"/>
+      <c r="O27" s="51" t="n"/>
+    </row>
+    <row r="28" ht="61.5" customHeight="1">
+      <c r="A28" s="28" t="inlineStr">
+        <is>
+          <t>Manufacture:</t>
+        </is>
+      </c>
+      <c r="B28" s="102" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
+XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
+        </is>
+      </c>
+      <c r="D28" s="102" t="n"/>
+      <c r="E28" s="102" t="n"/>
+      <c r="F28" s="4" t="n"/>
+      <c r="G28" s="96" t="n"/>
+      <c r="L28" s="49" t="n"/>
+      <c r="M28" s="50" t="n"/>
+      <c r="N28" s="51" t="n"/>
+      <c r="O28" s="51" t="n"/>
+    </row>
+    <row r="29" ht="42" customHeight="1">
+      <c r="A29" s="103" t="inlineStr">
+        <is>
+          <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
+                                                  /BANK OF CHINA PHNOM PENH BRANCH</t>
+        </is>
+      </c>
+      <c r="D29" s="103" t="n"/>
+      <c r="E29" s="103" t="n"/>
+      <c r="F29" s="103" t="n"/>
+      <c r="G29" s="96" t="n"/>
+      <c r="L29" s="49" t="n"/>
+      <c r="M29" s="50" t="n"/>
+      <c r="N29" s="51" t="n"/>
+      <c r="O29" s="51" t="n"/>
+    </row>
+    <row r="30" ht="24.75" customHeight="1">
+      <c r="A30" s="99" t="inlineStr">
+        <is>
+          <t>A/C NO:100001100764430</t>
+        </is>
+      </c>
+      <c r="L30" s="49" t="n"/>
+      <c r="M30" s="50" t="n"/>
+      <c r="N30" s="51" t="n"/>
+      <c r="O30" s="51" t="n"/>
+    </row>
+    <row r="31" ht="27" customHeight="1">
+      <c r="A31" s="99" t="inlineStr">
+        <is>
+          <t>SWIFT CODE  ：BKCHKHPPXXX</t>
+        </is>
+      </c>
+      <c r="L31" s="49" t="n"/>
+      <c r="M31" s="50" t="n"/>
+      <c r="N31" s="51" t="n"/>
+      <c r="O31" s="51" t="n"/>
+    </row>
+    <row r="32" ht="53.1" customHeight="1">
+      <c r="E32" s="81" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
+        </is>
+      </c>
+      <c r="F32" s="81" t="n"/>
+      <c r="G32" s="81" t="n"/>
+      <c r="H32" s="81" t="n"/>
+      <c r="L32" s="49" t="n"/>
+      <c r="M32" s="50" t="n"/>
+      <c r="N32" s="51" t="n"/>
+      <c r="O32" s="51" t="n"/>
     </row>
     <row r="33" ht="27.75" customHeight="1">
-      <c r="A33" s="21" t="n"/>
-      <c r="B33" s="21" t="n"/>
-      <c r="C33" s="22" t="n"/>
-      <c r="D33" s="22" t="n"/>
-      <c r="E33" s="22" t="n"/>
-      <c r="F33" s="22" t="n"/>
-      <c r="G33" s="18" t="n"/>
+      <c r="D33" s="78" t="n"/>
+      <c r="E33" s="76" t="n"/>
+      <c r="F33" s="79" t="inlineStr">
+        <is>
+          <t>Sign &amp; Stamp</t>
+        </is>
+      </c>
+      <c r="G33" s="80" t="n"/>
       <c r="L33" s="49" t="n"/>
       <c r="M33" s="50" t="n"/>
       <c r="N33" s="51" t="n"/>
       <c r="O33" s="51" t="n"/>
     </row>
-    <row r="34" ht="42" customHeight="1">
-      <c r="A34" s="101" t="inlineStr">
-        <is>
-          <t>Country of Original Cambodia</t>
-        </is>
-      </c>
-      <c r="D34" s="101" t="n"/>
-      <c r="E34" s="4" t="n"/>
-      <c r="F34" s="33" t="n"/>
-      <c r="G34" s="96" t="n"/>
+    <row r="34" ht="27.75" customHeight="1">
+      <c r="D34" s="78" t="n"/>
+      <c r="E34" s="76" t="n"/>
+      <c r="F34" s="76" t="n"/>
+      <c r="G34" s="80" t="n"/>
       <c r="L34" s="49" t="n"/>
       <c r="M34" s="50" t="n"/>
       <c r="N34" s="51" t="n"/>
       <c r="O34" s="51" t="n"/>
     </row>
-    <row r="35" ht="61.5" customHeight="1">
-      <c r="A35" s="28" t="inlineStr">
-        <is>
-          <t>Manufacture:</t>
-        </is>
-      </c>
-      <c r="B35" s="102" t="inlineStr">
-        <is>
-          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
-XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
-        </is>
-      </c>
-      <c r="D35" s="102" t="n"/>
-      <c r="E35" s="102" t="n"/>
-      <c r="F35" s="4" t="n"/>
-      <c r="G35" s="96" t="n"/>
+    <row r="35" ht="27.75" customHeight="1">
+      <c r="D35" s="78" t="n"/>
+      <c r="E35" s="76" t="n"/>
+      <c r="F35" s="76" t="n"/>
+      <c r="G35" s="80" t="n"/>
       <c r="L35" s="49" t="n"/>
       <c r="M35" s="50" t="n"/>
       <c r="N35" s="51" t="n"/>
       <c r="O35" s="51" t="n"/>
     </row>
-    <row r="36" ht="42" customHeight="1">
-      <c r="A36" s="103" t="inlineStr">
-        <is>
-          <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
-                                                  /BANK OF CHINA PHNOM PENH BRANCH</t>
-        </is>
-      </c>
-      <c r="D36" s="103" t="n"/>
-      <c r="E36" s="103" t="n"/>
-      <c r="F36" s="103" t="n"/>
-      <c r="G36" s="96" t="n"/>
+    <row r="36" ht="24.75" customHeight="1">
+      <c r="D36" s="78" t="n"/>
+      <c r="E36" s="76" t="n"/>
+      <c r="F36" s="77" t="inlineStr">
+        <is>
+          <t>ZENG XUELI</t>
+        </is>
+      </c>
+      <c r="G36" s="77" t="n"/>
       <c r="L36" s="49" t="n"/>
       <c r="M36" s="50" t="n"/>
       <c r="N36" s="51" t="n"/>
       <c r="O36" s="51" t="n"/>
     </row>
-    <row r="37" ht="24.75" customHeight="1">
-      <c r="A37" s="99" t="inlineStr">
-        <is>
-          <t>A/C NO:100001100764430</t>
-        </is>
-      </c>
-      <c r="L37" s="49" t="n"/>
-      <c r="M37" s="50" t="n"/>
-      <c r="N37" s="51" t="n"/>
-      <c r="O37" s="51" t="n"/>
-    </row>
-    <row r="38" ht="27" customHeight="1">
-      <c r="A38" s="99" t="inlineStr">
-        <is>
-          <t>SWIFT CODE  ：BKCHKHPPXXX</t>
-        </is>
-      </c>
-      <c r="L38" s="49" t="n"/>
-      <c r="M38" s="50" t="n"/>
-      <c r="N38" s="51" t="n"/>
-      <c r="O38" s="51" t="n"/>
+    <row r="37" ht="21" customHeight="1">
+      <c r="D37" s="74" t="n"/>
+      <c r="E37" s="74" t="n"/>
+      <c r="F37" s="74" t="n"/>
+      <c r="G37" s="75" t="n"/>
+    </row>
+    <row r="38" ht="21" customHeight="1">
+      <c r="D38" s="74" t="n"/>
+      <c r="E38" s="74" t="n"/>
+      <c r="F38" s="74" t="n"/>
+      <c r="G38" s="75" t="n"/>
     </row>
     <row r="39" ht="21" customHeight="1">
-      <c r="E39" s="81" t="inlineStr">
-        <is>
-          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
-        </is>
-      </c>
-      <c r="F39" s="81" t="n"/>
-      <c r="G39" s="81" t="n"/>
-      <c r="H39" s="81" t="n"/>
-      <c r="L39" s="49" t="n"/>
-      <c r="M39" s="50" t="n"/>
-      <c r="N39" s="51" t="n"/>
-      <c r="O39" s="51" t="n"/>
+      <c r="D39" s="74" t="n"/>
+      <c r="E39" s="74" t="n"/>
+      <c r="F39" s="74" t="n"/>
+      <c r="G39" s="75" t="n"/>
     </row>
     <row r="40" ht="21" customHeight="1">
-      <c r="D40" s="78" t="n"/>
-      <c r="E40" s="76" t="n"/>
-      <c r="F40" s="79" t="inlineStr">
-        <is>
-          <t>Sign &amp; Stamp</t>
-        </is>
-      </c>
-      <c r="G40" s="80" t="n"/>
-      <c r="L40" s="49" t="n"/>
-      <c r="M40" s="50" t="n"/>
-      <c r="N40" s="51" t="n"/>
-      <c r="O40" s="51" t="n"/>
+      <c r="D40" s="74" t="n"/>
+      <c r="E40" s="74" t="n"/>
+      <c r="F40" s="74" t="n"/>
+      <c r="G40" s="75" t="n"/>
     </row>
     <row r="41" ht="21" customHeight="1">
-      <c r="D41" s="78" t="n"/>
-      <c r="E41" s="76" t="n"/>
-      <c r="F41" s="76" t="n"/>
-      <c r="G41" s="80" t="n"/>
-      <c r="L41" s="49" t="n"/>
-      <c r="M41" s="50" t="n"/>
-      <c r="N41" s="51" t="n"/>
-      <c r="O41" s="51" t="n"/>
+      <c r="D41" s="74" t="n"/>
+      <c r="E41" s="74" t="n"/>
+      <c r="F41" s="74" t="n"/>
+      <c r="G41" s="75" t="n"/>
     </row>
     <row r="42" ht="21" customHeight="1">
-      <c r="D42" s="78" t="n"/>
-      <c r="E42" s="76" t="n"/>
-      <c r="F42" s="76" t="n"/>
-      <c r="G42" s="80" t="n"/>
-      <c r="L42" s="49" t="n"/>
-      <c r="M42" s="50" t="n"/>
-      <c r="N42" s="51" t="n"/>
-      <c r="O42" s="51" t="n"/>
+      <c r="D42" s="74" t="n"/>
+      <c r="E42" s="74" t="n"/>
+      <c r="F42" s="74" t="n"/>
+      <c r="G42" s="75" t="n"/>
     </row>
     <row r="43" ht="21" customHeight="1">
-      <c r="D43" s="78" t="n"/>
-      <c r="E43" s="76" t="n"/>
-      <c r="F43" s="77" t="inlineStr">
-        <is>
-          <t>ZENG XUELI</t>
-        </is>
-      </c>
-      <c r="G43" s="77" t="n"/>
-      <c r="L43" s="49" t="n"/>
-      <c r="M43" s="50" t="n"/>
-      <c r="N43" s="51" t="n"/>
-      <c r="O43" s="51" t="n"/>
+      <c r="D43" s="74" t="n"/>
+      <c r="E43" s="74" t="n"/>
+      <c r="F43" s="74" t="n"/>
+      <c r="G43" s="75" t="n"/>
     </row>
     <row r="44" ht="21" customHeight="1">
       <c r="D44" s="74" t="n"/>
@@ -2977,48 +2690,13 @@
       <c r="F48" s="74" t="n"/>
       <c r="G48" s="75" t="n"/>
     </row>
-    <row r="49" ht="21" customHeight="1">
-      <c r="D49" s="74" t="n"/>
-      <c r="E49" s="74" t="n"/>
-      <c r="F49" s="74" t="n"/>
-      <c r="G49" s="75" t="n"/>
-    </row>
-    <row r="50" ht="21" customHeight="1">
-      <c r="D50" s="74" t="n"/>
-      <c r="E50" s="74" t="n"/>
-      <c r="F50" s="74" t="n"/>
-      <c r="G50" s="75" t="n"/>
-    </row>
-    <row r="51" ht="17.25" customHeight="1">
-      <c r="D51" s="74" t="n"/>
-      <c r="E51" s="74" t="n"/>
-      <c r="F51" s="74" t="n"/>
-      <c r="G51" s="75" t="n"/>
-    </row>
-    <row r="52">
-      <c r="D52" s="74" t="n"/>
-      <c r="E52" s="74" t="n"/>
-      <c r="F52" s="74" t="n"/>
-      <c r="G52" s="75" t="n"/>
-    </row>
-    <row r="53">
-      <c r="D53" s="74" t="n"/>
-      <c r="E53" s="74" t="n"/>
-      <c r="F53" s="74" t="n"/>
-      <c r="G53" s="75" t="n"/>
-    </row>
-    <row r="54">
-      <c r="D54" s="74" t="n"/>
-      <c r="E54" s="74" t="n"/>
-      <c r="F54" s="74" t="n"/>
-      <c r="G54" s="75" t="n"/>
-    </row>
-    <row r="55">
-      <c r="D55" s="74" t="n"/>
-      <c r="E55" s="74" t="n"/>
-      <c r="F55" s="74" t="n"/>
-      <c r="G55" s="75" t="n"/>
-    </row>
+    <row r="49" ht="21" customHeight="1"/>
+    <row r="50" ht="21" customHeight="1"/>
+    <row r="51" ht="17.25" customHeight="1"/>
+    <row r="52"/>
+    <row r="53"/>
+    <row r="54"/>
+    <row r="55"/>
     <row r="56"/>
     <row r="57"/>
     <row r="58"/>
@@ -3165,19 +2843,20 @@
     <row r="199"/>
     <row r="200"/>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="B32"/>
-    <mergeCell ref="A36:C36"/>
+  <mergeCells count="13">
     <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A31:G31"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A6:G6"/>
     <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A38:G38"/>
+    <mergeCell ref="B25"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="B28:C28"/>
     <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="A29:C29"/>
     <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A37:G37"/>
   </mergeCells>
   <conditionalFormatting sqref="J23:J35">
     <cfRule type="duplicateValues" priority="1" stopIfTrue="1"/>
@@ -3349,12 +3028,12 @@
       <c r="G10" s="96" t="n"/>
       <c r="H10" s="9" t="inlineStr">
         <is>
-          <t>FCA :</t>
+          <t>FOB :</t>
         </is>
       </c>
       <c r="I10" s="107" t="inlineStr">
         <is>
-          <t>BAVET, SVAY RIENG</t>
+          <t>BAVET</t>
         </is>
       </c>
     </row>
@@ -3977,19 +3656,19 @@
         <f>SUM(E23:E34)</f>
         <v/>
       </c>
-      <c r="F36" s="114">
+      <c r="F36" s="132">
         <f>SUM(F23:F34)</f>
         <v/>
       </c>
-      <c r="G36" s="114">
+      <c r="G36" s="132">
         <f>SUM(G23:G34)</f>
         <v/>
       </c>
-      <c r="H36" s="114">
+      <c r="H36" s="132">
         <f>SUM(H23:H34)</f>
         <v/>
       </c>
-      <c r="I36" s="132">
+      <c r="I36" s="133">
         <f>SUM(I23:I34)</f>
         <v/>
       </c>
@@ -4508,26 +4187,121 @@
         <f>SUM(E40:E52)</f>
         <v/>
       </c>
-      <c r="F54" s="114">
+      <c r="F54" s="132">
         <f>SUM(F40:F52)</f>
         <v/>
       </c>
-      <c r="G54" s="114">
+      <c r="G54" s="132">
         <f>SUM(G40:G52)</f>
         <v/>
       </c>
-      <c r="H54" s="114">
+      <c r="H54" s="132">
         <f>SUM(H40:H52)</f>
         <v/>
       </c>
-      <c r="I54" s="132">
+      <c r="I54" s="133">
         <f>SUM(I40:I52)</f>
         <v/>
       </c>
     </row>
-    <row r="55" ht="42" customHeight="1"/>
-    <row r="56" ht="24" customHeight="1"/>
-    <row r="57" ht="69.75" customHeight="1"/>
+    <row r="55" ht="27" customHeight="1">
+      <c r="B55" s="134" t="inlineStr">
+        <is>
+          <t>TOTAL OF:</t>
+        </is>
+      </c>
+      <c r="D55" s="134" t="inlineStr">
+        <is>
+          <t>16 PALLETS</t>
+        </is>
+      </c>
+      <c r="E55" s="135">
+        <f>SUM(E23:E34,E40:E52)</f>
+        <v/>
+      </c>
+      <c r="F55" s="136">
+        <f>SUM(F23:F34,F40:F52)</f>
+        <v/>
+      </c>
+      <c r="G55" s="136">
+        <f>SUM(G23:G34,G40:G52)</f>
+        <v/>
+      </c>
+      <c r="H55" s="136">
+        <f>SUM(H23:H34,H40:H52)</f>
+        <v/>
+      </c>
+      <c r="I55" s="137">
+        <f>SUM(I23:I34,I40:I52)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" ht="27" customHeight="1">
+      <c r="A56" s="138" t="n"/>
+      <c r="B56" s="139" t="inlineStr">
+        <is>
+          <t>TOTAL OF:</t>
+        </is>
+      </c>
+      <c r="C56" s="139" t="inlineStr">
+        <is>
+          <t>BUFFALO</t>
+        </is>
+      </c>
+      <c r="D56" s="139" t="inlineStr">
+        <is>
+          <t>9 PALLETS</t>
+        </is>
+      </c>
+      <c r="E56" s="140" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F56" s="141" t="n">
+        <v>72108.09999999999</v>
+      </c>
+      <c r="G56" s="141" t="n">
+        <v>5995.5</v>
+      </c>
+      <c r="H56" s="141" t="n">
+        <v>5590.5</v>
+      </c>
+      <c r="I56" s="142" t="n">
+        <v>22.8096</v>
+      </c>
+    </row>
+    <row r="57" ht="27" customHeight="1">
+      <c r="A57" s="138" t="n"/>
+      <c r="B57" s="139" t="inlineStr">
+        <is>
+          <t>TOTAL OF:</t>
+        </is>
+      </c>
+      <c r="C57" s="139" t="inlineStr">
+        <is>
+          <t>LEATHER</t>
+        </is>
+      </c>
+      <c r="D57" s="139" t="inlineStr">
+        <is>
+          <t>7 PALLETS</t>
+        </is>
+      </c>
+      <c r="E57" s="140" t="n">
+        <v>1133</v>
+      </c>
+      <c r="F57" s="141" t="n">
+        <v>58119</v>
+      </c>
+      <c r="G57" s="141" t="n">
+        <v>4895.5</v>
+      </c>
+      <c r="H57" s="141" t="n">
+        <v>4580.5</v>
+      </c>
+      <c r="I57" s="142" t="n">
+        <v>16.038</v>
+      </c>
+    </row>
     <row r="58" ht="42" customHeight="1">
       <c r="A58" s="20" t="n"/>
       <c r="B58" s="65" t="n"/>
@@ -4881,9 +4655,10 @@
     <row r="199"/>
     <row r="200"/>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="30">
     <mergeCell ref="B60:D60"/>
     <mergeCell ref="H38:H39"/>
+    <mergeCell ref="B55"/>
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="H21:H22"/>
     <mergeCell ref="A3:I3"/>

</xml_diff>